<commit_message>
Created Global package/class with Enums. Created TrackPiece interface and implemented it in Block and Switch.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan94\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan94\Documents\Coding\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>EDGEBROOK</t>
-  </si>
-  <si>
-    <t>UNNAMED</t>
   </si>
   <si>
     <t>WHITED</t>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>isStaticSwitchBlock</t>
+  </si>
+  <si>
+    <t>PITT</t>
   </si>
 </sst>
 </file>
@@ -803,7 +803,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -830,55 +830,55 @@
   <sheetData>
     <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1506,7 +1506,7 @@
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
       <c r="N17" s="19" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="O17" s="16">
         <v>0</v>
@@ -1744,7 +1744,7 @@
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
       <c r="N23" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O23" s="24">
         <v>0</v>
@@ -2095,7 +2095,7 @@
       <c r="L32" s="31"/>
       <c r="M32" s="31"/>
       <c r="N32" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O32" s="28">
         <v>0</v>
@@ -2419,7 +2419,7 @@
         <v>24</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O40" s="5">
         <v>0</v>
@@ -2781,7 +2781,7 @@
         <v>24</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O49" s="5">
         <v>0</v>
@@ -3145,7 +3145,7 @@
         <v>24</v>
       </c>
       <c r="N58" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O58" s="5">
         <v>0</v>
@@ -3463,7 +3463,7 @@
       <c r="L66" s="14"/>
       <c r="M66" s="14"/>
       <c r="N66" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O66" s="12">
         <v>0</v>
@@ -3776,7 +3776,7 @@
       <c r="L74" s="19"/>
       <c r="M74" s="19"/>
       <c r="N74" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O74" s="16">
         <v>0</v>
@@ -3939,7 +3939,7 @@
       <c r="L78" s="27"/>
       <c r="M78" s="27"/>
       <c r="N78" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O78" s="24">
         <v>0</v>
@@ -4368,7 +4368,7 @@
       <c r="L89" s="31"/>
       <c r="M89" s="31"/>
       <c r="N89" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O89" s="28">
         <v>0</v>
@@ -4677,7 +4677,7 @@
       <c r="L97" s="36"/>
       <c r="M97" s="36"/>
       <c r="N97" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O97" s="32">
         <v>0</v>
@@ -5041,7 +5041,7 @@
       <c r="L106" s="19"/>
       <c r="M106" s="19"/>
       <c r="N106" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O106" s="16">
         <v>0</v>
@@ -5390,7 +5390,7 @@
       <c r="L115" s="23"/>
       <c r="M115" s="23"/>
       <c r="N115" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O115" s="20">
         <v>0</v>
@@ -5748,7 +5748,7 @@
         <v>24</v>
       </c>
       <c r="N124" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O124" s="28">
         <v>0</v>
@@ -6110,7 +6110,7 @@
         <v>24</v>
       </c>
       <c r="N133" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O133" s="28">
         <v>0</v>
@@ -6472,7 +6472,7 @@
         <v>24</v>
       </c>
       <c r="N142" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O142" s="28">
         <v>0</v>
@@ -7199,7 +7199,7 @@
       <c r="L160" s="31"/>
       <c r="M160" s="31"/>
       <c r="N160" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O160" s="41">
         <v>0.375</v>
@@ -7559,7 +7559,7 @@
       <c r="L169" s="35"/>
       <c r="M169" s="35"/>
       <c r="N169" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O169" s="44">
         <v>-0.25</v>
@@ -7755,7 +7755,7 @@
       <c r="L174" s="14"/>
       <c r="M174" s="14"/>
       <c r="N174" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O174" s="40">
         <v>0</v>
@@ -7917,7 +7917,7 @@
         <v>24</v>
       </c>
       <c r="N178" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O178" s="37">
         <v>0</v>
@@ -8323,7 +8323,7 @@
         <v>24</v>
       </c>
       <c r="N188" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O188" s="37">
         <v>0</v>
@@ -8731,7 +8731,7 @@
         <v>24</v>
       </c>
       <c r="N198" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O198" s="37">
         <v>0</v>
@@ -8855,7 +8855,7 @@
       <c r="L201" s="23"/>
       <c r="M201" s="23"/>
       <c r="N201" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O201" s="38">
         <v>0</v>
@@ -9327,7 +9327,7 @@
       <c r="L213" s="36"/>
       <c r="M213" s="36"/>
       <c r="N213" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O213" s="42">
         <v>0</v>
@@ -10078,16 +10078,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="45" t="s">
-        <v>50</v>
-      </c>
       <c r="D1" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Station info to TrackData file.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -13,14 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="BLOCK" sheetId="2" r:id="rId1"/>
-    <sheet name="SWITCH" sheetId="7" r:id="rId2"/>
+    <sheet name="STATION" sheetId="8" r:id="rId2"/>
+    <sheet name="SWITCH" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="78">
   <si>
     <t>A</t>
   </si>
@@ -231,6 +232,30 @@
   <si>
     <t>PITT</t>
   </si>
+  <si>
+    <t>blockA</t>
+  </si>
+  <si>
+    <t>blockB</t>
+  </si>
+  <si>
+    <t>stationID</t>
+  </si>
+  <si>
+    <t>containsStation</t>
+  </si>
+  <si>
+    <t>blockASection</t>
+  </si>
+  <si>
+    <t>blockBSection</t>
+  </si>
+  <si>
+    <t>rightSide</t>
+  </si>
+  <si>
+    <t>leftSide</t>
+  </si>
 </sst>
 </file>
 
@@ -342,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -461,6 +486,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,11 +825,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q231"/>
+  <dimension ref="A1:Q230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomLeft" activeCell="F153" sqref="F153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -869,7 +895,7 @@
         <v>64</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>66</v>
@@ -951,7 +977,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="O3" s="5">
         <v>1</v>
@@ -1229,7 +1255,7 @@
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
       <c r="N10" s="14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="O10" s="12">
         <v>-5</v>
@@ -1506,7 +1532,7 @@
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
       <c r="N17" s="19" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="O17" s="16">
         <v>0</v>
@@ -1744,7 +1770,7 @@
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
       <c r="N23" s="27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="O23" s="24">
         <v>0</v>
@@ -2095,7 +2121,7 @@
       <c r="L32" s="31"/>
       <c r="M32" s="31"/>
       <c r="N32" s="31" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O32" s="28">
         <v>0</v>
@@ -2419,7 +2445,7 @@
         <v>24</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="O40" s="5">
         <v>0</v>
@@ -2781,7 +2807,7 @@
         <v>24</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="O49" s="5">
         <v>0</v>
@@ -3145,7 +3171,7 @@
         <v>24</v>
       </c>
       <c r="N58" s="8" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="O58" s="5">
         <v>0</v>
@@ -3463,7 +3489,7 @@
       <c r="L66" s="14"/>
       <c r="M66" s="14"/>
       <c r="N66" s="14" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="O66" s="12">
         <v>0</v>
@@ -3776,7 +3802,7 @@
       <c r="L74" s="19"/>
       <c r="M74" s="19"/>
       <c r="N74" s="19" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="O74" s="16">
         <v>0</v>
@@ -3939,7 +3965,7 @@
       <c r="L78" s="27"/>
       <c r="M78" s="27"/>
       <c r="N78" s="27" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="O78" s="24">
         <v>0</v>
@@ -4368,7 +4394,7 @@
       <c r="L89" s="31"/>
       <c r="M89" s="31"/>
       <c r="N89" s="31" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="O89" s="28">
         <v>0</v>
@@ -4677,7 +4703,7 @@
       <c r="L97" s="36"/>
       <c r="M97" s="36"/>
       <c r="N97" s="36" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="O97" s="32">
         <v>0</v>
@@ -5041,7 +5067,7 @@
       <c r="L106" s="19"/>
       <c r="M106" s="19"/>
       <c r="N106" s="19" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="O106" s="16">
         <v>0</v>
@@ -5390,7 +5416,7 @@
       <c r="L115" s="23"/>
       <c r="M115" s="23"/>
       <c r="N115" s="23" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="O115" s="20">
         <v>0</v>
@@ -5748,7 +5774,7 @@
         <v>24</v>
       </c>
       <c r="N124" s="31" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="O124" s="28">
         <v>0</v>
@@ -6110,7 +6136,7 @@
         <v>24</v>
       </c>
       <c r="N133" s="31" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="O133" s="28">
         <v>0</v>
@@ -6472,7 +6498,7 @@
         <v>24</v>
       </c>
       <c r="N142" s="31" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="O142" s="28">
         <v>0</v>
@@ -7199,7 +7225,7 @@
       <c r="L160" s="31"/>
       <c r="M160" s="31"/>
       <c r="N160" s="31" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="O160" s="41">
         <v>0.375</v>
@@ -7559,7 +7585,7 @@
       <c r="L169" s="35"/>
       <c r="M169" s="35"/>
       <c r="N169" s="35" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="O169" s="44">
         <v>-0.25</v>
@@ -7755,7 +7781,7 @@
       <c r="L174" s="14"/>
       <c r="M174" s="14"/>
       <c r="N174" s="14" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="O174" s="40">
         <v>0</v>
@@ -7917,7 +7943,7 @@
         <v>24</v>
       </c>
       <c r="N178" s="19" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="O178" s="37">
         <v>0</v>
@@ -8323,7 +8349,7 @@
         <v>24</v>
       </c>
       <c r="N188" s="19" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="O188" s="37">
         <v>0</v>
@@ -8731,7 +8757,7 @@
         <v>24</v>
       </c>
       <c r="N198" s="19" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="O198" s="37">
         <v>0</v>
@@ -8855,7 +8881,7 @@
       <c r="L201" s="23"/>
       <c r="M201" s="23"/>
       <c r="N201" s="23" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="O201" s="38">
         <v>0</v>
@@ -9327,7 +9353,7 @@
       <c r="L213" s="36"/>
       <c r="M213" s="36"/>
       <c r="N213" s="36" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="O213" s="42">
         <v>0</v>
@@ -10029,43 +10055,555 @@
       </c>
       <c r="Q230" s="5"/>
     </row>
-    <row r="231" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="9"/>
-      <c r="B231" s="9"/>
-      <c r="C231" s="9"/>
-      <c r="E231" s="9">
-        <v>0</v>
-      </c>
-      <c r="F231" s="9"/>
-      <c r="G231" s="9"/>
-      <c r="H231" s="9"/>
-      <c r="I231" s="9">
-        <v>0</v>
-      </c>
-      <c r="J231" s="9">
-        <v>0</v>
-      </c>
-      <c r="K231" s="9">
-        <v>0</v>
-      </c>
-      <c r="L231" s="9"/>
-      <c r="M231" s="9"/>
-      <c r="N231" s="9"/>
-      <c r="O231" s="11">
-        <v>0</v>
-      </c>
-      <c r="P231" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q231" s="9"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>96</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>141</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>73</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>105</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>114</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>132</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>123</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>48</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D226">
+    <sortCondition ref="B2:B226"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>

</xml_diff>

<commit_message>
TrackModel now parses both Station and Switch data, then instantiates their objects with references to the associated Block objects.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BLOCK" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="76">
   <si>
     <t>A</t>
   </si>
@@ -167,18 +167,6 @@
     <t>SOUTH HILLS JUNCTION</t>
   </si>
   <si>
-    <t>PORT_A</t>
-  </si>
-  <si>
-    <t>PORT_B</t>
-  </si>
-  <si>
-    <t>PORT_C</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>line</t>
   </si>
   <si>
@@ -258,6 +246,9 @@
   </si>
   <si>
     <t>RED</t>
+  </si>
+  <si>
+    <t>portC</t>
   </si>
 </sst>
 </file>
@@ -830,7 +821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P221" sqref="P221"/>
     </sheetView>
@@ -859,60 +850,60 @@
   <sheetData>
     <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -954,7 +945,7 @@
     </row>
     <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -996,7 +987,7 @@
     </row>
     <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>0</v>
@@ -1041,7 +1032,7 @@
     </row>
     <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>1</v>
@@ -1085,7 +1076,7 @@
     </row>
     <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>1</v>
@@ -1127,7 +1118,7 @@
     </row>
     <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>1</v>
@@ -1172,7 +1163,7 @@
     </row>
     <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>2</v>
@@ -1216,7 +1207,7 @@
     </row>
     <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>2</v>
@@ -1258,7 +1249,7 @@
     </row>
     <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>2</v>
@@ -1300,7 +1291,7 @@
     </row>
     <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>2</v>
@@ -1342,7 +1333,7 @@
     </row>
     <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>2</v>
@@ -1384,7 +1375,7 @@
     </row>
     <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>2</v>
@@ -1429,7 +1420,7 @@
     </row>
     <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>3</v>
@@ -1471,7 +1462,7 @@
     </row>
     <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>3</v>
@@ -1513,7 +1504,7 @@
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>3</v>
@@ -1555,7 +1546,7 @@
     </row>
     <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>3</v>
@@ -1599,7 +1590,7 @@
     </row>
     <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>4</v>
@@ -1643,7 +1634,7 @@
     </row>
     <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>4</v>
@@ -1685,7 +1676,7 @@
     </row>
     <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>4</v>
@@ -1729,7 +1720,7 @@
     </row>
     <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>4</v>
@@ -1773,7 +1764,7 @@
     </row>
     <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>5</v>
@@ -1817,7 +1808,7 @@
     </row>
     <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>5</v>
@@ -1859,7 +1850,7 @@
     </row>
     <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>5</v>
@@ -1901,7 +1892,7 @@
     </row>
     <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>5</v>
@@ -1943,7 +1934,7 @@
     </row>
     <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>5</v>
@@ -1985,7 +1976,7 @@
     </row>
     <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>5</v>
@@ -2027,7 +2018,7 @@
     </row>
     <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>5</v>
@@ -2069,7 +2060,7 @@
     </row>
     <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>5</v>
@@ -2111,7 +2102,7 @@
     </row>
     <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>6</v>
@@ -2156,7 +2147,7 @@
     </row>
     <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>6</v>
@@ -2198,7 +2189,7 @@
     </row>
     <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>6</v>
@@ -2240,7 +2231,7 @@
     </row>
     <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>6</v>
@@ -2284,7 +2275,7 @@
     </row>
     <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B34" s="32" t="s">
         <v>7</v>
@@ -2329,7 +2320,7 @@
     </row>
     <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B35" s="32" t="s">
         <v>7</v>
@@ -2371,7 +2362,7 @@
     </row>
     <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B36" s="32" t="s">
         <v>7</v>
@@ -2415,7 +2406,7 @@
     </row>
     <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>8</v>
@@ -2462,7 +2453,7 @@
     </row>
     <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>8</v>
@@ -2506,7 +2497,7 @@
     </row>
     <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>8</v>
@@ -2550,7 +2541,7 @@
     </row>
     <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>8</v>
@@ -2594,7 +2585,7 @@
     </row>
     <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>8</v>
@@ -2638,7 +2629,7 @@
     </row>
     <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>8</v>
@@ -2682,7 +2673,7 @@
     </row>
     <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>8</v>
@@ -2726,7 +2717,7 @@
     </row>
     <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>8</v>
@@ -2770,7 +2761,7 @@
     </row>
     <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>8</v>
@@ -2814,7 +2805,7 @@
     </row>
     <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>8</v>
@@ -2858,7 +2849,7 @@
     </row>
     <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>8</v>
@@ -2902,7 +2893,7 @@
     </row>
     <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>8</v>
@@ -2946,7 +2937,7 @@
     </row>
     <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>8</v>
@@ -2990,7 +2981,7 @@
     </row>
     <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>8</v>
@@ -3034,7 +3025,7 @@
     </row>
     <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>8</v>
@@ -3078,7 +3069,7 @@
     </row>
     <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>8</v>
@@ -3122,7 +3113,7 @@
     </row>
     <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>8</v>
@@ -3166,7 +3157,7 @@
     </row>
     <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>8</v>
@@ -3210,7 +3201,7 @@
     </row>
     <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>8</v>
@@ -3254,7 +3245,7 @@
     </row>
     <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>8</v>
@@ -3298,7 +3289,7 @@
     </row>
     <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>8</v>
@@ -3342,7 +3333,7 @@
     </row>
     <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>8</v>
@@ -3386,7 +3377,7 @@
     </row>
     <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>9</v>
@@ -3431,7 +3422,7 @@
     </row>
     <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>9</v>
@@ -3473,7 +3464,7 @@
     </row>
     <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>9</v>
@@ -3515,7 +3506,7 @@
     </row>
     <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>9</v>
@@ -3555,7 +3546,7 @@
     </row>
     <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>9</v>
@@ -3599,7 +3590,7 @@
     </row>
     <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>10</v>
@@ -3644,7 +3635,7 @@
     </row>
     <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B65" s="12" t="s">
         <v>10</v>
@@ -3686,7 +3677,7 @@
     </row>
     <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B66" s="12" t="s">
         <v>10</v>
@@ -3728,7 +3719,7 @@
     </row>
     <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B67" s="12" t="s">
         <v>10</v>
@@ -3770,7 +3761,7 @@
     </row>
     <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B68" s="12" t="s">
         <v>10</v>
@@ -3812,7 +3803,7 @@
     </row>
     <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B69" s="12" t="s">
         <v>10</v>
@@ -3856,7 +3847,7 @@
     </row>
     <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B70" s="16" t="s">
         <v>11</v>
@@ -3901,7 +3892,7 @@
     </row>
     <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B71" s="16" t="s">
         <v>11</v>
@@ -3943,7 +3934,7 @@
     </row>
     <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B72" s="16" t="s">
         <v>11</v>
@@ -3985,7 +3976,7 @@
     </row>
     <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B73" s="16" t="s">
         <v>11</v>
@@ -4027,7 +4018,7 @@
     </row>
     <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B74" s="16" t="s">
         <v>11</v>
@@ -4071,7 +4062,7 @@
     </row>
     <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B75" s="20" t="s">
         <v>12</v>
@@ -4116,7 +4107,7 @@
     </row>
     <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B76" s="20" t="s">
         <v>12</v>
@@ -4158,7 +4149,7 @@
     </row>
     <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B77" s="20" t="s">
         <v>12</v>
@@ -4202,7 +4193,7 @@
     </row>
     <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B78" s="24" t="s">
         <v>13</v>
@@ -4244,7 +4235,7 @@
     </row>
     <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B79" s="24" t="s">
         <v>13</v>
@@ -4286,7 +4277,7 @@
     </row>
     <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B80" s="24" t="s">
         <v>13</v>
@@ -4328,7 +4319,7 @@
     </row>
     <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B81" s="24" t="s">
         <v>13</v>
@@ -4370,7 +4361,7 @@
     </row>
     <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B82" s="24" t="s">
         <v>13</v>
@@ -4412,7 +4403,7 @@
     </row>
     <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B83" s="24" t="s">
         <v>13</v>
@@ -4454,7 +4445,7 @@
     </row>
     <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B84" s="24" t="s">
         <v>13</v>
@@ -4496,7 +4487,7 @@
     </row>
     <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B85" s="24" t="s">
         <v>13</v>
@@ -4538,7 +4529,7 @@
     </row>
     <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B86" s="24" t="s">
         <v>13</v>
@@ -4580,7 +4571,7 @@
     </row>
     <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B87" s="28" t="s">
         <v>14</v>
@@ -4625,7 +4616,7 @@
     </row>
     <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B88" s="28" t="s">
         <v>14</v>
@@ -4667,7 +4658,7 @@
     </row>
     <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B89" s="28" t="s">
         <v>14</v>
@@ -4711,7 +4702,7 @@
     </row>
     <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B90" s="32" t="s">
         <v>15</v>
@@ -4756,7 +4747,7 @@
     </row>
     <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B91" s="32" t="s">
         <v>15</v>
@@ -4798,7 +4789,7 @@
     </row>
     <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B92" s="32" t="s">
         <v>15</v>
@@ -4840,7 +4831,7 @@
     </row>
     <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B93" s="32" t="s">
         <v>15</v>
@@ -4882,7 +4873,7 @@
     </row>
     <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B94" s="32" t="s">
         <v>15</v>
@@ -4924,7 +4915,7 @@
     </row>
     <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B95" s="32" t="s">
         <v>15</v>
@@ -4966,7 +4957,7 @@
     </row>
     <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B96" s="32" t="s">
         <v>15</v>
@@ -5008,7 +4999,7 @@
     </row>
     <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B97" s="32" t="s">
         <v>15</v>
@@ -5050,7 +5041,7 @@
     </row>
     <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B98" s="32" t="s">
         <v>15</v>
@@ -5094,7 +5085,7 @@
     </row>
     <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>16</v>
@@ -5139,7 +5130,7 @@
     </row>
     <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>16</v>
@@ -5181,7 +5172,7 @@
     </row>
     <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>16</v>
@@ -5223,7 +5214,7 @@
     </row>
     <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B102" s="9" t="s">
         <v>17</v>
@@ -5268,7 +5259,7 @@
     </row>
     <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B103" s="12" t="s">
         <v>18</v>
@@ -5313,7 +5304,7 @@
     </row>
     <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B104" s="12" t="s">
         <v>18</v>
@@ -5355,7 +5346,7 @@
     </row>
     <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B105" s="12" t="s">
         <v>18</v>
@@ -5399,7 +5390,7 @@
     </row>
     <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B106" s="16" t="s">
         <v>19</v>
@@ -5444,7 +5435,7 @@
     </row>
     <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B107" s="16" t="s">
         <v>19</v>
@@ -5486,7 +5477,7 @@
     </row>
     <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B108" s="16" t="s">
         <v>19</v>
@@ -5528,7 +5519,7 @@
     </row>
     <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B109" s="16" t="s">
         <v>19</v>
@@ -5570,7 +5561,7 @@
     </row>
     <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B110" s="16" t="s">
         <v>19</v>
@@ -5614,7 +5605,7 @@
     </row>
     <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B111" s="20" t="s">
         <v>20</v>
@@ -5659,7 +5650,7 @@
     </row>
     <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B112" s="20" t="s">
         <v>20</v>
@@ -5701,7 +5692,7 @@
     </row>
     <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B113" s="20" t="s">
         <v>20</v>
@@ -5743,7 +5734,7 @@
     </row>
     <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B114" s="20" t="s">
         <v>20</v>
@@ -5785,7 +5776,7 @@
     </row>
     <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B115" s="20" t="s">
         <v>20</v>
@@ -5827,7 +5818,7 @@
     </row>
     <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B116" s="20" t="s">
         <v>20</v>
@@ -5869,7 +5860,7 @@
     </row>
     <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B117" s="20" t="s">
         <v>20</v>
@@ -5913,7 +5904,7 @@
     </row>
     <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B118" s="24" t="s">
         <v>21</v>
@@ -5958,7 +5949,7 @@
     </row>
     <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B119" s="24" t="s">
         <v>21</v>
@@ -6000,7 +5991,7 @@
     </row>
     <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B120" s="24" t="s">
         <v>21</v>
@@ -6042,7 +6033,7 @@
     </row>
     <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B121" s="24" t="s">
         <v>21</v>
@@ -6084,7 +6075,7 @@
     </row>
     <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B122" s="24" t="s">
         <v>21</v>
@@ -6128,7 +6119,7 @@
     </row>
     <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B123" s="28" t="s">
         <v>22</v>
@@ -6175,7 +6166,7 @@
     </row>
     <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B124" s="28" t="s">
         <v>22</v>
@@ -6219,7 +6210,7 @@
     </row>
     <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B125" s="28" t="s">
         <v>22</v>
@@ -6263,7 +6254,7 @@
     </row>
     <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B126" s="28" t="s">
         <v>22</v>
@@ -6307,7 +6298,7 @@
     </row>
     <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B127" s="28" t="s">
         <v>22</v>
@@ -6351,7 +6342,7 @@
     </row>
     <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B128" s="28" t="s">
         <v>22</v>
@@ -6395,7 +6386,7 @@
     </row>
     <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B129" s="28" t="s">
         <v>22</v>
@@ -6439,7 +6430,7 @@
     </row>
     <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B130" s="28" t="s">
         <v>22</v>
@@ -6483,7 +6474,7 @@
     </row>
     <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B131" s="28" t="s">
         <v>22</v>
@@ -6527,7 +6518,7 @@
     </row>
     <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B132" s="28" t="s">
         <v>22</v>
@@ -6571,7 +6562,7 @@
     </row>
     <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B133" s="28" t="s">
         <v>22</v>
@@ -6615,7 +6606,7 @@
     </row>
     <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B134" s="28" t="s">
         <v>22</v>
@@ -6659,7 +6650,7 @@
     </row>
     <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B135" s="28" t="s">
         <v>22</v>
@@ -6703,7 +6694,7 @@
     </row>
     <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B136" s="28" t="s">
         <v>22</v>
@@ -6747,7 +6738,7 @@
     </row>
     <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B137" s="28" t="s">
         <v>22</v>
@@ -6791,7 +6782,7 @@
     </row>
     <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B138" s="28" t="s">
         <v>22</v>
@@ -6835,7 +6826,7 @@
     </row>
     <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B139" s="28" t="s">
         <v>22</v>
@@ -6879,7 +6870,7 @@
     </row>
     <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B140" s="28" t="s">
         <v>22</v>
@@ -6923,7 +6914,7 @@
     </row>
     <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B141" s="28" t="s">
         <v>22</v>
@@ -6967,7 +6958,7 @@
     </row>
     <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B142" s="28" t="s">
         <v>22</v>
@@ -7011,7 +7002,7 @@
     </row>
     <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B143" s="28" t="s">
         <v>22</v>
@@ -7055,7 +7046,7 @@
     </row>
     <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B144" s="28" t="s">
         <v>22</v>
@@ -7101,7 +7092,7 @@
     </row>
     <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B145" s="32" t="s">
         <v>23</v>
@@ -7146,7 +7137,7 @@
     </row>
     <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B146" s="32" t="s">
         <v>23</v>
@@ -7188,7 +7179,7 @@
     </row>
     <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B147" s="32" t="s">
         <v>23</v>
@@ -7232,7 +7223,7 @@
     </row>
     <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>24</v>
@@ -7277,7 +7268,7 @@
     </row>
     <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>24</v>
@@ -7319,7 +7310,7 @@
     </row>
     <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>24</v>
@@ -7363,7 +7354,7 @@
     </row>
     <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B151" s="9" t="s">
         <v>25</v>
@@ -7408,7 +7399,7 @@
     </row>
     <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B152" s="12" t="s">
         <v>26</v>
@@ -7453,7 +7444,7 @@
     </row>
     <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B153" s="16" t="s">
         <v>27</v>
@@ -7498,7 +7489,7 @@
     </row>
     <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B154" s="20" t="s">
         <v>0</v>
@@ -7540,7 +7531,7 @@
     </row>
     <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B155" s="20" t="s">
         <v>0</v>
@@ -7582,7 +7573,7 @@
     </row>
     <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B156" s="20" t="s">
         <v>0</v>
@@ -7626,7 +7617,7 @@
     </row>
     <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B157" s="24" t="s">
         <v>1</v>
@@ -7670,7 +7661,7 @@
     </row>
     <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B158" s="24" t="s">
         <v>1</v>
@@ -7712,7 +7703,7 @@
     </row>
     <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B159" s="24" t="s">
         <v>1</v>
@@ -7756,7 +7747,7 @@
     </row>
     <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B160" s="28" t="s">
         <v>2</v>
@@ -7800,7 +7791,7 @@
     </row>
     <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B161" s="28" t="s">
         <v>2</v>
@@ -7842,7 +7833,7 @@
     </row>
     <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B162" s="28" t="s">
         <v>2</v>
@@ -7886,7 +7877,7 @@
     </row>
     <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B163" s="32" t="s">
         <v>3</v>
@@ -7928,7 +7919,7 @@
     </row>
     <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B164" s="32" t="s">
         <v>3</v>
@@ -7970,7 +7961,7 @@
     </row>
     <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B165" s="32" t="s">
         <v>3</v>
@@ -8014,7 +8005,7 @@
     </row>
     <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>4</v>
@@ -8058,7 +8049,7 @@
     </row>
     <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>4</v>
@@ -8100,7 +8091,7 @@
     </row>
     <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B168" s="5" t="s">
         <v>4</v>
@@ -8144,7 +8135,7 @@
     </row>
     <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B169" s="9" t="s">
         <v>5</v>
@@ -8186,7 +8177,7 @@
     </row>
     <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B170" s="9" t="s">
         <v>5</v>
@@ -8228,7 +8219,7 @@
     </row>
     <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A171" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B171" s="9" t="s">
         <v>5</v>
@@ -8270,7 +8261,7 @@
     </row>
     <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B172" s="9" t="s">
         <v>5</v>
@@ -8312,7 +8303,7 @@
     </row>
     <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B173" s="9" t="s">
         <v>5</v>
@@ -8356,7 +8347,7 @@
     </row>
     <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B174" s="12" t="s">
         <v>6</v>
@@ -8400,7 +8391,7 @@
     </row>
     <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B175" s="12" t="s">
         <v>6</v>
@@ -8442,7 +8433,7 @@
     </row>
     <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B176" s="12" t="s">
         <v>6</v>
@@ -8486,7 +8477,7 @@
     </row>
     <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A177" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B177" s="16" t="s">
         <v>7</v>
@@ -8532,7 +8523,7 @@
     </row>
     <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B178" s="16" t="s">
         <v>7</v>
@@ -8576,7 +8567,7 @@
     </row>
     <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B179" s="16" t="s">
         <v>7</v>
@@ -8620,7 +8611,7 @@
     </row>
     <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B180" s="16" t="s">
         <v>7</v>
@@ -8664,7 +8655,7 @@
     </row>
     <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A181" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B181" s="16" t="s">
         <v>7</v>
@@ -8706,7 +8697,7 @@
     </row>
     <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B182" s="16" t="s">
         <v>7</v>
@@ -8750,7 +8741,7 @@
     </row>
     <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B183" s="16" t="s">
         <v>7</v>
@@ -8794,7 +8785,7 @@
     </row>
     <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B184" s="16" t="s">
         <v>7</v>
@@ -8838,7 +8829,7 @@
     </row>
     <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B185" s="16" t="s">
         <v>7</v>
@@ -8882,7 +8873,7 @@
     </row>
     <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A186" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B186" s="16" t="s">
         <v>7</v>
@@ -8924,7 +8915,7 @@
     </row>
     <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B187" s="16" t="s">
         <v>7</v>
@@ -8968,7 +8959,7 @@
     </row>
     <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B188" s="16" t="s">
         <v>7</v>
@@ -9012,7 +9003,7 @@
     </row>
     <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B189" s="16" t="s">
         <v>7</v>
@@ -9056,7 +9047,7 @@
     </row>
     <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B190" s="16" t="s">
         <v>7</v>
@@ -9100,7 +9091,7 @@
     </row>
     <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B191" s="16" t="s">
         <v>7</v>
@@ -9144,7 +9135,7 @@
     </row>
     <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B192" s="16" t="s">
         <v>7</v>
@@ -9186,7 +9177,7 @@
     </row>
     <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B193" s="16" t="s">
         <v>7</v>
@@ -9230,7 +9221,7 @@
     </row>
     <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B194" s="16" t="s">
         <v>7</v>
@@ -9274,7 +9265,7 @@
     </row>
     <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A195" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B195" s="16" t="s">
         <v>7</v>
@@ -9318,7 +9309,7 @@
     </row>
     <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B196" s="16" t="s">
         <v>7</v>
@@ -9362,7 +9353,7 @@
     </row>
     <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B197" s="16" t="s">
         <v>7</v>
@@ -9404,7 +9395,7 @@
     </row>
     <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B198" s="16" t="s">
         <v>7</v>
@@ -9450,7 +9441,7 @@
     </row>
     <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A199" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B199" s="20" t="s">
         <v>8</v>
@@ -9496,7 +9487,7 @@
     </row>
     <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A200" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B200" s="20" t="s">
         <v>8</v>
@@ -9540,7 +9531,7 @@
     </row>
     <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A201" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B201" s="20" t="s">
         <v>8</v>
@@ -9584,7 +9575,7 @@
     </row>
     <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B202" s="24" t="s">
         <v>9</v>
@@ -9628,7 +9619,7 @@
     </row>
     <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A203" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B203" s="24" t="s">
         <v>9</v>
@@ -9670,7 +9661,7 @@
     </row>
     <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A204" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B204" s="24" t="s">
         <v>9</v>
@@ -9712,7 +9703,7 @@
     </row>
     <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B205" s="24" t="s">
         <v>9</v>
@@ -9754,7 +9745,7 @@
     </row>
     <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A206" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B206" s="24" t="s">
         <v>9</v>
@@ -9794,7 +9785,7 @@
     </row>
     <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B207" s="24" t="s">
         <v>9</v>
@@ -9838,7 +9829,7 @@
     </row>
     <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B208" s="28" t="s">
         <v>10</v>
@@ -9882,7 +9873,7 @@
     </row>
     <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B209" s="28" t="s">
         <v>10</v>
@@ -9924,7 +9915,7 @@
     </row>
     <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B210" s="28" t="s">
         <v>10</v>
@@ -9968,7 +9959,7 @@
     </row>
     <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B211" s="32" t="s">
         <v>11</v>
@@ -10012,7 +10003,7 @@
     </row>
     <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B212" s="32" t="s">
         <v>11</v>
@@ -10054,7 +10045,7 @@
     </row>
     <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B213" s="32" t="s">
         <v>11</v>
@@ -10098,7 +10089,7 @@
     </row>
     <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B214" s="5" t="s">
         <v>12</v>
@@ -10142,7 +10133,7 @@
     </row>
     <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B215" s="5" t="s">
         <v>12</v>
@@ -10184,7 +10175,7 @@
     </row>
     <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B216" s="5" t="s">
         <v>12</v>
@@ -10228,7 +10219,7 @@
     </row>
     <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B217" s="9" t="s">
         <v>13</v>
@@ -10272,7 +10263,7 @@
     </row>
     <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B218" s="9" t="s">
         <v>13</v>
@@ -10314,7 +10305,7 @@
     </row>
     <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B219" s="9" t="s">
         <v>13</v>
@@ -10356,7 +10347,7 @@
     </row>
     <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A220" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B220" s="12" t="s">
         <v>14</v>
@@ -10400,7 +10391,7 @@
     </row>
     <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A221" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B221" s="16" t="s">
         <v>15</v>
@@ -10446,7 +10437,7 @@
     </row>
     <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A222" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B222" s="16" t="s">
         <v>15</v>
@@ -10490,7 +10481,7 @@
     </row>
     <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B223" s="16" t="s">
         <v>15</v>
@@ -10536,7 +10527,7 @@
     </row>
     <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A224" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B224" s="20" t="s">
         <v>16</v>
@@ -10580,7 +10571,7 @@
     </row>
     <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B225" s="24" t="s">
         <v>17</v>
@@ -10624,7 +10615,7 @@
     </row>
     <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A226" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B226" s="28" t="s">
         <v>18</v>
@@ -10670,7 +10661,7 @@
     </row>
     <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A227" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B227" s="28" t="s">
         <v>18</v>
@@ -10714,7 +10705,7 @@
     </row>
     <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B228" s="28" t="s">
         <v>18</v>
@@ -10760,7 +10751,7 @@
     </row>
     <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A229" s="32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B229" s="32" t="s">
         <v>19</v>
@@ -10804,7 +10795,7 @@
     </row>
     <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B230" s="5" t="s">
         <v>20</v>
@@ -10873,31 +10864,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="46" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="46" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -10908,7 +10899,7 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D2">
         <v>96</v>
@@ -10928,7 +10919,7 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D3">
         <v>39</v>
@@ -10954,7 +10945,7 @@
         <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D4">
         <v>73</v>
@@ -10980,7 +10971,7 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D5">
         <v>9</v>
@@ -11000,7 +10991,7 @@
         <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D6">
         <v>45</v>
@@ -11023,7 +11014,7 @@
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D7">
         <v>65</v>
@@ -11049,7 +11040,7 @@
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D8">
         <v>16</v>
@@ -11072,7 +11063,7 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D9">
         <v>48</v>
@@ -11098,7 +11089,7 @@
         <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D10">
         <v>77</v>
@@ -11121,7 +11112,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D11">
         <v>57</v>
@@ -11147,7 +11138,7 @@
         <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D12">
         <v>25</v>
@@ -11170,7 +11161,7 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -11187,10 +11178,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D14">
         <v>16</v>
@@ -11213,7 +11204,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D15">
         <v>88</v>
@@ -11233,7 +11224,7 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D16">
         <v>7</v>
@@ -11256,7 +11247,7 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D17">
         <v>31</v>
@@ -11276,7 +11267,7 @@
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D18">
         <v>60</v>
@@ -11299,7 +11290,7 @@
         <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D19">
         <v>48</v>
@@ -11322,7 +11313,7 @@
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D20">
         <v>35</v>
@@ -11345,7 +11336,7 @@
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D21">
         <v>21</v>
@@ -11368,7 +11359,7 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D22">
         <v>22</v>
@@ -11394,212 +11385,255 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>48</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2">
         <v>62</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>63</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4">
         <v>29</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>28</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5">
         <v>58</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>57</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6">
         <v>76</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>77</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7">
         <v>86</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>85</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8">
         <v>15</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9">
         <v>27</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>28</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10">
         <v>32</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>72</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11">
         <v>38</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>71</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12">
         <v>43</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>67</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13">
         <v>52</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>68</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14">
         <v>9</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>77</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Line and Section to TrackData file with classes for each. Organized Blocks into Sections and Sections into Lines. Added full instantiation of Station and Switch objects. Added print methods for all TrackModel classes.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -9,19 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BLOCK" sheetId="2" r:id="rId1"/>
-    <sheet name="STATION" sheetId="8" r:id="rId2"/>
-    <sheet name="SWITCH" sheetId="7" r:id="rId3"/>
+    <sheet name="LINE" sheetId="9" r:id="rId1"/>
+    <sheet name="SECTION" sheetId="10" r:id="rId2"/>
+    <sheet name="BLOCK" sheetId="2" r:id="rId3"/>
+    <sheet name="STATION" sheetId="8" r:id="rId4"/>
+    <sheet name="SWITCH" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="76">
   <si>
     <t>A</t>
   </si>
@@ -819,11 +821,457 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P221" sqref="P221"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1040,7 +1488,7 @@
       <c r="C5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="9">
         <v>3</v>
       </c>
       <c r="F5" s="10">
@@ -10841,7 +11289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
@@ -11383,11 +11831,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>

</xml_diff>

<commit_message>
Fixed small typo in TrackData file.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -854,7 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -11293,9 +11293,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11387,7 +11387,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Refactored blockASection and blockBSection variables to sectionA and sectionB.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -232,12 +232,6 @@
     <t>stationID</t>
   </si>
   <si>
-    <t>blockASection</t>
-  </si>
-  <si>
-    <t>blockBSection</t>
-  </si>
-  <si>
     <t>rightSide</t>
   </si>
   <si>
@@ -251,6 +245,12 @@
   </si>
   <si>
     <t>portC</t>
+  </si>
+  <si>
+    <t>sectionA</t>
+  </si>
+  <si>
+    <t>sectionB</t>
   </si>
 </sst>
 </file>
@@ -836,12 +836,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -870,7 +870,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -918,7 +918,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -990,7 +990,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
         <v>2</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
@@ -1166,7 +1166,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
@@ -1174,7 +1174,7 @@
     </row>
     <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B44" t="s">
         <v>14</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B46" t="s">
         <v>16</v>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
         <v>17</v>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
         <v>18</v>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B49" t="s">
         <v>19</v>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B50" t="s">
         <v>20</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>0</v>
@@ -1480,7 +1480,7 @@
     </row>
     <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>1</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>1</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>1</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>2</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>2</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>2</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>2</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>2</v>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>2</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>3</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>3</v>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>3</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>3</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>4</v>
@@ -2082,7 +2082,7 @@
     </row>
     <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>4</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>4</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>4</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>5</v>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>5</v>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>5</v>
@@ -2340,7 +2340,7 @@
     </row>
     <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>5</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>5</v>
@@ -2424,7 +2424,7 @@
     </row>
     <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>5</v>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>5</v>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>5</v>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>6</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>6</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>6</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>6</v>
@@ -2723,7 +2723,7 @@
     </row>
     <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B34" s="32" t="s">
         <v>7</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B35" s="32" t="s">
         <v>7</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B36" s="32" t="s">
         <v>7</v>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>8</v>
@@ -2901,7 +2901,7 @@
     </row>
     <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>8</v>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>8</v>
@@ -2989,7 +2989,7 @@
     </row>
     <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>8</v>
@@ -3033,7 +3033,7 @@
     </row>
     <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>8</v>
@@ -3077,7 +3077,7 @@
     </row>
     <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>8</v>
@@ -3121,7 +3121,7 @@
     </row>
     <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>8</v>
@@ -3165,7 +3165,7 @@
     </row>
     <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>8</v>
@@ -3209,7 +3209,7 @@
     </row>
     <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>8</v>
@@ -3253,7 +3253,7 @@
     </row>
     <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>8</v>
@@ -3297,7 +3297,7 @@
     </row>
     <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>8</v>
@@ -3341,7 +3341,7 @@
     </row>
     <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>8</v>
@@ -3385,7 +3385,7 @@
     </row>
     <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>8</v>
@@ -3429,7 +3429,7 @@
     </row>
     <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>8</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>8</v>
@@ -3517,7 +3517,7 @@
     </row>
     <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>8</v>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>8</v>
@@ -3605,7 +3605,7 @@
     </row>
     <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>8</v>
@@ -3649,7 +3649,7 @@
     </row>
     <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>8</v>
@@ -3693,7 +3693,7 @@
     </row>
     <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>8</v>
@@ -3737,7 +3737,7 @@
     </row>
     <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>8</v>
@@ -3781,7 +3781,7 @@
     </row>
     <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>8</v>
@@ -3825,7 +3825,7 @@
     </row>
     <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>9</v>
@@ -3870,7 +3870,7 @@
     </row>
     <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>9</v>
@@ -3912,7 +3912,7 @@
     </row>
     <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>9</v>
@@ -3954,7 +3954,7 @@
     </row>
     <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>9</v>
@@ -3994,7 +3994,7 @@
     </row>
     <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>9</v>
@@ -4038,7 +4038,7 @@
     </row>
     <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>10</v>
@@ -4083,7 +4083,7 @@
     </row>
     <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B65" s="12" t="s">
         <v>10</v>
@@ -4125,7 +4125,7 @@
     </row>
     <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B66" s="12" t="s">
         <v>10</v>
@@ -4167,7 +4167,7 @@
     </row>
     <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B67" s="12" t="s">
         <v>10</v>
@@ -4209,7 +4209,7 @@
     </row>
     <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B68" s="12" t="s">
         <v>10</v>
@@ -4251,7 +4251,7 @@
     </row>
     <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B69" s="12" t="s">
         <v>10</v>
@@ -4295,7 +4295,7 @@
     </row>
     <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B70" s="16" t="s">
         <v>11</v>
@@ -4340,7 +4340,7 @@
     </row>
     <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B71" s="16" t="s">
         <v>11</v>
@@ -4382,7 +4382,7 @@
     </row>
     <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B72" s="16" t="s">
         <v>11</v>
@@ -4424,7 +4424,7 @@
     </row>
     <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B73" s="16" t="s">
         <v>11</v>
@@ -4466,7 +4466,7 @@
     </row>
     <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B74" s="16" t="s">
         <v>11</v>
@@ -4510,7 +4510,7 @@
     </row>
     <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B75" s="20" t="s">
         <v>12</v>
@@ -4555,7 +4555,7 @@
     </row>
     <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B76" s="20" t="s">
         <v>12</v>
@@ -4597,7 +4597,7 @@
     </row>
     <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B77" s="20" t="s">
         <v>12</v>
@@ -4641,7 +4641,7 @@
     </row>
     <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B78" s="24" t="s">
         <v>13</v>
@@ -4683,7 +4683,7 @@
     </row>
     <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B79" s="24" t="s">
         <v>13</v>
@@ -4725,7 +4725,7 @@
     </row>
     <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B80" s="24" t="s">
         <v>13</v>
@@ -4767,7 +4767,7 @@
     </row>
     <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B81" s="24" t="s">
         <v>13</v>
@@ -4809,7 +4809,7 @@
     </row>
     <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B82" s="24" t="s">
         <v>13</v>
@@ -4851,7 +4851,7 @@
     </row>
     <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B83" s="24" t="s">
         <v>13</v>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B84" s="24" t="s">
         <v>13</v>
@@ -4935,7 +4935,7 @@
     </row>
     <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B85" s="24" t="s">
         <v>13</v>
@@ -4977,7 +4977,7 @@
     </row>
     <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B86" s="24" t="s">
         <v>13</v>
@@ -5019,7 +5019,7 @@
     </row>
     <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B87" s="28" t="s">
         <v>14</v>
@@ -5064,7 +5064,7 @@
     </row>
     <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B88" s="28" t="s">
         <v>14</v>
@@ -5106,7 +5106,7 @@
     </row>
     <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B89" s="28" t="s">
         <v>14</v>
@@ -5150,7 +5150,7 @@
     </row>
     <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B90" s="32" t="s">
         <v>15</v>
@@ -5195,7 +5195,7 @@
     </row>
     <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B91" s="32" t="s">
         <v>15</v>
@@ -5237,7 +5237,7 @@
     </row>
     <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B92" s="32" t="s">
         <v>15</v>
@@ -5279,7 +5279,7 @@
     </row>
     <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B93" s="32" t="s">
         <v>15</v>
@@ -5321,7 +5321,7 @@
     </row>
     <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B94" s="32" t="s">
         <v>15</v>
@@ -5363,7 +5363,7 @@
     </row>
     <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B95" s="32" t="s">
         <v>15</v>
@@ -5405,7 +5405,7 @@
     </row>
     <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B96" s="32" t="s">
         <v>15</v>
@@ -5447,7 +5447,7 @@
     </row>
     <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B97" s="32" t="s">
         <v>15</v>
@@ -5489,7 +5489,7 @@
     </row>
     <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B98" s="32" t="s">
         <v>15</v>
@@ -5533,7 +5533,7 @@
     </row>
     <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>16</v>
@@ -5578,7 +5578,7 @@
     </row>
     <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>16</v>
@@ -5620,7 +5620,7 @@
     </row>
     <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>16</v>
@@ -5662,7 +5662,7 @@
     </row>
     <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B102" s="9" t="s">
         <v>17</v>
@@ -5707,7 +5707,7 @@
     </row>
     <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B103" s="12" t="s">
         <v>18</v>
@@ -5752,7 +5752,7 @@
     </row>
     <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B104" s="12" t="s">
         <v>18</v>
@@ -5794,7 +5794,7 @@
     </row>
     <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B105" s="12" t="s">
         <v>18</v>
@@ -5838,7 +5838,7 @@
     </row>
     <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B106" s="16" t="s">
         <v>19</v>
@@ -5883,7 +5883,7 @@
     </row>
     <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B107" s="16" t="s">
         <v>19</v>
@@ -5925,7 +5925,7 @@
     </row>
     <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B108" s="16" t="s">
         <v>19</v>
@@ -5967,7 +5967,7 @@
     </row>
     <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B109" s="16" t="s">
         <v>19</v>
@@ -6009,7 +6009,7 @@
     </row>
     <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B110" s="16" t="s">
         <v>19</v>
@@ -6053,7 +6053,7 @@
     </row>
     <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B111" s="20" t="s">
         <v>20</v>
@@ -6098,7 +6098,7 @@
     </row>
     <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B112" s="20" t="s">
         <v>20</v>
@@ -6140,7 +6140,7 @@
     </row>
     <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B113" s="20" t="s">
         <v>20</v>
@@ -6182,7 +6182,7 @@
     </row>
     <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B114" s="20" t="s">
         <v>20</v>
@@ -6224,7 +6224,7 @@
     </row>
     <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B115" s="20" t="s">
         <v>20</v>
@@ -6266,7 +6266,7 @@
     </row>
     <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B116" s="20" t="s">
         <v>20</v>
@@ -6308,7 +6308,7 @@
     </row>
     <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B117" s="20" t="s">
         <v>20</v>
@@ -6352,7 +6352,7 @@
     </row>
     <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B118" s="24" t="s">
         <v>21</v>
@@ -6397,7 +6397,7 @@
     </row>
     <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B119" s="24" t="s">
         <v>21</v>
@@ -6439,7 +6439,7 @@
     </row>
     <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B120" s="24" t="s">
         <v>21</v>
@@ -6481,7 +6481,7 @@
     </row>
     <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B121" s="24" t="s">
         <v>21</v>
@@ -6523,7 +6523,7 @@
     </row>
     <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B122" s="24" t="s">
         <v>21</v>
@@ -6567,7 +6567,7 @@
     </row>
     <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B123" s="28" t="s">
         <v>22</v>
@@ -6614,7 +6614,7 @@
     </row>
     <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B124" s="28" t="s">
         <v>22</v>
@@ -6658,7 +6658,7 @@
     </row>
     <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B125" s="28" t="s">
         <v>22</v>
@@ -6702,7 +6702,7 @@
     </row>
     <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B126" s="28" t="s">
         <v>22</v>
@@ -6746,7 +6746,7 @@
     </row>
     <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B127" s="28" t="s">
         <v>22</v>
@@ -6790,7 +6790,7 @@
     </row>
     <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B128" s="28" t="s">
         <v>22</v>
@@ -6834,7 +6834,7 @@
     </row>
     <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B129" s="28" t="s">
         <v>22</v>
@@ -6878,7 +6878,7 @@
     </row>
     <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B130" s="28" t="s">
         <v>22</v>
@@ -6922,7 +6922,7 @@
     </row>
     <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B131" s="28" t="s">
         <v>22</v>
@@ -6966,7 +6966,7 @@
     </row>
     <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B132" s="28" t="s">
         <v>22</v>
@@ -7010,7 +7010,7 @@
     </row>
     <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B133" s="28" t="s">
         <v>22</v>
@@ -7054,7 +7054,7 @@
     </row>
     <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B134" s="28" t="s">
         <v>22</v>
@@ -7098,7 +7098,7 @@
     </row>
     <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B135" s="28" t="s">
         <v>22</v>
@@ -7142,7 +7142,7 @@
     </row>
     <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B136" s="28" t="s">
         <v>22</v>
@@ -7186,7 +7186,7 @@
     </row>
     <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B137" s="28" t="s">
         <v>22</v>
@@ -7230,7 +7230,7 @@
     </row>
     <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B138" s="28" t="s">
         <v>22</v>
@@ -7274,7 +7274,7 @@
     </row>
     <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B139" s="28" t="s">
         <v>22</v>
@@ -7318,7 +7318,7 @@
     </row>
     <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B140" s="28" t="s">
         <v>22</v>
@@ -7362,7 +7362,7 @@
     </row>
     <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B141" s="28" t="s">
         <v>22</v>
@@ -7406,7 +7406,7 @@
     </row>
     <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B142" s="28" t="s">
         <v>22</v>
@@ -7450,7 +7450,7 @@
     </row>
     <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B143" s="28" t="s">
         <v>22</v>
@@ -7494,7 +7494,7 @@
     </row>
     <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B144" s="28" t="s">
         <v>22</v>
@@ -7540,7 +7540,7 @@
     </row>
     <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B145" s="32" t="s">
         <v>23</v>
@@ -7585,7 +7585,7 @@
     </row>
     <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B146" s="32" t="s">
         <v>23</v>
@@ -7627,7 +7627,7 @@
     </row>
     <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B147" s="32" t="s">
         <v>23</v>
@@ -7671,7 +7671,7 @@
     </row>
     <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>24</v>
@@ -7716,7 +7716,7 @@
     </row>
     <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>24</v>
@@ -7758,7 +7758,7 @@
     </row>
     <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>24</v>
@@ -7802,7 +7802,7 @@
     </row>
     <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B151" s="9" t="s">
         <v>25</v>
@@ -7847,7 +7847,7 @@
     </row>
     <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B152" s="12" t="s">
         <v>26</v>
@@ -7892,7 +7892,7 @@
     </row>
     <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B153" s="16" t="s">
         <v>27</v>
@@ -7937,7 +7937,7 @@
     </row>
     <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B154" s="20" t="s">
         <v>0</v>
@@ -7979,7 +7979,7 @@
     </row>
     <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B155" s="20" t="s">
         <v>0</v>
@@ -8021,7 +8021,7 @@
     </row>
     <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B156" s="20" t="s">
         <v>0</v>
@@ -8065,7 +8065,7 @@
     </row>
     <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B157" s="24" t="s">
         <v>1</v>
@@ -8109,7 +8109,7 @@
     </row>
     <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B158" s="24" t="s">
         <v>1</v>
@@ -8151,7 +8151,7 @@
     </row>
     <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B159" s="24" t="s">
         <v>1</v>
@@ -8195,7 +8195,7 @@
     </row>
     <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B160" s="28" t="s">
         <v>2</v>
@@ -8239,7 +8239,7 @@
     </row>
     <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B161" s="28" t="s">
         <v>2</v>
@@ -8281,7 +8281,7 @@
     </row>
     <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B162" s="28" t="s">
         <v>2</v>
@@ -8325,7 +8325,7 @@
     </row>
     <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B163" s="32" t="s">
         <v>3</v>
@@ -8367,7 +8367,7 @@
     </row>
     <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B164" s="32" t="s">
         <v>3</v>
@@ -8409,7 +8409,7 @@
     </row>
     <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B165" s="32" t="s">
         <v>3</v>
@@ -8453,7 +8453,7 @@
     </row>
     <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>4</v>
@@ -8497,7 +8497,7 @@
     </row>
     <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>4</v>
@@ -8539,7 +8539,7 @@
     </row>
     <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B168" s="5" t="s">
         <v>4</v>
@@ -8583,7 +8583,7 @@
     </row>
     <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B169" s="9" t="s">
         <v>5</v>
@@ -8625,7 +8625,7 @@
     </row>
     <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B170" s="9" t="s">
         <v>5</v>
@@ -8667,7 +8667,7 @@
     </row>
     <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A171" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B171" s="9" t="s">
         <v>5</v>
@@ -8709,7 +8709,7 @@
     </row>
     <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B172" s="9" t="s">
         <v>5</v>
@@ -8751,7 +8751,7 @@
     </row>
     <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B173" s="9" t="s">
         <v>5</v>
@@ -8795,7 +8795,7 @@
     </row>
     <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B174" s="12" t="s">
         <v>6</v>
@@ -8839,7 +8839,7 @@
     </row>
     <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B175" s="12" t="s">
         <v>6</v>
@@ -8881,7 +8881,7 @@
     </row>
     <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B176" s="12" t="s">
         <v>6</v>
@@ -8925,7 +8925,7 @@
     </row>
     <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A177" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B177" s="16" t="s">
         <v>7</v>
@@ -8971,7 +8971,7 @@
     </row>
     <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B178" s="16" t="s">
         <v>7</v>
@@ -9015,7 +9015,7 @@
     </row>
     <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B179" s="16" t="s">
         <v>7</v>
@@ -9059,7 +9059,7 @@
     </row>
     <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B180" s="16" t="s">
         <v>7</v>
@@ -9103,7 +9103,7 @@
     </row>
     <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A181" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B181" s="16" t="s">
         <v>7</v>
@@ -9145,7 +9145,7 @@
     </row>
     <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B182" s="16" t="s">
         <v>7</v>
@@ -9189,7 +9189,7 @@
     </row>
     <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B183" s="16" t="s">
         <v>7</v>
@@ -9233,7 +9233,7 @@
     </row>
     <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B184" s="16" t="s">
         <v>7</v>
@@ -9277,7 +9277,7 @@
     </row>
     <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B185" s="16" t="s">
         <v>7</v>
@@ -9321,7 +9321,7 @@
     </row>
     <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A186" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B186" s="16" t="s">
         <v>7</v>
@@ -9363,7 +9363,7 @@
     </row>
     <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B187" s="16" t="s">
         <v>7</v>
@@ -9407,7 +9407,7 @@
     </row>
     <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B188" s="16" t="s">
         <v>7</v>
@@ -9451,7 +9451,7 @@
     </row>
     <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B189" s="16" t="s">
         <v>7</v>
@@ -9495,7 +9495,7 @@
     </row>
     <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B190" s="16" t="s">
         <v>7</v>
@@ -9539,7 +9539,7 @@
     </row>
     <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B191" s="16" t="s">
         <v>7</v>
@@ -9583,7 +9583,7 @@
     </row>
     <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B192" s="16" t="s">
         <v>7</v>
@@ -9625,7 +9625,7 @@
     </row>
     <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B193" s="16" t="s">
         <v>7</v>
@@ -9669,7 +9669,7 @@
     </row>
     <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B194" s="16" t="s">
         <v>7</v>
@@ -9713,7 +9713,7 @@
     </row>
     <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A195" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B195" s="16" t="s">
         <v>7</v>
@@ -9757,7 +9757,7 @@
     </row>
     <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B196" s="16" t="s">
         <v>7</v>
@@ -9801,7 +9801,7 @@
     </row>
     <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B197" s="16" t="s">
         <v>7</v>
@@ -9843,7 +9843,7 @@
     </row>
     <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B198" s="16" t="s">
         <v>7</v>
@@ -9889,7 +9889,7 @@
     </row>
     <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A199" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B199" s="20" t="s">
         <v>8</v>
@@ -9935,7 +9935,7 @@
     </row>
     <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A200" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B200" s="20" t="s">
         <v>8</v>
@@ -9979,7 +9979,7 @@
     </row>
     <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A201" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B201" s="20" t="s">
         <v>8</v>
@@ -10023,7 +10023,7 @@
     </row>
     <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B202" s="24" t="s">
         <v>9</v>
@@ -10067,7 +10067,7 @@
     </row>
     <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A203" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B203" s="24" t="s">
         <v>9</v>
@@ -10109,7 +10109,7 @@
     </row>
     <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A204" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B204" s="24" t="s">
         <v>9</v>
@@ -10151,7 +10151,7 @@
     </row>
     <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B205" s="24" t="s">
         <v>9</v>
@@ -10193,7 +10193,7 @@
     </row>
     <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A206" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B206" s="24" t="s">
         <v>9</v>
@@ -10233,7 +10233,7 @@
     </row>
     <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B207" s="24" t="s">
         <v>9</v>
@@ -10277,7 +10277,7 @@
     </row>
     <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B208" s="28" t="s">
         <v>10</v>
@@ -10321,7 +10321,7 @@
     </row>
     <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B209" s="28" t="s">
         <v>10</v>
@@ -10363,7 +10363,7 @@
     </row>
     <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B210" s="28" t="s">
         <v>10</v>
@@ -10407,7 +10407,7 @@
     </row>
     <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B211" s="32" t="s">
         <v>11</v>
@@ -10451,7 +10451,7 @@
     </row>
     <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B212" s="32" t="s">
         <v>11</v>
@@ -10493,7 +10493,7 @@
     </row>
     <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B213" s="32" t="s">
         <v>11</v>
@@ -10537,7 +10537,7 @@
     </row>
     <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B214" s="5" t="s">
         <v>12</v>
@@ -10581,7 +10581,7 @@
     </row>
     <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B215" s="5" t="s">
         <v>12</v>
@@ -10623,7 +10623,7 @@
     </row>
     <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B216" s="5" t="s">
         <v>12</v>
@@ -10667,7 +10667,7 @@
     </row>
     <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B217" s="9" t="s">
         <v>13</v>
@@ -10711,7 +10711,7 @@
     </row>
     <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B218" s="9" t="s">
         <v>13</v>
@@ -10753,7 +10753,7 @@
     </row>
     <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B219" s="9" t="s">
         <v>13</v>
@@ -10795,7 +10795,7 @@
     </row>
     <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A220" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B220" s="12" t="s">
         <v>14</v>
@@ -10839,7 +10839,7 @@
     </row>
     <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A221" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B221" s="16" t="s">
         <v>15</v>
@@ -10885,7 +10885,7 @@
     </row>
     <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A222" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B222" s="16" t="s">
         <v>15</v>
@@ -10929,7 +10929,7 @@
     </row>
     <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B223" s="16" t="s">
         <v>15</v>
@@ -10975,7 +10975,7 @@
     </row>
     <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A224" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B224" s="20" t="s">
         <v>16</v>
@@ -11019,7 +11019,7 @@
     </row>
     <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B225" s="24" t="s">
         <v>17</v>
@@ -11063,7 +11063,7 @@
     </row>
     <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A226" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B226" s="28" t="s">
         <v>18</v>
@@ -11109,7 +11109,7 @@
     </row>
     <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A227" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B227" s="28" t="s">
         <v>18</v>
@@ -11153,7 +11153,7 @@
     </row>
     <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B228" s="28" t="s">
         <v>18</v>
@@ -11199,7 +11199,7 @@
     </row>
     <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A229" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B229" s="32" t="s">
         <v>19</v>
@@ -11243,7 +11243,7 @@
     </row>
     <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B230" s="5" t="s">
         <v>20</v>
@@ -11295,7 +11295,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11303,9 +11303,9 @@
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -11324,19 +11324,19 @@
         <v>66</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>67</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H1" s="46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I1" s="46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -11347,7 +11347,7 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D2">
         <v>96</v>
@@ -11367,7 +11367,7 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D3">
         <v>39</v>
@@ -11393,7 +11393,7 @@
         <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4">
         <v>73</v>
@@ -11419,7 +11419,7 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5">
         <v>9</v>
@@ -11439,7 +11439,7 @@
         <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6">
         <v>45</v>
@@ -11462,7 +11462,7 @@
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7">
         <v>65</v>
@@ -11488,7 +11488,7 @@
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8">
         <v>16</v>
@@ -11511,7 +11511,7 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <v>48</v>
@@ -11537,7 +11537,7 @@
         <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D10">
         <v>77</v>
@@ -11560,7 +11560,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11">
         <v>57</v>
@@ -11586,7 +11586,7 @@
         <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12">
         <v>25</v>
@@ -11609,7 +11609,7 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -11629,7 +11629,7 @@
         <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14">
         <v>16</v>
@@ -11652,7 +11652,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D15">
         <v>88</v>
@@ -11672,7 +11672,7 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D16">
         <v>7</v>
@@ -11695,7 +11695,7 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17">
         <v>31</v>
@@ -11715,7 +11715,7 @@
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D18">
         <v>60</v>
@@ -11738,7 +11738,7 @@
         <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D19">
         <v>48</v>
@@ -11761,7 +11761,7 @@
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D20">
         <v>35</v>
@@ -11784,7 +11784,7 @@
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D21">
         <v>21</v>
@@ -11807,7 +11807,7 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D22">
         <v>22</v>
@@ -11856,7 +11856,7 @@
         <v>54</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -11864,7 +11864,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <v>62</v>
@@ -11881,7 +11881,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -11898,7 +11898,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C4">
         <v>29</v>
@@ -11915,7 +11915,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5">
         <v>58</v>
@@ -11932,7 +11932,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6">
         <v>76</v>
@@ -11949,7 +11949,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7">
         <v>86</v>
@@ -11966,7 +11966,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8">
         <v>15</v>
@@ -11983,7 +11983,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C9">
         <v>27</v>
@@ -12000,7 +12000,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10">
         <v>32</v>
@@ -12017,7 +12017,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11">
         <v>38</v>
@@ -12034,7 +12034,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12">
         <v>43</v>
@@ -12051,7 +12051,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13">
         <v>52</v>
@@ -12068,7 +12068,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14">
         <v>9</v>

</xml_diff>

<commit_message>
Fixed all issues with block/switch/yard connectivity.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -1269,9 +1269,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E211" sqref="E211"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1365,7 +1365,9 @@
       <c r="F2" s="6">
         <v>2</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="6">
+        <v>-1</v>
+      </c>
       <c r="H2" s="5">
         <v>1</v>
       </c>
@@ -1838,7 +1840,9 @@
       <c r="F13" s="13">
         <v>11</v>
       </c>
-      <c r="G13" s="13"/>
+      <c r="G13" s="13">
+        <v>-1</v>
+      </c>
       <c r="H13" s="12">
         <v>1</v>
       </c>
@@ -1882,7 +1886,9 @@
       <c r="F14" s="16">
         <v>14</v>
       </c>
-      <c r="G14" s="16"/>
+      <c r="G14" s="16">
+        <v>-1</v>
+      </c>
       <c r="H14" s="16">
         <v>1</v>
       </c>
@@ -2522,7 +2528,9 @@
       <c r="F29" s="24">
         <v>27</v>
       </c>
-      <c r="G29" s="24"/>
+      <c r="G29" s="24">
+        <v>-1</v>
+      </c>
       <c r="H29" s="24">
         <v>2</v>
       </c>
@@ -2565,7 +2573,9 @@
       <c r="F30" s="28">
         <v>30</v>
       </c>
-      <c r="G30" s="28"/>
+      <c r="G30" s="28">
+        <v>-1</v>
+      </c>
       <c r="H30" s="28">
         <v>2</v>
       </c>
@@ -3795,7 +3805,9 @@
       <c r="F58" s="5">
         <v>56</v>
       </c>
-      <c r="G58" s="5"/>
+      <c r="G58" s="5">
+        <v>-1</v>
+      </c>
       <c r="H58" s="5">
         <v>3</v>
       </c>
@@ -3840,7 +3852,9 @@
       <c r="F59" s="9">
         <v>59</v>
       </c>
-      <c r="G59" s="9"/>
+      <c r="G59" s="9">
+        <v>-1</v>
+      </c>
       <c r="H59" s="9">
         <v>3</v>
       </c>
@@ -3966,9 +3980,11 @@
       <c r="F62" s="9">
         <v>60</v>
       </c>
-      <c r="G62" s="9"/>
+      <c r="G62" s="9">
+        <v>-1</v>
+      </c>
       <c r="H62" s="9">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I62" s="9">
         <v>50</v>
@@ -4008,9 +4024,11 @@
       <c r="F63" s="10">
         <v>63</v>
       </c>
-      <c r="G63" s="10"/>
+      <c r="G63" s="10">
+        <v>-1</v>
+      </c>
       <c r="H63" s="9">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I63" s="9">
         <v>50</v>
@@ -4611,7 +4629,9 @@
       <c r="F77" s="20">
         <v>75</v>
       </c>
-      <c r="G77" s="20"/>
+      <c r="G77" s="20">
+        <v>-1</v>
+      </c>
       <c r="H77" s="20">
         <v>4</v>
       </c>
@@ -4655,7 +4675,9 @@
       <c r="F78" s="24">
         <v>78</v>
       </c>
-      <c r="G78" s="24"/>
+      <c r="G78" s="24">
+        <v>-1</v>
+      </c>
       <c r="H78" s="24">
         <v>4</v>
       </c>
@@ -4991,7 +5013,9 @@
       <c r="F86" s="24">
         <v>84</v>
       </c>
-      <c r="G86" s="24"/>
+      <c r="G86" s="24">
+        <v>-1</v>
+      </c>
       <c r="H86" s="24">
         <v>5</v>
       </c>
@@ -5034,7 +5058,9 @@
       <c r="F87" s="30">
         <v>87</v>
       </c>
-      <c r="G87" s="30"/>
+      <c r="G87" s="30">
+        <v>-1</v>
+      </c>
       <c r="H87" s="28">
         <v>5</v>
       </c>
@@ -5634,7 +5660,9 @@
       <c r="F101" s="5">
         <v>99</v>
       </c>
-      <c r="G101" s="5"/>
+      <c r="G101" s="5">
+        <v>-1</v>
+      </c>
       <c r="H101" s="5">
         <v>5</v>
       </c>
@@ -5679,7 +5707,9 @@
       <c r="F102" s="9">
         <v>102</v>
       </c>
-      <c r="G102" s="9"/>
+      <c r="G102" s="9">
+        <v>-1</v>
+      </c>
       <c r="H102" s="9">
         <v>4</v>
       </c>
@@ -7819,7 +7849,9 @@
       <c r="F151" s="10">
         <v>149</v>
       </c>
-      <c r="G151" s="10"/>
+      <c r="G151" s="10">
+        <v>-1</v>
+      </c>
       <c r="H151" s="9">
         <v>2</v>
       </c>
@@ -7864,7 +7896,9 @@
       <c r="F152" s="13">
         <v>0</v>
       </c>
-      <c r="G152" s="13"/>
+      <c r="G152" s="13">
+        <v>-1</v>
+      </c>
       <c r="H152" s="12">
         <v>3</v>
       </c>
@@ -7909,9 +7943,11 @@
       <c r="F153" s="18">
         <v>0</v>
       </c>
-      <c r="G153" s="18"/>
+      <c r="G153" s="18">
+        <v>-1</v>
+      </c>
       <c r="H153" s="16">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I153" s="16">
         <v>50</v>
@@ -7951,7 +7987,9 @@
       <c r="F154" s="21">
         <v>2</v>
       </c>
-      <c r="G154" s="21"/>
+      <c r="G154" s="21">
+        <v>-1</v>
+      </c>
       <c r="H154" s="20">
         <v>6</v>
       </c>
@@ -8295,7 +8333,9 @@
       <c r="F162" s="28">
         <v>8</v>
       </c>
-      <c r="G162" s="28"/>
+      <c r="G162" s="28">
+        <v>-1</v>
+      </c>
       <c r="H162" s="28">
         <v>12</v>
       </c>
@@ -8339,7 +8379,9 @@
       <c r="F163" s="34">
         <v>11</v>
       </c>
-      <c r="G163" s="34"/>
+      <c r="G163" s="34">
+        <v>-1</v>
+      </c>
       <c r="H163" s="32">
         <v>12</v>
       </c>
@@ -8553,7 +8595,9 @@
       <c r="F168" s="6">
         <v>14</v>
       </c>
-      <c r="G168" s="6"/>
+      <c r="G168" s="6">
+        <v>-1</v>
+      </c>
       <c r="H168" s="5">
         <v>6</v>
       </c>
@@ -8597,7 +8641,9 @@
       <c r="F169" s="9">
         <v>17</v>
       </c>
-      <c r="G169" s="9"/>
+      <c r="G169" s="9">
+        <v>-1</v>
+      </c>
       <c r="H169" s="9">
         <v>6</v>
       </c>
@@ -9071,7 +9117,9 @@
       <c r="F180" s="18">
         <v>26</v>
       </c>
-      <c r="G180" s="18"/>
+      <c r="G180" s="18">
+        <v>-1</v>
+      </c>
       <c r="H180" s="16">
         <v>7</v>
       </c>
@@ -9115,7 +9163,9 @@
       <c r="F181" s="16">
         <v>29</v>
       </c>
-      <c r="G181" s="16"/>
+      <c r="G181" s="16">
+        <v>-1</v>
+      </c>
       <c r="H181" s="16">
         <v>7</v>
       </c>
@@ -9289,7 +9339,9 @@
       <c r="F185" s="18">
         <v>31</v>
       </c>
-      <c r="G185" s="18"/>
+      <c r="G185" s="18">
+        <v>-1</v>
+      </c>
       <c r="H185" s="16">
         <v>8</v>
       </c>
@@ -9333,7 +9385,9 @@
       <c r="F186" s="16">
         <v>34</v>
       </c>
-      <c r="G186" s="16"/>
+      <c r="G186" s="16">
+        <v>-1</v>
+      </c>
       <c r="H186" s="16">
         <v>8</v>
       </c>
@@ -9551,7 +9605,9 @@
       <c r="F191" s="18">
         <v>37</v>
       </c>
-      <c r="G191" s="18"/>
+      <c r="G191" s="18">
+        <v>-1</v>
+      </c>
       <c r="H191" s="16">
         <v>9</v>
       </c>
@@ -9595,7 +9651,9 @@
       <c r="F192" s="16">
         <v>40</v>
       </c>
-      <c r="G192" s="16"/>
+      <c r="G192" s="16">
+        <v>-1</v>
+      </c>
       <c r="H192" s="16">
         <v>9</v>
       </c>
@@ -9769,7 +9827,9 @@
       <c r="F196" s="16">
         <v>42</v>
       </c>
-      <c r="G196" s="16"/>
+      <c r="G196" s="16">
+        <v>-1</v>
+      </c>
       <c r="H196" s="16">
         <v>10</v>
       </c>
@@ -9813,7 +9873,9 @@
       <c r="F197" s="18">
         <v>45</v>
       </c>
-      <c r="G197" s="18"/>
+      <c r="G197" s="18">
+        <v>-1</v>
+      </c>
       <c r="H197" s="16">
         <v>10</v>
       </c>
@@ -10163,7 +10225,9 @@
       <c r="F205" s="24">
         <v>51</v>
       </c>
-      <c r="G205" s="24"/>
+      <c r="G205" s="24">
+        <v>-1</v>
+      </c>
       <c r="H205" s="24">
         <v>11</v>
       </c>
@@ -10205,7 +10269,9 @@
       <c r="F206" s="26">
         <v>54</v>
       </c>
-      <c r="G206" s="26"/>
+      <c r="G206" s="26">
+        <v>-1</v>
+      </c>
       <c r="H206" s="24">
         <v>11</v>
       </c>
@@ -10767,7 +10833,9 @@
       <c r="F219" s="9">
         <v>65</v>
       </c>
-      <c r="G219" s="9"/>
+      <c r="G219" s="9">
+        <v>-1</v>
+      </c>
       <c r="H219" s="9">
         <v>11</v>
       </c>
@@ -10809,7 +10877,9 @@
       <c r="F220" s="12">
         <v>68</v>
       </c>
-      <c r="G220" s="12"/>
+      <c r="G220" s="12">
+        <v>-1</v>
+      </c>
       <c r="H220" s="12">
         <v>10</v>
       </c>
@@ -10989,7 +11059,9 @@
       <c r="F224" s="21">
         <v>70</v>
       </c>
-      <c r="G224" s="21"/>
+      <c r="G224" s="21">
+        <v>-1</v>
+      </c>
       <c r="H224" s="20">
         <v>9</v>
       </c>
@@ -11033,7 +11105,9 @@
       <c r="F225" s="24">
         <v>73</v>
       </c>
-      <c r="G225" s="24"/>
+      <c r="G225" s="24">
+        <v>-1</v>
+      </c>
       <c r="H225" s="24">
         <v>8</v>
       </c>
@@ -11213,7 +11287,9 @@
       <c r="F229" s="32">
         <v>75</v>
       </c>
-      <c r="G229" s="32"/>
+      <c r="G229" s="32">
+        <v>-1</v>
+      </c>
       <c r="H229" s="32">
         <v>7</v>
       </c>
@@ -11257,7 +11333,9 @@
       <c r="F230" s="6">
         <v>0</v>
       </c>
-      <c r="G230" s="6"/>
+      <c r="G230" s="6">
+        <v>-1</v>
+      </c>
       <c r="H230" s="5">
         <v>12</v>
       </c>
@@ -11835,9 +11913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11861,7 +11939,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Implemented exitBlock() method and a simulated train running through the green line.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -1270,8 +1270,8 @@
   <dimension ref="A1:Q230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11915,7 +11915,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11945,10 +11945,10 @@
         <v>71</v>
       </c>
       <c r="C2">
+        <v>61</v>
+      </c>
+      <c r="D2">
         <v>62</v>
-      </c>
-      <c r="D2">
-        <v>63</v>
       </c>
       <c r="E2">
         <v>152</v>
@@ -11965,10 +11965,10 @@
         <v>12</v>
       </c>
       <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3">
         <v>1</v>
-      </c>
-      <c r="E3">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Trains now dispatch from the Yard.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -11915,7 +11915,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11945,13 +11945,13 @@
         <v>71</v>
       </c>
       <c r="C2">
+        <v>62</v>
+      </c>
+      <c r="D2">
+        <v>152</v>
+      </c>
+      <c r="E2">
         <v>61</v>
-      </c>
-      <c r="D2">
-        <v>62</v>
-      </c>
-      <c r="E2">
-        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
TrainModel occupancy commented out, track data asset file updated
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan94\Documents\Coding\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Kenneson\SCHOOL\University of Pitt\Senior Year\Spring 2017\Software Engineering\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -1269,9 +1269,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q230"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H154" sqref="H154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3984,7 +3984,7 @@
         <v>-1</v>
       </c>
       <c r="H62" s="9">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I62" s="9">
         <v>50</v>
@@ -4028,7 +4028,7 @@
         <v>-1</v>
       </c>
       <c r="H63" s="9">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I63" s="9">
         <v>50</v>
@@ -7947,7 +7947,7 @@
         <v>-1</v>
       </c>
       <c r="H153" s="16">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I153" s="16">
         <v>50</v>
@@ -11913,9 +11913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11939,7 +11939,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Updated track data file to reflect the changes discussed in class.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Kenneson\SCHOOL\University of Pitt\Senior Year\Spring 2017\Software Engineering\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan94\Documents\Coding\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -1269,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H154" sqref="H154"/>
     </sheetView>
@@ -11913,9 +11913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11962,10 +11962,10 @@
         <v>71</v>
       </c>
       <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
         <v>12</v>
-      </c>
-      <c r="D3">
-        <v>13</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -11979,10 +11979,10 @@
         <v>71</v>
       </c>
       <c r="C4">
+        <v>28</v>
+      </c>
+      <c r="D4">
         <v>29</v>
-      </c>
-      <c r="D4">
-        <v>28</v>
       </c>
       <c r="E4">
         <v>150</v>
@@ -11996,10 +11996,10 @@
         <v>71</v>
       </c>
       <c r="C5">
+        <v>57</v>
+      </c>
+      <c r="D5">
         <v>58</v>
-      </c>
-      <c r="D5">
-        <v>57</v>
       </c>
       <c r="E5">
         <v>151</v>
@@ -12013,10 +12013,10 @@
         <v>71</v>
       </c>
       <c r="C6">
+        <v>77</v>
+      </c>
+      <c r="D6">
         <v>76</v>
-      </c>
-      <c r="D6">
-        <v>77</v>
       </c>
       <c r="E6">
         <v>101</v>
@@ -12030,10 +12030,10 @@
         <v>71</v>
       </c>
       <c r="C7">
+        <v>85</v>
+      </c>
+      <c r="D7">
         <v>86</v>
-      </c>
-      <c r="D7">
-        <v>85</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -12047,13 +12047,13 @@
         <v>72</v>
       </c>
       <c r="C8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -12081,13 +12081,13 @@
         <v>72</v>
       </c>
       <c r="C10">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>72</v>
       </c>
       <c r="E10">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -12115,13 +12115,13 @@
         <v>72</v>
       </c>
       <c r="C12">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D12">
         <v>67</v>
       </c>
       <c r="E12">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated TrackData.xlsx switch 2 and 3 to agree with wayside logic
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan94\Documents\Coding\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylemonto/Documents/Pitt/Senior/COE 1186/ECE1186/TrainSystem/src/com/rogueone/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="4"/>
+    <workbookView xWindow="1300" yWindow="6840" windowWidth="33240" windowHeight="11560" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -18,7 +18,15 @@
     <sheet name="STATION" sheetId="8" r:id="rId4"/>
     <sheet name="SWITCH" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -256,7 +264,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -546,9 +554,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -576,31 +584,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -628,23 +619,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -827,19 +801,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -858,9 +832,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
@@ -868,7 +842,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -876,7 +850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -884,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -892,7 +866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -900,7 +874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -908,7 +882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -916,7 +890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -924,7 +898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -932,7 +906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -940,7 +914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -948,7 +922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -956,7 +930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>71</v>
       </c>
@@ -964,7 +938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -972,7 +946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -980,7 +954,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -988,7 +962,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -996,7 +970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -1004,7 +978,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -1012,7 +986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -1020,7 +994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -1028,7 +1002,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -1036,7 +1010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -1044,7 +1018,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -1052,7 +1026,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1060,7 +1034,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -1068,7 +1042,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -1076,7 +1050,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -1084,7 +1058,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -1092,7 +1066,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -1100,7 +1074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -1108,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -1116,7 +1090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -1124,7 +1098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -1132,7 +1106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -1140,7 +1114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -1148,7 +1122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -1156,7 +1130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1164,7 +1138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -1172,7 +1146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1180,7 +1154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -1188,7 +1162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -1196,7 +1170,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -1204,7 +1178,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -1212,7 +1186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -1220,7 +1194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -1228,7 +1202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -1236,7 +1210,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -1244,7 +1218,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -1252,7 +1226,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -1270,33 +1244,33 @@
   <dimension ref="A1:Q230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H154" sqref="H154"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="16" max="16" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -1349,7 +1323,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>71</v>
       </c>
@@ -1393,7 +1367,7 @@
       </c>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>71</v>
       </c>
@@ -1435,7 +1409,7 @@
       </c>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>71</v>
       </c>
@@ -1480,7 +1454,7 @@
       </c>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
@@ -1524,7 +1498,7 @@
       </c>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>71</v>
       </c>
@@ -1566,7 +1540,7 @@
       </c>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>71</v>
       </c>
@@ -1611,7 +1585,7 @@
       </c>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>71</v>
       </c>
@@ -1655,7 +1629,7 @@
       </c>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>71</v>
       </c>
@@ -1697,7 +1671,7 @@
       </c>
       <c r="Q9" s="12"/>
     </row>
-    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>71</v>
       </c>
@@ -1739,7 +1713,7 @@
       </c>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>71</v>
       </c>
@@ -1781,7 +1755,7 @@
       </c>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>71</v>
       </c>
@@ -1823,7 +1797,7 @@
       </c>
       <c r="Q12" s="12"/>
     </row>
-    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>71</v>
       </c>
@@ -1870,7 +1844,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>71</v>
       </c>
@@ -1914,7 +1888,7 @@
       </c>
       <c r="Q14" s="16"/>
     </row>
-    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>71</v>
       </c>
@@ -1956,7 +1930,7 @@
       </c>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>71</v>
       </c>
@@ -1998,7 +1972,7 @@
       </c>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>71</v>
       </c>
@@ -2042,7 +2016,7 @@
       </c>
       <c r="Q17" s="19"/>
     </row>
-    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>71</v>
       </c>
@@ -2086,7 +2060,7 @@
       </c>
       <c r="Q18" s="20"/>
     </row>
-    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>71</v>
       </c>
@@ -2128,7 +2102,7 @@
       </c>
       <c r="Q19" s="20"/>
     </row>
-    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>71</v>
       </c>
@@ -2172,7 +2146,7 @@
       </c>
       <c r="Q20" s="23"/>
     </row>
-    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>71</v>
       </c>
@@ -2216,7 +2190,7 @@
       </c>
       <c r="Q21" s="20"/>
     </row>
-    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
         <v>71</v>
       </c>
@@ -2260,7 +2234,7 @@
       </c>
       <c r="Q22" s="24"/>
     </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
         <v>71</v>
       </c>
@@ -2302,7 +2276,7 @@
       </c>
       <c r="Q23" s="27"/>
     </row>
-    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
         <v>71</v>
       </c>
@@ -2344,7 +2318,7 @@
       </c>
       <c r="Q24" s="24"/>
     </row>
-    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
         <v>71</v>
       </c>
@@ -2386,7 +2360,7 @@
       </c>
       <c r="Q25" s="24"/>
     </row>
-    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="24" t="s">
         <v>71</v>
       </c>
@@ -2428,7 +2402,7 @@
       </c>
       <c r="Q26" s="24"/>
     </row>
-    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
         <v>71</v>
       </c>
@@ -2470,7 +2444,7 @@
       </c>
       <c r="Q27" s="24"/>
     </row>
-    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
         <v>71</v>
       </c>
@@ -2512,7 +2486,7 @@
       </c>
       <c r="Q28" s="24"/>
     </row>
-    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="24" t="s">
         <v>71</v>
       </c>
@@ -2556,7 +2530,7 @@
       </c>
       <c r="Q29" s="24"/>
     </row>
-    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="28" t="s">
         <v>71</v>
       </c>
@@ -2603,7 +2577,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28" t="s">
         <v>71</v>
       </c>
@@ -2645,7 +2619,7 @@
       </c>
       <c r="Q31" s="28"/>
     </row>
-    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
         <v>71</v>
       </c>
@@ -2687,7 +2661,7 @@
       </c>
       <c r="Q32" s="31"/>
     </row>
-    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="28" t="s">
         <v>71</v>
       </c>
@@ -2731,7 +2705,7 @@
       </c>
       <c r="Q33" s="28"/>
     </row>
-    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>71</v>
       </c>
@@ -2776,7 +2750,7 @@
       </c>
       <c r="Q34" s="32"/>
     </row>
-    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>71</v>
       </c>
@@ -2818,7 +2792,7 @@
       </c>
       <c r="Q35" s="32"/>
     </row>
-    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>71</v>
       </c>
@@ -2862,7 +2836,7 @@
       </c>
       <c r="Q36" s="32"/>
     </row>
-    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>71</v>
       </c>
@@ -2909,7 +2883,7 @@
       </c>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>71</v>
       </c>
@@ -2953,7 +2927,7 @@
       </c>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>71</v>
       </c>
@@ -2997,7 +2971,7 @@
       </c>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>71</v>
       </c>
@@ -3041,7 +3015,7 @@
       </c>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>71</v>
       </c>
@@ -3085,7 +3059,7 @@
       </c>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>71</v>
       </c>
@@ -3129,7 +3103,7 @@
       </c>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>71</v>
       </c>
@@ -3173,7 +3147,7 @@
       </c>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>71</v>
       </c>
@@ -3217,7 +3191,7 @@
       </c>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>71</v>
       </c>
@@ -3261,7 +3235,7 @@
       </c>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>71</v>
       </c>
@@ -3305,7 +3279,7 @@
       </c>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>71</v>
       </c>
@@ -3349,7 +3323,7 @@
       </c>
       <c r="Q47" s="5"/>
     </row>
-    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>71</v>
       </c>
@@ -3393,7 +3367,7 @@
       </c>
       <c r="Q48" s="5"/>
     </row>
-    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>71</v>
       </c>
@@ -3437,7 +3411,7 @@
       </c>
       <c r="Q49" s="8"/>
     </row>
-    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>71</v>
       </c>
@@ -3481,7 +3455,7 @@
       </c>
       <c r="Q50" s="5"/>
     </row>
-    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>71</v>
       </c>
@@ -3525,7 +3499,7 @@
       </c>
       <c r="Q51" s="5"/>
     </row>
-    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>71</v>
       </c>
@@ -3569,7 +3543,7 @@
       </c>
       <c r="Q52" s="5"/>
     </row>
-    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>71</v>
       </c>
@@ -3613,7 +3587,7 @@
       </c>
       <c r="Q53" s="5"/>
     </row>
-    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>71</v>
       </c>
@@ -3657,7 +3631,7 @@
       </c>
       <c r="Q54" s="5"/>
     </row>
-    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>71</v>
       </c>
@@ -3701,7 +3675,7 @@
       </c>
       <c r="Q55" s="5"/>
     </row>
-    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>71</v>
       </c>
@@ -3745,7 +3719,7 @@
       </c>
       <c r="Q56" s="5"/>
     </row>
-    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>71</v>
       </c>
@@ -3789,7 +3763,7 @@
       </c>
       <c r="Q57" s="5"/>
     </row>
-    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>71</v>
       </c>
@@ -3835,7 +3809,7 @@
       </c>
       <c r="Q58" s="8"/>
     </row>
-    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
         <v>71</v>
       </c>
@@ -3882,7 +3856,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>71</v>
       </c>
@@ -3924,7 +3898,7 @@
       </c>
       <c r="Q60" s="9"/>
     </row>
-    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>71</v>
       </c>
@@ -3966,7 +3940,7 @@
       </c>
       <c r="Q61" s="9"/>
     </row>
-    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
         <v>71</v>
       </c>
@@ -4008,7 +3982,7 @@
       </c>
       <c r="Q62" s="9"/>
     </row>
-    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>71</v>
       </c>
@@ -4054,7 +4028,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
         <v>71</v>
       </c>
@@ -4099,7 +4073,7 @@
       </c>
       <c r="Q64" s="12"/>
     </row>
-    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
         <v>71</v>
       </c>
@@ -4141,7 +4115,7 @@
       </c>
       <c r="Q65" s="12"/>
     </row>
-    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
         <v>71</v>
       </c>
@@ -4183,7 +4157,7 @@
       </c>
       <c r="Q66" s="14"/>
     </row>
-    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
         <v>71</v>
       </c>
@@ -4225,7 +4199,7 @@
       </c>
       <c r="Q67" s="12"/>
     </row>
-    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="s">
         <v>71</v>
       </c>
@@ -4267,7 +4241,7 @@
       </c>
       <c r="Q68" s="12"/>
     </row>
-    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="12" t="s">
         <v>71</v>
       </c>
@@ -4311,7 +4285,7 @@
       </c>
       <c r="Q69" s="12"/>
     </row>
-    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="16" t="s">
         <v>71</v>
       </c>
@@ -4356,7 +4330,7 @@
       </c>
       <c r="Q70" s="16"/>
     </row>
-    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="s">
         <v>71</v>
       </c>
@@ -4398,7 +4372,7 @@
       </c>
       <c r="Q71" s="16"/>
     </row>
-    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="16" t="s">
         <v>71</v>
       </c>
@@ -4440,7 +4414,7 @@
       </c>
       <c r="Q72" s="16"/>
     </row>
-    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="16" t="s">
         <v>71</v>
       </c>
@@ -4482,7 +4456,7 @@
       </c>
       <c r="Q73" s="16"/>
     </row>
-    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="16" t="s">
         <v>71</v>
       </c>
@@ -4526,7 +4500,7 @@
       </c>
       <c r="Q74" s="19"/>
     </row>
-    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
         <v>71</v>
       </c>
@@ -4571,7 +4545,7 @@
       </c>
       <c r="Q75" s="20"/>
     </row>
-    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
         <v>71</v>
       </c>
@@ -4613,7 +4587,7 @@
       </c>
       <c r="Q76" s="20"/>
     </row>
-    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="20" t="s">
         <v>71</v>
       </c>
@@ -4659,7 +4633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="24" t="s">
         <v>71</v>
       </c>
@@ -4703,7 +4677,7 @@
       </c>
       <c r="Q78" s="27"/>
     </row>
-    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="24" t="s">
         <v>71</v>
       </c>
@@ -4745,7 +4719,7 @@
       </c>
       <c r="Q79" s="24"/>
     </row>
-    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="24" t="s">
         <v>71</v>
       </c>
@@ -4787,7 +4761,7 @@
       </c>
       <c r="Q80" s="24"/>
     </row>
-    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="24" t="s">
         <v>71</v>
       </c>
@@ -4829,7 +4803,7 @@
       </c>
       <c r="Q81" s="24"/>
     </row>
-    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="24" t="s">
         <v>71</v>
       </c>
@@ -4871,7 +4845,7 @@
       </c>
       <c r="Q82" s="24"/>
     </row>
-    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="24" t="s">
         <v>71</v>
       </c>
@@ -4913,7 +4887,7 @@
       </c>
       <c r="Q83" s="24"/>
     </row>
-    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="24" t="s">
         <v>71</v>
       </c>
@@ -4955,7 +4929,7 @@
       </c>
       <c r="Q84" s="24"/>
     </row>
-    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="24" t="s">
         <v>71</v>
       </c>
@@ -4997,7 +4971,7 @@
       </c>
       <c r="Q85" s="24"/>
     </row>
-    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="24" t="s">
         <v>71</v>
       </c>
@@ -5041,7 +5015,7 @@
       </c>
       <c r="Q86" s="24"/>
     </row>
-    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="28" t="s">
         <v>71</v>
       </c>
@@ -5088,7 +5062,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="28" t="s">
         <v>71</v>
       </c>
@@ -5130,7 +5104,7 @@
       </c>
       <c r="Q88" s="28"/>
     </row>
-    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="28" t="s">
         <v>71</v>
       </c>
@@ -5174,7 +5148,7 @@
       </c>
       <c r="Q89" s="31"/>
     </row>
-    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="32" t="s">
         <v>71</v>
       </c>
@@ -5219,7 +5193,7 @@
       </c>
       <c r="Q90" s="32"/>
     </row>
-    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="32" t="s">
         <v>71</v>
       </c>
@@ -5261,7 +5235,7 @@
       </c>
       <c r="Q91" s="32"/>
     </row>
-    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="32" t="s">
         <v>71</v>
       </c>
@@ -5303,7 +5277,7 @@
       </c>
       <c r="Q92" s="32"/>
     </row>
-    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="32" t="s">
         <v>71</v>
       </c>
@@ -5345,7 +5319,7 @@
       </c>
       <c r="Q93" s="32"/>
     </row>
-    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="32" t="s">
         <v>71</v>
       </c>
@@ -5387,7 +5361,7 @@
       </c>
       <c r="Q94" s="32"/>
     </row>
-    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="32" t="s">
         <v>71</v>
       </c>
@@ -5429,7 +5403,7 @@
       </c>
       <c r="Q95" s="32"/>
     </row>
-    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="32" t="s">
         <v>71</v>
       </c>
@@ -5471,7 +5445,7 @@
       </c>
       <c r="Q96" s="32"/>
     </row>
-    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="32" t="s">
         <v>71</v>
       </c>
@@ -5513,7 +5487,7 @@
       </c>
       <c r="Q97" s="36"/>
     </row>
-    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="32" t="s">
         <v>71</v>
       </c>
@@ -5557,7 +5531,7 @@
       </c>
       <c r="Q98" s="32"/>
     </row>
-    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>71</v>
       </c>
@@ -5602,7 +5576,7 @@
       </c>
       <c r="Q99" s="5"/>
     </row>
-    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>71</v>
       </c>
@@ -5644,7 +5618,7 @@
       </c>
       <c r="Q100" s="5"/>
     </row>
-    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>71</v>
       </c>
@@ -5688,7 +5662,7 @@
       </c>
       <c r="Q101" s="5"/>
     </row>
-    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
         <v>71</v>
       </c>
@@ -5735,7 +5709,7 @@
       </c>
       <c r="Q102" s="9"/>
     </row>
-    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="12" t="s">
         <v>71</v>
       </c>
@@ -5780,7 +5754,7 @@
       </c>
       <c r="Q103" s="12"/>
     </row>
-    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="12" t="s">
         <v>71</v>
       </c>
@@ -5822,7 +5796,7 @@
       </c>
       <c r="Q104" s="12"/>
     </row>
-    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="12" t="s">
         <v>71</v>
       </c>
@@ -5866,7 +5840,7 @@
       </c>
       <c r="Q105" s="12"/>
     </row>
-    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="16" t="s">
         <v>71</v>
       </c>
@@ -5911,7 +5885,7 @@
       </c>
       <c r="Q106" s="19"/>
     </row>
-    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="16" t="s">
         <v>71</v>
       </c>
@@ -5953,7 +5927,7 @@
       </c>
       <c r="Q107" s="16"/>
     </row>
-    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="16" t="s">
         <v>71</v>
       </c>
@@ -5995,7 +5969,7 @@
       </c>
       <c r="Q108" s="16"/>
     </row>
-    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="16" t="s">
         <v>71</v>
       </c>
@@ -6037,7 +6011,7 @@
       </c>
       <c r="Q109" s="16"/>
     </row>
-    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="16" t="s">
         <v>71</v>
       </c>
@@ -6081,7 +6055,7 @@
       </c>
       <c r="Q110" s="16"/>
     </row>
-    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="20" t="s">
         <v>71</v>
       </c>
@@ -6126,7 +6100,7 @@
       </c>
       <c r="Q111" s="20"/>
     </row>
-    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="20" t="s">
         <v>71</v>
       </c>
@@ -6168,7 +6142,7 @@
       </c>
       <c r="Q112" s="20"/>
     </row>
-    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="20" t="s">
         <v>71</v>
       </c>
@@ -6210,7 +6184,7 @@
       </c>
       <c r="Q113" s="20"/>
     </row>
-    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="20" t="s">
         <v>71</v>
       </c>
@@ -6252,7 +6226,7 @@
       </c>
       <c r="Q114" s="20"/>
     </row>
-    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="20" t="s">
         <v>71</v>
       </c>
@@ -6294,7 +6268,7 @@
       </c>
       <c r="Q115" s="23"/>
     </row>
-    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="20" t="s">
         <v>71</v>
       </c>
@@ -6336,7 +6310,7 @@
       </c>
       <c r="Q116" s="20"/>
     </row>
-    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="20" t="s">
         <v>71</v>
       </c>
@@ -6380,7 +6354,7 @@
       </c>
       <c r="Q117" s="20"/>
     </row>
-    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="24" t="s">
         <v>71</v>
       </c>
@@ -6425,7 +6399,7 @@
       </c>
       <c r="Q118" s="24"/>
     </row>
-    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="24" t="s">
         <v>71</v>
       </c>
@@ -6467,7 +6441,7 @@
       </c>
       <c r="Q119" s="24"/>
     </row>
-    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="24" t="s">
         <v>71</v>
       </c>
@@ -6509,7 +6483,7 @@
       </c>
       <c r="Q120" s="24"/>
     </row>
-    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="24" t="s">
         <v>71</v>
       </c>
@@ -6551,7 +6525,7 @@
       </c>
       <c r="Q121" s="24"/>
     </row>
-    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="24" t="s">
         <v>71</v>
       </c>
@@ -6595,7 +6569,7 @@
       </c>
       <c r="Q122" s="24"/>
     </row>
-    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="28" t="s">
         <v>71</v>
       </c>
@@ -6642,7 +6616,7 @@
       </c>
       <c r="Q123" s="28"/>
     </row>
-    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="28" t="s">
         <v>71</v>
       </c>
@@ -6686,7 +6660,7 @@
       </c>
       <c r="Q124" s="28"/>
     </row>
-    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="28" t="s">
         <v>71</v>
       </c>
@@ -6730,7 +6704,7 @@
       </c>
       <c r="Q125" s="28"/>
     </row>
-    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="28" t="s">
         <v>71</v>
       </c>
@@ -6774,7 +6748,7 @@
       </c>
       <c r="Q126" s="28"/>
     </row>
-    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="28" t="s">
         <v>71</v>
       </c>
@@ -6818,7 +6792,7 @@
       </c>
       <c r="Q127" s="28"/>
     </row>
-    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="28" t="s">
         <v>71</v>
       </c>
@@ -6862,7 +6836,7 @@
       </c>
       <c r="Q128" s="28"/>
     </row>
-    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="28" t="s">
         <v>71</v>
       </c>
@@ -6906,7 +6880,7 @@
       </c>
       <c r="Q129" s="28"/>
     </row>
-    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="28" t="s">
         <v>71</v>
       </c>
@@ -6950,7 +6924,7 @@
       </c>
       <c r="Q130" s="28"/>
     </row>
-    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="28" t="s">
         <v>71</v>
       </c>
@@ -6994,7 +6968,7 @@
       </c>
       <c r="Q131" s="28"/>
     </row>
-    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="28" t="s">
         <v>71</v>
       </c>
@@ -7038,7 +7012,7 @@
       </c>
       <c r="Q132" s="28"/>
     </row>
-    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="28" t="s">
         <v>71</v>
       </c>
@@ -7082,7 +7056,7 @@
       </c>
       <c r="Q133" s="28"/>
     </row>
-    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="28" t="s">
         <v>71</v>
       </c>
@@ -7126,7 +7100,7 @@
       </c>
       <c r="Q134" s="28"/>
     </row>
-    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="28" t="s">
         <v>71</v>
       </c>
@@ -7170,7 +7144,7 @@
       </c>
       <c r="Q135" s="28"/>
     </row>
-    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="28" t="s">
         <v>71</v>
       </c>
@@ -7214,7 +7188,7 @@
       </c>
       <c r="Q136" s="28"/>
     </row>
-    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="28" t="s">
         <v>71</v>
       </c>
@@ -7258,7 +7232,7 @@
       </c>
       <c r="Q137" s="28"/>
     </row>
-    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="28" t="s">
         <v>71</v>
       </c>
@@ -7302,7 +7276,7 @@
       </c>
       <c r="Q138" s="28"/>
     </row>
-    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="28" t="s">
         <v>71</v>
       </c>
@@ -7346,7 +7320,7 @@
       </c>
       <c r="Q139" s="28"/>
     </row>
-    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="28" t="s">
         <v>71</v>
       </c>
@@ -7390,7 +7364,7 @@
       </c>
       <c r="Q140" s="28"/>
     </row>
-    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="28" t="s">
         <v>71</v>
       </c>
@@ -7434,7 +7408,7 @@
       </c>
       <c r="Q141" s="28"/>
     </row>
-    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="28" t="s">
         <v>71</v>
       </c>
@@ -7478,7 +7452,7 @@
       </c>
       <c r="Q142" s="28"/>
     </row>
-    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="28" t="s">
         <v>71</v>
       </c>
@@ -7522,7 +7496,7 @@
       </c>
       <c r="Q143" s="28"/>
     </row>
-    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="28" t="s">
         <v>71</v>
       </c>
@@ -7568,7 +7542,7 @@
       </c>
       <c r="Q144" s="28"/>
     </row>
-    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="32" t="s">
         <v>71</v>
       </c>
@@ -7613,7 +7587,7 @@
       </c>
       <c r="Q145" s="32"/>
     </row>
-    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="32" t="s">
         <v>71</v>
       </c>
@@ -7655,7 +7629,7 @@
       </c>
       <c r="Q146" s="32"/>
     </row>
-    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="32" t="s">
         <v>71</v>
       </c>
@@ -7699,7 +7673,7 @@
       </c>
       <c r="Q147" s="32"/>
     </row>
-    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
         <v>71</v>
       </c>
@@ -7744,7 +7718,7 @@
       </c>
       <c r="Q148" s="5"/>
     </row>
-    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
         <v>71</v>
       </c>
@@ -7786,7 +7760,7 @@
       </c>
       <c r="Q149" s="5"/>
     </row>
-    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
         <v>71</v>
       </c>
@@ -7830,7 +7804,7 @@
       </c>
       <c r="Q150" s="5"/>
     </row>
-    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="9" t="s">
         <v>71</v>
       </c>
@@ -7877,7 +7851,7 @@
       </c>
       <c r="Q151" s="9"/>
     </row>
-    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="12" t="s">
         <v>71</v>
       </c>
@@ -7924,7 +7898,7 @@
       </c>
       <c r="Q152" s="12"/>
     </row>
-    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="16" t="s">
         <v>71</v>
       </c>
@@ -7971,7 +7945,7 @@
       </c>
       <c r="Q153" s="16"/>
     </row>
-    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="20" t="s">
         <v>72</v>
       </c>
@@ -8015,7 +7989,7 @@
       </c>
       <c r="Q154" s="20"/>
     </row>
-    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="20" t="s">
         <v>72</v>
       </c>
@@ -8057,7 +8031,7 @@
       </c>
       <c r="Q155" s="20"/>
     </row>
-    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="20" t="s">
         <v>72</v>
       </c>
@@ -8101,7 +8075,7 @@
       </c>
       <c r="Q156" s="20"/>
     </row>
-    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="24" t="s">
         <v>72</v>
       </c>
@@ -8145,7 +8119,7 @@
       </c>
       <c r="Q157" s="24"/>
     </row>
-    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="24" t="s">
         <v>72</v>
       </c>
@@ -8187,7 +8161,7 @@
       </c>
       <c r="Q158" s="24"/>
     </row>
-    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="24" t="s">
         <v>72</v>
       </c>
@@ -8231,7 +8205,7 @@
       </c>
       <c r="Q159" s="24"/>
     </row>
-    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="28" t="s">
         <v>72</v>
       </c>
@@ -8275,7 +8249,7 @@
       </c>
       <c r="Q160" s="31"/>
     </row>
-    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="28" t="s">
         <v>72</v>
       </c>
@@ -8317,7 +8291,7 @@
       </c>
       <c r="Q161" s="28"/>
     </row>
-    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="28" t="s">
         <v>72</v>
       </c>
@@ -8363,7 +8337,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163" s="32" t="s">
         <v>72</v>
       </c>
@@ -8407,7 +8381,7 @@
       </c>
       <c r="Q163" s="32"/>
     </row>
-    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="32" t="s">
         <v>72</v>
       </c>
@@ -8449,7 +8423,7 @@
       </c>
       <c r="Q164" s="32"/>
     </row>
-    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="32" t="s">
         <v>72</v>
       </c>
@@ -8493,7 +8467,7 @@
       </c>
       <c r="Q165" s="32"/>
     </row>
-    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
         <v>72</v>
       </c>
@@ -8537,7 +8511,7 @@
       </c>
       <c r="Q166" s="5"/>
     </row>
-    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
         <v>72</v>
       </c>
@@ -8579,7 +8553,7 @@
       </c>
       <c r="Q167" s="5"/>
     </row>
-    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
         <v>72</v>
       </c>
@@ -8625,7 +8599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="9" t="s">
         <v>72</v>
       </c>
@@ -8669,7 +8643,7 @@
       </c>
       <c r="Q169" s="35"/>
     </row>
-    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="9" t="s">
         <v>72</v>
       </c>
@@ -8711,7 +8685,7 @@
       </c>
       <c r="Q170" s="9"/>
     </row>
-    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A171" s="9" t="s">
         <v>72</v>
       </c>
@@ -8753,7 +8727,7 @@
       </c>
       <c r="Q171" s="9"/>
     </row>
-    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172" s="9" t="s">
         <v>72</v>
       </c>
@@ -8795,7 +8769,7 @@
       </c>
       <c r="Q172" s="9"/>
     </row>
-    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A173" s="9" t="s">
         <v>72</v>
       </c>
@@ -8839,7 +8813,7 @@
       </c>
       <c r="Q173" s="9"/>
     </row>
-    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="12" t="s">
         <v>72</v>
       </c>
@@ -8883,7 +8857,7 @@
       </c>
       <c r="Q174" s="14"/>
     </row>
-    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175" s="12" t="s">
         <v>72</v>
       </c>
@@ -8925,7 +8899,7 @@
       </c>
       <c r="Q175" s="12"/>
     </row>
-    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A176" s="12" t="s">
         <v>72</v>
       </c>
@@ -8969,7 +8943,7 @@
       </c>
       <c r="Q176" s="12"/>
     </row>
-    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A177" s="16" t="s">
         <v>72</v>
       </c>
@@ -9015,7 +8989,7 @@
       </c>
       <c r="Q177" s="16"/>
     </row>
-    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A178" s="16" t="s">
         <v>72</v>
       </c>
@@ -9059,7 +9033,7 @@
       </c>
       <c r="Q178" s="19"/>
     </row>
-    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A179" s="16" t="s">
         <v>72</v>
       </c>
@@ -9103,7 +9077,7 @@
       </c>
       <c r="Q179" s="16"/>
     </row>
-    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A180" s="16" t="s">
         <v>72</v>
       </c>
@@ -9149,7 +9123,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A181" s="16" t="s">
         <v>72</v>
       </c>
@@ -9193,7 +9167,7 @@
       </c>
       <c r="Q181" s="16"/>
     </row>
-    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A182" s="16" t="s">
         <v>72</v>
       </c>
@@ -9237,7 +9211,7 @@
       </c>
       <c r="Q182" s="16"/>
     </row>
-    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A183" s="16" t="s">
         <v>72</v>
       </c>
@@ -9281,7 +9255,7 @@
       </c>
       <c r="Q183" s="16"/>
     </row>
-    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A184" s="16" t="s">
         <v>72</v>
       </c>
@@ -9325,7 +9299,7 @@
       </c>
       <c r="Q184" s="16"/>
     </row>
-    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A185" s="16" t="s">
         <v>72</v>
       </c>
@@ -9371,7 +9345,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A186" s="16" t="s">
         <v>72</v>
       </c>
@@ -9415,7 +9389,7 @@
       </c>
       <c r="Q186" s="16"/>
     </row>
-    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A187" s="16" t="s">
         <v>72</v>
       </c>
@@ -9459,7 +9433,7 @@
       </c>
       <c r="Q187" s="16"/>
     </row>
-    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A188" s="16" t="s">
         <v>72</v>
       </c>
@@ -9503,7 +9477,7 @@
       </c>
       <c r="Q188" s="19"/>
     </row>
-    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A189" s="16" t="s">
         <v>72</v>
       </c>
@@ -9547,7 +9521,7 @@
       </c>
       <c r="Q189" s="16"/>
     </row>
-    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A190" s="16" t="s">
         <v>72</v>
       </c>
@@ -9591,7 +9565,7 @@
       </c>
       <c r="Q190" s="16"/>
     </row>
-    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A191" s="16" t="s">
         <v>72</v>
       </c>
@@ -9637,7 +9611,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192" s="16" t="s">
         <v>72</v>
       </c>
@@ -9681,7 +9655,7 @@
       </c>
       <c r="Q192" s="16"/>
     </row>
-    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193" s="16" t="s">
         <v>72</v>
       </c>
@@ -9725,7 +9699,7 @@
       </c>
       <c r="Q193" s="16"/>
     </row>
-    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="16" t="s">
         <v>72</v>
       </c>
@@ -9769,7 +9743,7 @@
       </c>
       <c r="Q194" s="16"/>
     </row>
-    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="16" t="s">
         <v>72</v>
       </c>
@@ -9813,7 +9787,7 @@
       </c>
       <c r="Q195" s="16"/>
     </row>
-    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196" s="16" t="s">
         <v>72</v>
       </c>
@@ -9859,7 +9833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A197" s="16" t="s">
         <v>72</v>
       </c>
@@ -9903,7 +9877,7 @@
       </c>
       <c r="Q197" s="16"/>
     </row>
-    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198" s="16" t="s">
         <v>72</v>
       </c>
@@ -9949,7 +9923,7 @@
       </c>
       <c r="Q198" s="19"/>
     </row>
-    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199" s="20" t="s">
         <v>72</v>
       </c>
@@ -9995,7 +9969,7 @@
       </c>
       <c r="Q199" s="20"/>
     </row>
-    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200" s="20" t="s">
         <v>72</v>
       </c>
@@ -10039,7 +10013,7 @@
       </c>
       <c r="Q200" s="23"/>
     </row>
-    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201" s="20" t="s">
         <v>72</v>
       </c>
@@ -10083,7 +10057,7 @@
       </c>
       <c r="Q201" s="23"/>
     </row>
-    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202" s="24" t="s">
         <v>72</v>
       </c>
@@ -10127,7 +10101,7 @@
       </c>
       <c r="Q202" s="24"/>
     </row>
-    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A203" s="24" t="s">
         <v>72</v>
       </c>
@@ -10169,7 +10143,7 @@
       </c>
       <c r="Q203" s="24"/>
     </row>
-    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204" s="24" t="s">
         <v>72</v>
       </c>
@@ -10211,7 +10185,7 @@
       </c>
       <c r="Q204" s="24"/>
     </row>
-    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A205" s="24" t="s">
         <v>72</v>
       </c>
@@ -10255,7 +10229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206" s="24" t="s">
         <v>72</v>
       </c>
@@ -10297,7 +10271,7 @@
       </c>
       <c r="Q206" s="24"/>
     </row>
-    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A207" s="24" t="s">
         <v>72</v>
       </c>
@@ -10341,7 +10315,7 @@
       </c>
       <c r="Q207" s="24"/>
     </row>
-    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A208" s="28" t="s">
         <v>72</v>
       </c>
@@ -10385,7 +10359,7 @@
       </c>
       <c r="Q208" s="28"/>
     </row>
-    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A209" s="28" t="s">
         <v>72</v>
       </c>
@@ -10427,7 +10401,7 @@
       </c>
       <c r="Q209" s="28"/>
     </row>
-    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" s="28" t="s">
         <v>72</v>
       </c>
@@ -10471,7 +10445,7 @@
       </c>
       <c r="Q210" s="28"/>
     </row>
-    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A211" s="32" t="s">
         <v>72</v>
       </c>
@@ -10515,7 +10489,7 @@
       </c>
       <c r="Q211" s="32"/>
     </row>
-    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A212" s="32" t="s">
         <v>72</v>
       </c>
@@ -10557,7 +10531,7 @@
       </c>
       <c r="Q212" s="32"/>
     </row>
-    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A213" s="32" t="s">
         <v>72</v>
       </c>
@@ -10601,7 +10575,7 @@
       </c>
       <c r="Q213" s="36"/>
     </row>
-    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A214" s="5" t="s">
         <v>72</v>
       </c>
@@ -10645,7 +10619,7 @@
       </c>
       <c r="Q214" s="5"/>
     </row>
-    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A215" s="5" t="s">
         <v>72</v>
       </c>
@@ -10687,7 +10661,7 @@
       </c>
       <c r="Q215" s="5"/>
     </row>
-    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A216" s="5" t="s">
         <v>72</v>
       </c>
@@ -10731,7 +10705,7 @@
       </c>
       <c r="Q216" s="5"/>
     </row>
-    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A217" s="9" t="s">
         <v>72</v>
       </c>
@@ -10775,7 +10749,7 @@
       </c>
       <c r="Q217" s="9"/>
     </row>
-    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218" s="9" t="s">
         <v>72</v>
       </c>
@@ -10817,7 +10791,7 @@
       </c>
       <c r="Q218" s="9"/>
     </row>
-    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A219" s="9" t="s">
         <v>72</v>
       </c>
@@ -10861,7 +10835,7 @@
       </c>
       <c r="Q219" s="9"/>
     </row>
-    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A220" s="12" t="s">
         <v>72</v>
       </c>
@@ -10907,7 +10881,7 @@
       </c>
       <c r="Q220" s="12"/>
     </row>
-    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A221" s="16" t="s">
         <v>72</v>
       </c>
@@ -10953,7 +10927,7 @@
       </c>
       <c r="Q221" s="16"/>
     </row>
-    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A222" s="16" t="s">
         <v>72</v>
       </c>
@@ -10997,7 +10971,7 @@
       </c>
       <c r="Q222" s="16"/>
     </row>
-    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A223" s="16" t="s">
         <v>72</v>
       </c>
@@ -11043,7 +11017,7 @@
       </c>
       <c r="Q223" s="16"/>
     </row>
-    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A224" s="20" t="s">
         <v>72</v>
       </c>
@@ -11089,7 +11063,7 @@
       </c>
       <c r="Q224" s="20"/>
     </row>
-    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225" s="24" t="s">
         <v>72</v>
       </c>
@@ -11135,7 +11109,7 @@
       </c>
       <c r="Q225" s="24"/>
     </row>
-    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A226" s="28" t="s">
         <v>72</v>
       </c>
@@ -11181,7 +11155,7 @@
       </c>
       <c r="Q226" s="28"/>
     </row>
-    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A227" s="28" t="s">
         <v>72</v>
       </c>
@@ -11225,7 +11199,7 @@
       </c>
       <c r="Q227" s="28"/>
     </row>
-    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A228" s="28" t="s">
         <v>72</v>
       </c>
@@ -11271,7 +11245,7 @@
       </c>
       <c r="Q228" s="28"/>
     </row>
-    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A229" s="32" t="s">
         <v>72</v>
       </c>
@@ -11317,7 +11291,7 @@
       </c>
       <c r="Q229" s="32"/>
     </row>
-    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A230" s="5" t="s">
         <v>72</v>
       </c>
@@ -11376,19 +11350,19 @@
       <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
         <v>68</v>
       </c>
@@ -11417,7 +11391,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11437,7 +11411,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11463,7 +11437,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11489,7 +11463,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11509,7 +11483,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11532,7 +11506,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11558,7 +11532,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11581,7 +11555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11607,7 +11581,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11630,7 +11604,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11656,7 +11630,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11679,7 +11653,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11699,7 +11673,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11722,7 +11696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11742,7 +11716,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11765,7 +11739,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11785,7 +11759,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11808,7 +11782,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -11831,7 +11805,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -11854,7 +11828,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -11877,7 +11851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -11915,12 +11889,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>55</v>
       </c>
@@ -11937,7 +11911,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -11954,7 +11928,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -11971,7 +11945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -11982,13 +11956,13 @@
         <v>28</v>
       </c>
       <c r="D4">
+        <v>150</v>
+      </c>
+      <c r="E4">
         <v>29</v>
       </c>
-      <c r="E4">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -11999,13 +11973,13 @@
         <v>57</v>
       </c>
       <c r="D5">
+        <v>151</v>
+      </c>
+      <c r="E5">
         <v>58</v>
       </c>
-      <c r="E5">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -12022,7 +11996,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -12039,7 +12013,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -12056,7 +12030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -12073,7 +12047,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -12090,7 +12064,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -12107,7 +12081,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -12124,7 +12098,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -12141,7 +12115,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Removed track side information from Stations.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylemonto/Documents/Pitt/Senior/COE 1186/ECE1186/TrainSystem/src/com/rogueone/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan94\Documents\Coding\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="6840" windowWidth="33240" windowHeight="11560" activeTab="4"/>
+    <workbookView xWindow="1296" yWindow="6840" windowWidth="33240" windowHeight="11556" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="74">
   <si>
     <t>A</t>
   </si>
@@ -240,12 +240,6 @@
     <t>stationID</t>
   </si>
   <si>
-    <t>rightSide</t>
-  </si>
-  <si>
-    <t>leftSide</t>
-  </si>
-  <si>
     <t>GREEN</t>
   </si>
   <si>
@@ -264,7 +258,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -801,21 +795,21 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -832,9 +826,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
@@ -842,393 +836,393 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B44" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B47" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
         <v>20</v>
@@ -1248,29 +1242,29 @@
       <selection pane="bottomLeft" activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.83203125" style="1"/>
+    <col min="16" max="16" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -1323,9 +1317,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -1367,9 +1361,9 @@
       </c>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -1409,9 +1403,9 @@
       </c>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>0</v>
@@ -1454,9 +1448,9 @@
       </c>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>1</v>
@@ -1498,9 +1492,9 @@
       </c>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>1</v>
@@ -1540,9 +1534,9 @@
       </c>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>1</v>
@@ -1585,9 +1579,9 @@
       </c>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>2</v>
@@ -1629,9 +1623,9 @@
       </c>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>2</v>
@@ -1671,9 +1665,9 @@
       </c>
       <c r="Q9" s="12"/>
     </row>
-    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>2</v>
@@ -1713,9 +1707,9 @@
       </c>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>2</v>
@@ -1755,9 +1749,9 @@
       </c>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>2</v>
@@ -1797,9 +1791,9 @@
       </c>
       <c r="Q12" s="12"/>
     </row>
-    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>2</v>
@@ -1844,9 +1838,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>3</v>
@@ -1888,9 +1882,9 @@
       </c>
       <c r="Q14" s="16"/>
     </row>
-    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>3</v>
@@ -1930,9 +1924,9 @@
       </c>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>3</v>
@@ -1972,9 +1966,9 @@
       </c>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>3</v>
@@ -2016,9 +2010,9 @@
       </c>
       <c r="Q17" s="19"/>
     </row>
-    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>4</v>
@@ -2060,9 +2054,9 @@
       </c>
       <c r="Q18" s="20"/>
     </row>
-    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>4</v>
@@ -2102,9 +2096,9 @@
       </c>
       <c r="Q19" s="20"/>
     </row>
-    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>4</v>
@@ -2146,9 +2140,9 @@
       </c>
       <c r="Q20" s="23"/>
     </row>
-    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>4</v>
@@ -2190,9 +2184,9 @@
       </c>
       <c r="Q21" s="20"/>
     </row>
-    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>5</v>
@@ -2234,9 +2228,9 @@
       </c>
       <c r="Q22" s="24"/>
     </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>5</v>
@@ -2276,9 +2270,9 @@
       </c>
       <c r="Q23" s="27"/>
     </row>
-    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>5</v>
@@ -2318,9 +2312,9 @@
       </c>
       <c r="Q24" s="24"/>
     </row>
-    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>5</v>
@@ -2360,9 +2354,9 @@
       </c>
       <c r="Q25" s="24"/>
     </row>
-    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>5</v>
@@ -2402,9 +2396,9 @@
       </c>
       <c r="Q26" s="24"/>
     </row>
-    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>5</v>
@@ -2444,9 +2438,9 @@
       </c>
       <c r="Q27" s="24"/>
     </row>
-    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>5</v>
@@ -2486,9 +2480,9 @@
       </c>
       <c r="Q28" s="24"/>
     </row>
-    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>5</v>
@@ -2530,9 +2524,9 @@
       </c>
       <c r="Q29" s="24"/>
     </row>
-    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>6</v>
@@ -2577,9 +2571,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>6</v>
@@ -2619,9 +2613,9 @@
       </c>
       <c r="Q31" s="28"/>
     </row>
-    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>6</v>
@@ -2661,9 +2655,9 @@
       </c>
       <c r="Q32" s="31"/>
     </row>
-    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>6</v>
@@ -2705,9 +2699,9 @@
       </c>
       <c r="Q33" s="28"/>
     </row>
-    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B34" s="32" t="s">
         <v>7</v>
@@ -2750,9 +2744,9 @@
       </c>
       <c r="Q34" s="32"/>
     </row>
-    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B35" s="32" t="s">
         <v>7</v>
@@ -2792,9 +2786,9 @@
       </c>
       <c r="Q35" s="32"/>
     </row>
-    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B36" s="32" t="s">
         <v>7</v>
@@ -2836,9 +2830,9 @@
       </c>
       <c r="Q36" s="32"/>
     </row>
-    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>8</v>
@@ -2883,9 +2877,9 @@
       </c>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>8</v>
@@ -2927,9 +2921,9 @@
       </c>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>8</v>
@@ -2971,9 +2965,9 @@
       </c>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>8</v>
@@ -3015,9 +3009,9 @@
       </c>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>8</v>
@@ -3059,9 +3053,9 @@
       </c>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>8</v>
@@ -3103,9 +3097,9 @@
       </c>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>8</v>
@@ -3147,9 +3141,9 @@
       </c>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>8</v>
@@ -3191,9 +3185,9 @@
       </c>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>8</v>
@@ -3235,9 +3229,9 @@
       </c>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>8</v>
@@ -3279,9 +3273,9 @@
       </c>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>8</v>
@@ -3323,9 +3317,9 @@
       </c>
       <c r="Q47" s="5"/>
     </row>
-    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>8</v>
@@ -3367,9 +3361,9 @@
       </c>
       <c r="Q48" s="5"/>
     </row>
-    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>8</v>
@@ -3411,9 +3405,9 @@
       </c>
       <c r="Q49" s="8"/>
     </row>
-    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>8</v>
@@ -3455,9 +3449,9 @@
       </c>
       <c r="Q50" s="5"/>
     </row>
-    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>8</v>
@@ -3499,9 +3493,9 @@
       </c>
       <c r="Q51" s="5"/>
     </row>
-    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>8</v>
@@ -3543,9 +3537,9 @@
       </c>
       <c r="Q52" s="5"/>
     </row>
-    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>8</v>
@@ -3587,9 +3581,9 @@
       </c>
       <c r="Q53" s="5"/>
     </row>
-    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>8</v>
@@ -3631,9 +3625,9 @@
       </c>
       <c r="Q54" s="5"/>
     </row>
-    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>8</v>
@@ -3675,9 +3669,9 @@
       </c>
       <c r="Q55" s="5"/>
     </row>
-    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>8</v>
@@ -3719,9 +3713,9 @@
       </c>
       <c r="Q56" s="5"/>
     </row>
-    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>8</v>
@@ -3763,9 +3757,9 @@
       </c>
       <c r="Q57" s="5"/>
     </row>
-    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>8</v>
@@ -3809,9 +3803,9 @@
       </c>
       <c r="Q58" s="8"/>
     </row>
-    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>9</v>
@@ -3856,9 +3850,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>9</v>
@@ -3898,9 +3892,9 @@
       </c>
       <c r="Q60" s="9"/>
     </row>
-    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>9</v>
@@ -3940,9 +3934,9 @@
       </c>
       <c r="Q61" s="9"/>
     </row>
-    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>9</v>
@@ -3982,9 +3976,9 @@
       </c>
       <c r="Q62" s="9"/>
     </row>
-    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>9</v>
@@ -4028,9 +4022,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>10</v>
@@ -4073,9 +4067,9 @@
       </c>
       <c r="Q64" s="12"/>
     </row>
-    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B65" s="12" t="s">
         <v>10</v>
@@ -4115,9 +4109,9 @@
       </c>
       <c r="Q65" s="12"/>
     </row>
-    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B66" s="12" t="s">
         <v>10</v>
@@ -4157,9 +4151,9 @@
       </c>
       <c r="Q66" s="14"/>
     </row>
-    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B67" s="12" t="s">
         <v>10</v>
@@ -4199,9 +4193,9 @@
       </c>
       <c r="Q67" s="12"/>
     </row>
-    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B68" s="12" t="s">
         <v>10</v>
@@ -4241,9 +4235,9 @@
       </c>
       <c r="Q68" s="12"/>
     </row>
-    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B69" s="12" t="s">
         <v>10</v>
@@ -4285,9 +4279,9 @@
       </c>
       <c r="Q69" s="12"/>
     </row>
-    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B70" s="16" t="s">
         <v>11</v>
@@ -4330,9 +4324,9 @@
       </c>
       <c r="Q70" s="16"/>
     </row>
-    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B71" s="16" t="s">
         <v>11</v>
@@ -4372,9 +4366,9 @@
       </c>
       <c r="Q71" s="16"/>
     </row>
-    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B72" s="16" t="s">
         <v>11</v>
@@ -4414,9 +4408,9 @@
       </c>
       <c r="Q72" s="16"/>
     </row>
-    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B73" s="16" t="s">
         <v>11</v>
@@ -4456,9 +4450,9 @@
       </c>
       <c r="Q73" s="16"/>
     </row>
-    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B74" s="16" t="s">
         <v>11</v>
@@ -4500,9 +4494,9 @@
       </c>
       <c r="Q74" s="19"/>
     </row>
-    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B75" s="20" t="s">
         <v>12</v>
@@ -4545,9 +4539,9 @@
       </c>
       <c r="Q75" s="20"/>
     </row>
-    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B76" s="20" t="s">
         <v>12</v>
@@ -4587,9 +4581,9 @@
       </c>
       <c r="Q76" s="20"/>
     </row>
-    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B77" s="20" t="s">
         <v>12</v>
@@ -4633,9 +4627,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B78" s="24" t="s">
         <v>13</v>
@@ -4677,9 +4671,9 @@
       </c>
       <c r="Q78" s="27"/>
     </row>
-    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B79" s="24" t="s">
         <v>13</v>
@@ -4719,9 +4713,9 @@
       </c>
       <c r="Q79" s="24"/>
     </row>
-    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B80" s="24" t="s">
         <v>13</v>
@@ -4761,9 +4755,9 @@
       </c>
       <c r="Q80" s="24"/>
     </row>
-    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B81" s="24" t="s">
         <v>13</v>
@@ -4803,9 +4797,9 @@
       </c>
       <c r="Q81" s="24"/>
     </row>
-    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B82" s="24" t="s">
         <v>13</v>
@@ -4845,9 +4839,9 @@
       </c>
       <c r="Q82" s="24"/>
     </row>
-    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B83" s="24" t="s">
         <v>13</v>
@@ -4887,9 +4881,9 @@
       </c>
       <c r="Q83" s="24"/>
     </row>
-    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B84" s="24" t="s">
         <v>13</v>
@@ -4929,9 +4923,9 @@
       </c>
       <c r="Q84" s="24"/>
     </row>
-    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B85" s="24" t="s">
         <v>13</v>
@@ -4971,9 +4965,9 @@
       </c>
       <c r="Q85" s="24"/>
     </row>
-    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B86" s="24" t="s">
         <v>13</v>
@@ -5015,9 +5009,9 @@
       </c>
       <c r="Q86" s="24"/>
     </row>
-    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B87" s="28" t="s">
         <v>14</v>
@@ -5062,9 +5056,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B88" s="28" t="s">
         <v>14</v>
@@ -5104,9 +5098,9 @@
       </c>
       <c r="Q88" s="28"/>
     </row>
-    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B89" s="28" t="s">
         <v>14</v>
@@ -5148,9 +5142,9 @@
       </c>
       <c r="Q89" s="31"/>
     </row>
-    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B90" s="32" t="s">
         <v>15</v>
@@ -5193,9 +5187,9 @@
       </c>
       <c r="Q90" s="32"/>
     </row>
-    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B91" s="32" t="s">
         <v>15</v>
@@ -5235,9 +5229,9 @@
       </c>
       <c r="Q91" s="32"/>
     </row>
-    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B92" s="32" t="s">
         <v>15</v>
@@ -5277,9 +5271,9 @@
       </c>
       <c r="Q92" s="32"/>
     </row>
-    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B93" s="32" t="s">
         <v>15</v>
@@ -5319,9 +5313,9 @@
       </c>
       <c r="Q93" s="32"/>
     </row>
-    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B94" s="32" t="s">
         <v>15</v>
@@ -5361,9 +5355,9 @@
       </c>
       <c r="Q94" s="32"/>
     </row>
-    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B95" s="32" t="s">
         <v>15</v>
@@ -5403,9 +5397,9 @@
       </c>
       <c r="Q95" s="32"/>
     </row>
-    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B96" s="32" t="s">
         <v>15</v>
@@ -5445,9 +5439,9 @@
       </c>
       <c r="Q96" s="32"/>
     </row>
-    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B97" s="32" t="s">
         <v>15</v>
@@ -5487,9 +5481,9 @@
       </c>
       <c r="Q97" s="36"/>
     </row>
-    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B98" s="32" t="s">
         <v>15</v>
@@ -5531,9 +5525,9 @@
       </c>
       <c r="Q98" s="32"/>
     </row>
-    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>16</v>
@@ -5576,9 +5570,9 @@
       </c>
       <c r="Q99" s="5"/>
     </row>
-    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>16</v>
@@ -5618,9 +5612,9 @@
       </c>
       <c r="Q100" s="5"/>
     </row>
-    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>16</v>
@@ -5662,9 +5656,9 @@
       </c>
       <c r="Q101" s="5"/>
     </row>
-    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B102" s="9" t="s">
         <v>17</v>
@@ -5709,9 +5703,9 @@
       </c>
       <c r="Q102" s="9"/>
     </row>
-    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B103" s="12" t="s">
         <v>18</v>
@@ -5754,9 +5748,9 @@
       </c>
       <c r="Q103" s="12"/>
     </row>
-    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B104" s="12" t="s">
         <v>18</v>
@@ -5796,9 +5790,9 @@
       </c>
       <c r="Q104" s="12"/>
     </row>
-    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B105" s="12" t="s">
         <v>18</v>
@@ -5840,9 +5834,9 @@
       </c>
       <c r="Q105" s="12"/>
     </row>
-    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B106" s="16" t="s">
         <v>19</v>
@@ -5885,9 +5879,9 @@
       </c>
       <c r="Q106" s="19"/>
     </row>
-    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B107" s="16" t="s">
         <v>19</v>
@@ -5927,9 +5921,9 @@
       </c>
       <c r="Q107" s="16"/>
     </row>
-    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B108" s="16" t="s">
         <v>19</v>
@@ -5969,9 +5963,9 @@
       </c>
       <c r="Q108" s="16"/>
     </row>
-    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B109" s="16" t="s">
         <v>19</v>
@@ -6011,9 +6005,9 @@
       </c>
       <c r="Q109" s="16"/>
     </row>
-    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B110" s="16" t="s">
         <v>19</v>
@@ -6055,9 +6049,9 @@
       </c>
       <c r="Q110" s="16"/>
     </row>
-    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B111" s="20" t="s">
         <v>20</v>
@@ -6100,9 +6094,9 @@
       </c>
       <c r="Q111" s="20"/>
     </row>
-    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B112" s="20" t="s">
         <v>20</v>
@@ -6142,9 +6136,9 @@
       </c>
       <c r="Q112" s="20"/>
     </row>
-    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B113" s="20" t="s">
         <v>20</v>
@@ -6184,9 +6178,9 @@
       </c>
       <c r="Q113" s="20"/>
     </row>
-    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B114" s="20" t="s">
         <v>20</v>
@@ -6226,9 +6220,9 @@
       </c>
       <c r="Q114" s="20"/>
     </row>
-    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B115" s="20" t="s">
         <v>20</v>
@@ -6268,9 +6262,9 @@
       </c>
       <c r="Q115" s="23"/>
     </row>
-    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B116" s="20" t="s">
         <v>20</v>
@@ -6310,9 +6304,9 @@
       </c>
       <c r="Q116" s="20"/>
     </row>
-    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B117" s="20" t="s">
         <v>20</v>
@@ -6354,9 +6348,9 @@
       </c>
       <c r="Q117" s="20"/>
     </row>
-    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B118" s="24" t="s">
         <v>21</v>
@@ -6399,9 +6393,9 @@
       </c>
       <c r="Q118" s="24"/>
     </row>
-    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B119" s="24" t="s">
         <v>21</v>
@@ -6441,9 +6435,9 @@
       </c>
       <c r="Q119" s="24"/>
     </row>
-    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B120" s="24" t="s">
         <v>21</v>
@@ -6483,9 +6477,9 @@
       </c>
       <c r="Q120" s="24"/>
     </row>
-    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B121" s="24" t="s">
         <v>21</v>
@@ -6525,9 +6519,9 @@
       </c>
       <c r="Q121" s="24"/>
     </row>
-    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B122" s="24" t="s">
         <v>21</v>
@@ -6569,9 +6563,9 @@
       </c>
       <c r="Q122" s="24"/>
     </row>
-    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B123" s="28" t="s">
         <v>22</v>
@@ -6616,9 +6610,9 @@
       </c>
       <c r="Q123" s="28"/>
     </row>
-    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B124" s="28" t="s">
         <v>22</v>
@@ -6660,9 +6654,9 @@
       </c>
       <c r="Q124" s="28"/>
     </row>
-    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B125" s="28" t="s">
         <v>22</v>
@@ -6704,9 +6698,9 @@
       </c>
       <c r="Q125" s="28"/>
     </row>
-    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B126" s="28" t="s">
         <v>22</v>
@@ -6748,9 +6742,9 @@
       </c>
       <c r="Q126" s="28"/>
     </row>
-    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B127" s="28" t="s">
         <v>22</v>
@@ -6792,9 +6786,9 @@
       </c>
       <c r="Q127" s="28"/>
     </row>
-    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B128" s="28" t="s">
         <v>22</v>
@@ -6836,9 +6830,9 @@
       </c>
       <c r="Q128" s="28"/>
     </row>
-    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B129" s="28" t="s">
         <v>22</v>
@@ -6880,9 +6874,9 @@
       </c>
       <c r="Q129" s="28"/>
     </row>
-    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B130" s="28" t="s">
         <v>22</v>
@@ -6924,9 +6918,9 @@
       </c>
       <c r="Q130" s="28"/>
     </row>
-    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B131" s="28" t="s">
         <v>22</v>
@@ -6968,9 +6962,9 @@
       </c>
       <c r="Q131" s="28"/>
     </row>
-    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B132" s="28" t="s">
         <v>22</v>
@@ -7012,9 +7006,9 @@
       </c>
       <c r="Q132" s="28"/>
     </row>
-    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B133" s="28" t="s">
         <v>22</v>
@@ -7056,9 +7050,9 @@
       </c>
       <c r="Q133" s="28"/>
     </row>
-    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B134" s="28" t="s">
         <v>22</v>
@@ -7100,9 +7094,9 @@
       </c>
       <c r="Q134" s="28"/>
     </row>
-    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B135" s="28" t="s">
         <v>22</v>
@@ -7144,9 +7138,9 @@
       </c>
       <c r="Q135" s="28"/>
     </row>
-    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B136" s="28" t="s">
         <v>22</v>
@@ -7188,9 +7182,9 @@
       </c>
       <c r="Q136" s="28"/>
     </row>
-    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B137" s="28" t="s">
         <v>22</v>
@@ -7232,9 +7226,9 @@
       </c>
       <c r="Q137" s="28"/>
     </row>
-    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B138" s="28" t="s">
         <v>22</v>
@@ -7276,9 +7270,9 @@
       </c>
       <c r="Q138" s="28"/>
     </row>
-    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B139" s="28" t="s">
         <v>22</v>
@@ -7320,9 +7314,9 @@
       </c>
       <c r="Q139" s="28"/>
     </row>
-    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B140" s="28" t="s">
         <v>22</v>
@@ -7364,9 +7358,9 @@
       </c>
       <c r="Q140" s="28"/>
     </row>
-    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B141" s="28" t="s">
         <v>22</v>
@@ -7408,9 +7402,9 @@
       </c>
       <c r="Q141" s="28"/>
     </row>
-    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B142" s="28" t="s">
         <v>22</v>
@@ -7452,9 +7446,9 @@
       </c>
       <c r="Q142" s="28"/>
     </row>
-    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B143" s="28" t="s">
         <v>22</v>
@@ -7496,9 +7490,9 @@
       </c>
       <c r="Q143" s="28"/>
     </row>
-    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B144" s="28" t="s">
         <v>22</v>
@@ -7542,9 +7536,9 @@
       </c>
       <c r="Q144" s="28"/>
     </row>
-    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B145" s="32" t="s">
         <v>23</v>
@@ -7587,9 +7581,9 @@
       </c>
       <c r="Q145" s="32"/>
     </row>
-    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B146" s="32" t="s">
         <v>23</v>
@@ -7629,9 +7623,9 @@
       </c>
       <c r="Q146" s="32"/>
     </row>
-    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B147" s="32" t="s">
         <v>23</v>
@@ -7673,9 +7667,9 @@
       </c>
       <c r="Q147" s="32"/>
     </row>
-    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>24</v>
@@ -7718,9 +7712,9 @@
       </c>
       <c r="Q148" s="5"/>
     </row>
-    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>24</v>
@@ -7760,9 +7754,9 @@
       </c>
       <c r="Q149" s="5"/>
     </row>
-    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>24</v>
@@ -7804,9 +7798,9 @@
       </c>
       <c r="Q150" s="5"/>
     </row>
-    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B151" s="9" t="s">
         <v>25</v>
@@ -7851,9 +7845,9 @@
       </c>
       <c r="Q151" s="9"/>
     </row>
-    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B152" s="12" t="s">
         <v>26</v>
@@ -7898,9 +7892,9 @@
       </c>
       <c r="Q152" s="12"/>
     </row>
-    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B153" s="16" t="s">
         <v>27</v>
@@ -7945,9 +7939,9 @@
       </c>
       <c r="Q153" s="16"/>
     </row>
-    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B154" s="20" t="s">
         <v>0</v>
@@ -7989,9 +7983,9 @@
       </c>
       <c r="Q154" s="20"/>
     </row>
-    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B155" s="20" t="s">
         <v>0</v>
@@ -8031,9 +8025,9 @@
       </c>
       <c r="Q155" s="20"/>
     </row>
-    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B156" s="20" t="s">
         <v>0</v>
@@ -8075,9 +8069,9 @@
       </c>
       <c r="Q156" s="20"/>
     </row>
-    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B157" s="24" t="s">
         <v>1</v>
@@ -8119,9 +8113,9 @@
       </c>
       <c r="Q157" s="24"/>
     </row>
-    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B158" s="24" t="s">
         <v>1</v>
@@ -8161,9 +8155,9 @@
       </c>
       <c r="Q158" s="24"/>
     </row>
-    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B159" s="24" t="s">
         <v>1</v>
@@ -8205,9 +8199,9 @@
       </c>
       <c r="Q159" s="24"/>
     </row>
-    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B160" s="28" t="s">
         <v>2</v>
@@ -8249,9 +8243,9 @@
       </c>
       <c r="Q160" s="31"/>
     </row>
-    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B161" s="28" t="s">
         <v>2</v>
@@ -8291,9 +8285,9 @@
       </c>
       <c r="Q161" s="28"/>
     </row>
-    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B162" s="28" t="s">
         <v>2</v>
@@ -8337,9 +8331,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B163" s="32" t="s">
         <v>3</v>
@@ -8381,9 +8375,9 @@
       </c>
       <c r="Q163" s="32"/>
     </row>
-    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B164" s="32" t="s">
         <v>3</v>
@@ -8423,9 +8417,9 @@
       </c>
       <c r="Q164" s="32"/>
     </row>
-    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B165" s="32" t="s">
         <v>3</v>
@@ -8467,9 +8461,9 @@
       </c>
       <c r="Q165" s="32"/>
     </row>
-    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>4</v>
@@ -8511,9 +8505,9 @@
       </c>
       <c r="Q166" s="5"/>
     </row>
-    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>4</v>
@@ -8553,9 +8547,9 @@
       </c>
       <c r="Q167" s="5"/>
     </row>
-    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B168" s="5" t="s">
         <v>4</v>
@@ -8599,9 +8593,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B169" s="9" t="s">
         <v>5</v>
@@ -8643,9 +8637,9 @@
       </c>
       <c r="Q169" s="35"/>
     </row>
-    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B170" s="9" t="s">
         <v>5</v>
@@ -8685,9 +8679,9 @@
       </c>
       <c r="Q170" s="9"/>
     </row>
-    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A171" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B171" s="9" t="s">
         <v>5</v>
@@ -8727,9 +8721,9 @@
       </c>
       <c r="Q171" s="9"/>
     </row>
-    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B172" s="9" t="s">
         <v>5</v>
@@ -8769,9 +8763,9 @@
       </c>
       <c r="Q172" s="9"/>
     </row>
-    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B173" s="9" t="s">
         <v>5</v>
@@ -8813,9 +8807,9 @@
       </c>
       <c r="Q173" s="9"/>
     </row>
-    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B174" s="12" t="s">
         <v>6</v>
@@ -8857,9 +8851,9 @@
       </c>
       <c r="Q174" s="14"/>
     </row>
-    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B175" s="12" t="s">
         <v>6</v>
@@ -8899,9 +8893,9 @@
       </c>
       <c r="Q175" s="12"/>
     </row>
-    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B176" s="12" t="s">
         <v>6</v>
@@ -8943,9 +8937,9 @@
       </c>
       <c r="Q176" s="12"/>
     </row>
-    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A177" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B177" s="16" t="s">
         <v>7</v>
@@ -8989,9 +8983,9 @@
       </c>
       <c r="Q177" s="16"/>
     </row>
-    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B178" s="16" t="s">
         <v>7</v>
@@ -9033,9 +9027,9 @@
       </c>
       <c r="Q178" s="19"/>
     </row>
-    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B179" s="16" t="s">
         <v>7</v>
@@ -9077,9 +9071,9 @@
       </c>
       <c r="Q179" s="16"/>
     </row>
-    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B180" s="16" t="s">
         <v>7</v>
@@ -9123,9 +9117,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A181" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B181" s="16" t="s">
         <v>7</v>
@@ -9167,9 +9161,9 @@
       </c>
       <c r="Q181" s="16"/>
     </row>
-    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B182" s="16" t="s">
         <v>7</v>
@@ -9211,9 +9205,9 @@
       </c>
       <c r="Q182" s="16"/>
     </row>
-    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B183" s="16" t="s">
         <v>7</v>
@@ -9255,9 +9249,9 @@
       </c>
       <c r="Q183" s="16"/>
     </row>
-    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B184" s="16" t="s">
         <v>7</v>
@@ -9299,9 +9293,9 @@
       </c>
       <c r="Q184" s="16"/>
     </row>
-    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B185" s="16" t="s">
         <v>7</v>
@@ -9345,9 +9339,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A186" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B186" s="16" t="s">
         <v>7</v>
@@ -9389,9 +9383,9 @@
       </c>
       <c r="Q186" s="16"/>
     </row>
-    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B187" s="16" t="s">
         <v>7</v>
@@ -9433,9 +9427,9 @@
       </c>
       <c r="Q187" s="16"/>
     </row>
-    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B188" s="16" t="s">
         <v>7</v>
@@ -9477,9 +9471,9 @@
       </c>
       <c r="Q188" s="19"/>
     </row>
-    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B189" s="16" t="s">
         <v>7</v>
@@ -9521,9 +9515,9 @@
       </c>
       <c r="Q189" s="16"/>
     </row>
-    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B190" s="16" t="s">
         <v>7</v>
@@ -9565,9 +9559,9 @@
       </c>
       <c r="Q190" s="16"/>
     </row>
-    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B191" s="16" t="s">
         <v>7</v>
@@ -9611,9 +9605,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B192" s="16" t="s">
         <v>7</v>
@@ -9655,9 +9649,9 @@
       </c>
       <c r="Q192" s="16"/>
     </row>
-    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B193" s="16" t="s">
         <v>7</v>
@@ -9699,9 +9693,9 @@
       </c>
       <c r="Q193" s="16"/>
     </row>
-    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B194" s="16" t="s">
         <v>7</v>
@@ -9743,9 +9737,9 @@
       </c>
       <c r="Q194" s="16"/>
     </row>
-    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A195" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B195" s="16" t="s">
         <v>7</v>
@@ -9787,9 +9781,9 @@
       </c>
       <c r="Q195" s="16"/>
     </row>
-    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B196" s="16" t="s">
         <v>7</v>
@@ -9833,9 +9827,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B197" s="16" t="s">
         <v>7</v>
@@ -9877,9 +9871,9 @@
       </c>
       <c r="Q197" s="16"/>
     </row>
-    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B198" s="16" t="s">
         <v>7</v>
@@ -9923,9 +9917,9 @@
       </c>
       <c r="Q198" s="19"/>
     </row>
-    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A199" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B199" s="20" t="s">
         <v>8</v>
@@ -9969,9 +9963,9 @@
       </c>
       <c r="Q199" s="20"/>
     </row>
-    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A200" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B200" s="20" t="s">
         <v>8</v>
@@ -10013,9 +10007,9 @@
       </c>
       <c r="Q200" s="23"/>
     </row>
-    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A201" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B201" s="20" t="s">
         <v>8</v>
@@ -10057,9 +10051,9 @@
       </c>
       <c r="Q201" s="23"/>
     </row>
-    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B202" s="24" t="s">
         <v>9</v>
@@ -10101,9 +10095,9 @@
       </c>
       <c r="Q202" s="24"/>
     </row>
-    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A203" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B203" s="24" t="s">
         <v>9</v>
@@ -10143,9 +10137,9 @@
       </c>
       <c r="Q203" s="24"/>
     </row>
-    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A204" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B204" s="24" t="s">
         <v>9</v>
@@ -10185,9 +10179,9 @@
       </c>
       <c r="Q204" s="24"/>
     </row>
-    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B205" s="24" t="s">
         <v>9</v>
@@ -10229,9 +10223,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A206" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B206" s="24" t="s">
         <v>9</v>
@@ -10271,9 +10265,9 @@
       </c>
       <c r="Q206" s="24"/>
     </row>
-    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B207" s="24" t="s">
         <v>9</v>
@@ -10315,9 +10309,9 @@
       </c>
       <c r="Q207" s="24"/>
     </row>
-    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B208" s="28" t="s">
         <v>10</v>
@@ -10359,9 +10353,9 @@
       </c>
       <c r="Q208" s="28"/>
     </row>
-    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B209" s="28" t="s">
         <v>10</v>
@@ -10401,9 +10395,9 @@
       </c>
       <c r="Q209" s="28"/>
     </row>
-    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B210" s="28" t="s">
         <v>10</v>
@@ -10445,9 +10439,9 @@
       </c>
       <c r="Q210" s="28"/>
     </row>
-    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B211" s="32" t="s">
         <v>11</v>
@@ -10489,9 +10483,9 @@
       </c>
       <c r="Q211" s="32"/>
     </row>
-    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B212" s="32" t="s">
         <v>11</v>
@@ -10531,9 +10525,9 @@
       </c>
       <c r="Q212" s="32"/>
     </row>
-    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B213" s="32" t="s">
         <v>11</v>
@@ -10575,9 +10569,9 @@
       </c>
       <c r="Q213" s="36"/>
     </row>
-    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B214" s="5" t="s">
         <v>12</v>
@@ -10619,9 +10613,9 @@
       </c>
       <c r="Q214" s="5"/>
     </row>
-    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B215" s="5" t="s">
         <v>12</v>
@@ -10661,9 +10655,9 @@
       </c>
       <c r="Q215" s="5"/>
     </row>
-    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B216" s="5" t="s">
         <v>12</v>
@@ -10705,9 +10699,9 @@
       </c>
       <c r="Q216" s="5"/>
     </row>
-    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B217" s="9" t="s">
         <v>13</v>
@@ -10749,9 +10743,9 @@
       </c>
       <c r="Q217" s="9"/>
     </row>
-    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B218" s="9" t="s">
         <v>13</v>
@@ -10791,9 +10785,9 @@
       </c>
       <c r="Q218" s="9"/>
     </row>
-    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B219" s="9" t="s">
         <v>13</v>
@@ -10835,9 +10829,9 @@
       </c>
       <c r="Q219" s="9"/>
     </row>
-    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A220" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B220" s="12" t="s">
         <v>14</v>
@@ -10881,9 +10875,9 @@
       </c>
       <c r="Q220" s="12"/>
     </row>
-    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A221" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B221" s="16" t="s">
         <v>15</v>
@@ -10927,9 +10921,9 @@
       </c>
       <c r="Q221" s="16"/>
     </row>
-    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A222" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B222" s="16" t="s">
         <v>15</v>
@@ -10971,9 +10965,9 @@
       </c>
       <c r="Q222" s="16"/>
     </row>
-    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B223" s="16" t="s">
         <v>15</v>
@@ -11017,9 +11011,9 @@
       </c>
       <c r="Q223" s="16"/>
     </row>
-    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A224" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B224" s="20" t="s">
         <v>16</v>
@@ -11063,9 +11057,9 @@
       </c>
       <c r="Q224" s="20"/>
     </row>
-    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B225" s="24" t="s">
         <v>17</v>
@@ -11109,9 +11103,9 @@
       </c>
       <c r="Q225" s="24"/>
     </row>
-    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A226" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B226" s="28" t="s">
         <v>18</v>
@@ -11155,9 +11149,9 @@
       </c>
       <c r="Q226" s="28"/>
     </row>
-    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A227" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B227" s="28" t="s">
         <v>18</v>
@@ -11199,9 +11193,9 @@
       </c>
       <c r="Q227" s="28"/>
     </row>
-    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B228" s="28" t="s">
         <v>18</v>
@@ -11245,9 +11239,9 @@
       </c>
       <c r="Q228" s="28"/>
     </row>
-    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A229" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B229" s="32" t="s">
         <v>19</v>
@@ -11291,9 +11285,9 @@
       </c>
       <c r="Q229" s="32"/>
     </row>
-    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B230" s="5" t="s">
         <v>20</v>
@@ -11343,26 +11337,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>68</v>
       </c>
@@ -11376,22 +11370,16 @@
         <v>66</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>67</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="46" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11399,7 +11387,7 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2">
         <v>96</v>
@@ -11407,11 +11395,8 @@
       <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11419,7 +11404,7 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3">
         <v>39</v>
@@ -11433,11 +11418,8 @@
       <c r="G3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11445,7 +11427,7 @@
         <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4">
         <v>73</v>
@@ -11459,11 +11441,8 @@
       <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11471,7 +11450,7 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5">
         <v>9</v>
@@ -11479,11 +11458,8 @@
       <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11491,7 +11467,7 @@
         <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>45</v>
@@ -11499,14 +11475,8 @@
       <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11514,7 +11484,7 @@
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7">
         <v>65</v>
@@ -11528,11 +11498,8 @@
       <c r="G7" t="s">
         <v>20</v>
       </c>
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11540,7 +11507,7 @@
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8">
         <v>16</v>
@@ -11548,14 +11515,8 @@
       <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="H8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11563,7 +11524,7 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9">
         <v>48</v>
@@ -11577,11 +11538,8 @@
       <c r="G9" t="s">
         <v>22</v>
       </c>
-      <c r="H9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11589,7 +11547,7 @@
         <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D10">
         <v>77</v>
@@ -11597,14 +11555,8 @@
       <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="H10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11612,7 +11564,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D11">
         <v>57</v>
@@ -11626,11 +11578,8 @@
       <c r="G11" t="s">
         <v>22</v>
       </c>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11638,7 +11587,7 @@
         <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D12">
         <v>25</v>
@@ -11646,14 +11595,8 @@
       <c r="E12" t="s">
         <v>7</v>
       </c>
-      <c r="H12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11661,7 +11604,7 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -11669,11 +11612,8 @@
       <c r="E13" t="s">
         <v>0</v>
       </c>
-      <c r="I13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11681,7 +11621,7 @@
         <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D14">
         <v>16</v>
@@ -11689,14 +11629,8 @@
       <c r="E14" t="s">
         <v>3</v>
       </c>
-      <c r="H14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11704,7 +11638,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15">
         <v>88</v>
@@ -11712,11 +11646,8 @@
       <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="H15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11724,7 +11655,7 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D16">
         <v>7</v>
@@ -11732,14 +11663,8 @@
       <c r="E16" t="s">
         <v>2</v>
       </c>
-      <c r="H16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11747,7 +11672,7 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D17">
         <v>31</v>
@@ -11755,11 +11680,8 @@
       <c r="E17" t="s">
         <v>6</v>
       </c>
-      <c r="I17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11767,7 +11689,7 @@
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D18">
         <v>60</v>
@@ -11775,14 +11697,8 @@
       <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="H18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -11790,7 +11706,7 @@
         <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D19">
         <v>48</v>
@@ -11798,14 +11714,8 @@
       <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="H19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -11813,7 +11723,7 @@
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D20">
         <v>35</v>
@@ -11821,14 +11731,8 @@
       <c r="E20" t="s">
         <v>7</v>
       </c>
-      <c r="H20" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -11836,7 +11740,7 @@
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D21">
         <v>21</v>
@@ -11844,14 +11748,8 @@
       <c r="E21" t="s">
         <v>6</v>
       </c>
-      <c r="H21" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -11859,19 +11757,13 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D22">
         <v>22</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
-      </c>
-      <c r="H22" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -11887,14 +11779,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>55</v>
       </c>
@@ -11908,15 +11800,15 @@
         <v>54</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>62</v>
@@ -11928,12 +11820,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>13</v>
@@ -11945,12 +11837,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4">
         <v>28</v>
@@ -11962,12 +11854,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>57</v>
@@ -11979,12 +11871,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6">
         <v>77</v>
@@ -11996,12 +11888,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7">
         <v>85</v>
@@ -12013,12 +11905,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -12030,12 +11922,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9">
         <v>27</v>
@@ -12047,12 +11939,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10">
         <v>33</v>
@@ -12064,12 +11956,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11">
         <v>38</v>
@@ -12081,12 +11973,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12">
         <v>44</v>
@@ -12098,12 +11990,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13">
         <v>52</v>
@@ -12115,12 +12007,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14">
         <v>9</v>

</xml_diff>

<commit_message>
Added support for Beacons.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1296" yWindow="6840" windowWidth="33240" windowHeight="11556" activeTab="3"/>
+    <workbookView xWindow="1296" yWindow="6840" windowWidth="33240" windowHeight="11556" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="75">
   <si>
     <t>A</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>sectionB</t>
+  </si>
+  <si>
+    <t>beaconMessage</t>
   </si>
 </sst>
 </file>
@@ -1235,11 +1238,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q230"/>
+  <dimension ref="A1:R230"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H89" sqref="H89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1261,10 +1264,11 @@
     <col min="15" max="15" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.77734375" style="1"/>
+    <col min="18" max="18" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -1316,8 +1320,11 @@
       <c r="Q1" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R1" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>69</v>
       </c>
@@ -1361,7 +1368,7 @@
       </c>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>69</v>
       </c>
@@ -1403,7 +1410,7 @@
       </c>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>69</v>
       </c>
@@ -1448,7 +1455,7 @@
       </c>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>69</v>
       </c>
@@ -1492,7 +1499,7 @@
       </c>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>69</v>
       </c>
@@ -1534,7 +1541,7 @@
       </c>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>69</v>
       </c>
@@ -1579,7 +1586,7 @@
       </c>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>69</v>
       </c>
@@ -1623,7 +1630,7 @@
       </c>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>69</v>
       </c>
@@ -1665,7 +1672,7 @@
       </c>
       <c r="Q9" s="12"/>
     </row>
-    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -1707,7 +1714,7 @@
       </c>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>69</v>
       </c>
@@ -1749,7 +1756,7 @@
       </c>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>69</v>
       </c>
@@ -1791,7 +1798,7 @@
       </c>
       <c r="Q12" s="12"/>
     </row>
-    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>69</v>
       </c>
@@ -1838,7 +1845,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>69</v>
       </c>
@@ -1882,7 +1889,7 @@
       </c>
       <c r="Q14" s="16"/>
     </row>
-    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>69</v>
       </c>
@@ -1924,7 +1931,7 @@
       </c>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>69</v>
       </c>
@@ -11339,7 +11346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>

</xml_diff>

<commit_message>
Added full beacon data to TrackData file
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1296" yWindow="6840" windowWidth="33240" windowHeight="11556" activeTab="2"/>
+    <workbookView xWindow="1296" yWindow="6840" windowWidth="33240" windowHeight="11556" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -17,8 +17,9 @@
     <sheet name="BLOCK" sheetId="2" r:id="rId3"/>
     <sheet name="STATION" sheetId="8" r:id="rId4"/>
     <sheet name="SWITCH" sheetId="7" r:id="rId5"/>
+    <sheet name="BEACON" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="78">
   <si>
     <t>A</t>
   </si>
@@ -255,7 +256,16 @@
     <t>sectionB</t>
   </si>
   <si>
-    <t>beaconMessage</t>
+    <t>beaconID</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>isRightSide</t>
   </si>
 </sst>
 </file>
@@ -368,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -488,6 +498,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1238,11 +1257,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R230"/>
+  <dimension ref="A1:Q230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R55" sqref="R55"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1268,7 +1287,7 @@
     <col min="19" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -1320,11 +1339,8 @@
       <c r="Q1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>69</v>
       </c>
@@ -1368,7 +1384,7 @@
       </c>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>69</v>
       </c>
@@ -1410,7 +1426,7 @@
       </c>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>69</v>
       </c>
@@ -1455,7 +1471,7 @@
       </c>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>69</v>
       </c>
@@ -1499,7 +1515,7 @@
       </c>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>69</v>
       </c>
@@ -1541,7 +1557,7 @@
       </c>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>69</v>
       </c>
@@ -1586,7 +1602,7 @@
       </c>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>69</v>
       </c>
@@ -1630,7 +1646,7 @@
       </c>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>69</v>
       </c>
@@ -1672,7 +1688,7 @@
       </c>
       <c r="Q9" s="12"/>
     </row>
-    <row r="10" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -1714,7 +1730,7 @@
       </c>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>69</v>
       </c>
@@ -1756,7 +1772,7 @@
       </c>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>69</v>
       </c>
@@ -1798,7 +1814,7 @@
       </c>
       <c r="Q12" s="12"/>
     </row>
-    <row r="13" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>69</v>
       </c>
@@ -1845,7 +1861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>69</v>
       </c>
@@ -1889,7 +1905,7 @@
       </c>
       <c r="Q14" s="16"/>
     </row>
-    <row r="15" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>69</v>
       </c>
@@ -1931,7 +1947,7 @@
       </c>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>69</v>
       </c>
@@ -11348,7 +11364,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11788,7 +11804,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12035,4 +12051,887 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.88671875" style="47"/>
+    <col min="6" max="6" width="10.109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="47"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48">
+        <v>1</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="48">
+        <v>76</v>
+      </c>
+      <c r="D2" s="48">
+        <v>0</v>
+      </c>
+      <c r="E2" s="48">
+        <v>-1</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="48">
+        <v>2</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="48">
+        <v>72</v>
+      </c>
+      <c r="D3" s="48">
+        <v>0</v>
+      </c>
+      <c r="E3" s="48">
+        <v>-1</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="48">
+        <v>3</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="48">
+        <v>71</v>
+      </c>
+      <c r="D4" s="48">
+        <v>0</v>
+      </c>
+      <c r="E4" s="48">
+        <v>-1</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="48">
+        <v>4</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="48">
+        <v>67</v>
+      </c>
+      <c r="D5" s="48">
+        <v>0</v>
+      </c>
+      <c r="E5" s="48">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="49">
+        <v>6</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="49">
+        <v>93</v>
+      </c>
+      <c r="D6" s="49">
+        <v>1</v>
+      </c>
+      <c r="E6" s="49">
+        <v>225</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="49">
+        <v>7</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="49">
+        <v>35</v>
+      </c>
+      <c r="D7" s="49">
+        <v>2</v>
+      </c>
+      <c r="E7" s="49">
+        <v>200</v>
+      </c>
+      <c r="F7" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="49">
+        <v>8</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="49">
+        <v>137</v>
+      </c>
+      <c r="D8" s="49">
+        <v>2</v>
+      </c>
+      <c r="E8" s="49">
+        <v>200</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="49">
+        <v>9</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="49">
+        <v>69</v>
+      </c>
+      <c r="D9" s="49">
+        <v>3</v>
+      </c>
+      <c r="E9" s="49">
+        <v>240</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="49">
+        <v>10</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="49">
+        <v>103</v>
+      </c>
+      <c r="D10" s="49">
+        <v>3</v>
+      </c>
+      <c r="E10" s="49">
+        <v>180</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="49">
+        <v>11</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="49">
+        <v>7</v>
+      </c>
+      <c r="D11" s="49">
+        <v>4</v>
+      </c>
+      <c r="E11" s="49">
+        <v>200</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="49">
+        <v>12</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="49">
+        <v>41</v>
+      </c>
+      <c r="D12" s="49">
+        <v>5</v>
+      </c>
+      <c r="E12" s="49">
+        <v>210</v>
+      </c>
+      <c r="F12" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49">
+        <v>13</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="49">
+        <v>48</v>
+      </c>
+      <c r="D13" s="49">
+        <v>5</v>
+      </c>
+      <c r="E13" s="49">
+        <v>225</v>
+      </c>
+      <c r="F13" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="49">
+        <v>14</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="49">
+        <v>63</v>
+      </c>
+      <c r="D14" s="49">
+        <v>6</v>
+      </c>
+      <c r="E14" s="49">
+        <v>200</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="49">
+        <v>15</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="49">
+        <v>112</v>
+      </c>
+      <c r="D15" s="49">
+        <v>6</v>
+      </c>
+      <c r="E15" s="49">
+        <v>200</v>
+      </c>
+      <c r="F15" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="49">
+        <v>16</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="49">
+        <v>13</v>
+      </c>
+      <c r="D16" s="49">
+        <v>7</v>
+      </c>
+      <c r="E16" s="49">
+        <v>188.4</v>
+      </c>
+      <c r="F16" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="49">
+        <v>17</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="49">
+        <v>17</v>
+      </c>
+      <c r="D17" s="49">
+        <v>7</v>
+      </c>
+      <c r="E17" s="49">
+        <v>200</v>
+      </c>
+      <c r="F17" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="49">
+        <v>18</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="49">
+        <v>4</v>
+      </c>
+      <c r="D18" s="49">
+        <v>7</v>
+      </c>
+      <c r="E18" s="49">
+        <v>200</v>
+      </c>
+      <c r="F18" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="49">
+        <v>19</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="49">
+        <v>44</v>
+      </c>
+      <c r="D19" s="49">
+        <v>8</v>
+      </c>
+      <c r="E19" s="49">
+        <v>200</v>
+      </c>
+      <c r="F19" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="49">
+        <v>20</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="49">
+        <v>128</v>
+      </c>
+      <c r="D20" s="49">
+        <v>8</v>
+      </c>
+      <c r="E20" s="49">
+        <v>200</v>
+      </c>
+      <c r="F20" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="49">
+        <v>21</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="49">
+        <v>74</v>
+      </c>
+      <c r="D21" s="49">
+        <v>9</v>
+      </c>
+      <c r="E21" s="49">
+        <v>200</v>
+      </c>
+      <c r="F21" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="49">
+        <v>22</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="49">
+        <v>77</v>
+      </c>
+      <c r="D22" s="49">
+        <v>9</v>
+      </c>
+      <c r="E22" s="49">
+        <v>300</v>
+      </c>
+      <c r="F22" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="49">
+        <v>23</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="49">
+        <v>53</v>
+      </c>
+      <c r="D23" s="49">
+        <v>10</v>
+      </c>
+      <c r="E23" s="49">
+        <v>200</v>
+      </c>
+      <c r="F23" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="49">
+        <v>24</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="49">
+        <v>119</v>
+      </c>
+      <c r="D24" s="49">
+        <v>10</v>
+      </c>
+      <c r="E24" s="49">
+        <v>190</v>
+      </c>
+      <c r="F24" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="49">
+        <v>25</v>
+      </c>
+      <c r="B25" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="49">
+        <v>22</v>
+      </c>
+      <c r="D25" s="49">
+        <v>11</v>
+      </c>
+      <c r="E25" s="49">
+        <v>250</v>
+      </c>
+      <c r="F25" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="49">
+        <v>26</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="49">
+        <v>29</v>
+      </c>
+      <c r="D26" s="49">
+        <v>11</v>
+      </c>
+      <c r="E26" s="49">
+        <v>210</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="49">
+        <v>27</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="49">
+        <v>4</v>
+      </c>
+      <c r="D27" s="49">
+        <v>12</v>
+      </c>
+      <c r="E27" s="49">
+        <v>200</v>
+      </c>
+      <c r="F27" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="49">
+        <v>28</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="49">
+        <v>14</v>
+      </c>
+      <c r="D28" s="49">
+        <v>13</v>
+      </c>
+      <c r="E28" s="49">
+        <v>300</v>
+      </c>
+      <c r="F28" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="49">
+        <v>29</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="49">
+        <v>18</v>
+      </c>
+      <c r="D29" s="49">
+        <v>13</v>
+      </c>
+      <c r="E29" s="49">
+        <v>300</v>
+      </c>
+      <c r="F29" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="49">
+        <v>30</v>
+      </c>
+      <c r="B30" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="49">
+        <v>86</v>
+      </c>
+      <c r="D30" s="49">
+        <v>14</v>
+      </c>
+      <c r="E30" s="49">
+        <v>186.6</v>
+      </c>
+      <c r="F30" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="49">
+        <v>31</v>
+      </c>
+      <c r="B31" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="49">
+        <v>3</v>
+      </c>
+      <c r="D31" s="49">
+        <v>15</v>
+      </c>
+      <c r="E31" s="49">
+        <v>200</v>
+      </c>
+      <c r="F31" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="49">
+        <v>32</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="49">
+        <v>10</v>
+      </c>
+      <c r="D32" s="49">
+        <v>15</v>
+      </c>
+      <c r="E32" s="49">
+        <v>225</v>
+      </c>
+      <c r="F32" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="49">
+        <v>33</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="49">
+        <v>27</v>
+      </c>
+      <c r="D33" s="49">
+        <v>16</v>
+      </c>
+      <c r="E33" s="49">
+        <v>200</v>
+      </c>
+      <c r="F33" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="49">
+        <v>34</v>
+      </c>
+      <c r="B34" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="49">
+        <v>57</v>
+      </c>
+      <c r="D34" s="49">
+        <v>17</v>
+      </c>
+      <c r="E34" s="49">
+        <v>225</v>
+      </c>
+      <c r="F34" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="49">
+        <v>35</v>
+      </c>
+      <c r="B35" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="49">
+        <v>63</v>
+      </c>
+      <c r="D35" s="49">
+        <v>17</v>
+      </c>
+      <c r="E35" s="49">
+        <v>225</v>
+      </c>
+      <c r="F35" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="49">
+        <v>36</v>
+      </c>
+      <c r="B36" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="49">
+        <v>45</v>
+      </c>
+      <c r="D36" s="49">
+        <v>18</v>
+      </c>
+      <c r="E36" s="49">
+        <v>200</v>
+      </c>
+      <c r="F36" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="49">
+        <v>37</v>
+      </c>
+      <c r="B37" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="49">
+        <v>52</v>
+      </c>
+      <c r="D37" s="49">
+        <v>18</v>
+      </c>
+      <c r="E37" s="49">
+        <v>192.2</v>
+      </c>
+      <c r="F37" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="49">
+        <v>38</v>
+      </c>
+      <c r="B38" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="49">
+        <v>31</v>
+      </c>
+      <c r="D38" s="49">
+        <v>19</v>
+      </c>
+      <c r="E38" s="49">
+        <v>200</v>
+      </c>
+      <c r="F38" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="49">
+        <v>39</v>
+      </c>
+      <c r="B39" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="49">
+        <v>38</v>
+      </c>
+      <c r="D39" s="49">
+        <v>19</v>
+      </c>
+      <c r="E39" s="49">
+        <v>200</v>
+      </c>
+      <c r="F39" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="49">
+        <v>40</v>
+      </c>
+      <c r="B40" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="49">
+        <v>20</v>
+      </c>
+      <c r="D40" s="49">
+        <v>20</v>
+      </c>
+      <c r="E40" s="49">
+        <v>200</v>
+      </c>
+      <c r="F40" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="49">
+        <v>41</v>
+      </c>
+      <c r="B41" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="49">
+        <v>23</v>
+      </c>
+      <c r="D41" s="49">
+        <v>20</v>
+      </c>
+      <c r="E41" s="49">
+        <v>200</v>
+      </c>
+      <c r="F41" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="49">
+        <v>42</v>
+      </c>
+      <c r="B42" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="49">
+        <v>21</v>
+      </c>
+      <c r="D42" s="49">
+        <v>21</v>
+      </c>
+      <c r="E42" s="49">
+        <v>300</v>
+      </c>
+      <c r="F42" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="49">
+        <v>43</v>
+      </c>
+      <c r="B43" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="49">
+        <v>23</v>
+      </c>
+      <c r="D43" s="49">
+        <v>21</v>
+      </c>
+      <c r="E43" s="49">
+        <v>300</v>
+      </c>
+      <c r="F43" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected Beacon 9 in TrackData file.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -1260,8 +1260,8 @@
   <dimension ref="A1:Q230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I120" sqref="I120"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11364,7 +11364,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12059,7 +12059,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12239,13 +12239,13 @@
         <v>69</v>
       </c>
       <c r="C9" s="49">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D9" s="49">
         <v>3</v>
       </c>
       <c r="E9" s="49">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="F9" s="49" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Small corrections to TrackData file and stopping distance calculation.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -1260,8 +1260,8 @@
   <dimension ref="A1:Q230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12058,8 +12058,8 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12479,7 +12479,7 @@
         <v>69</v>
       </c>
       <c r="C21" s="49">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="49">
         <v>9</v>
@@ -12499,7 +12499,7 @@
         <v>69</v>
       </c>
       <c r="C22" s="49">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D22" s="49">
         <v>9</v>

</xml_diff>

<commit_message>
Small corrections to TrackData file.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -1260,8 +1260,8 @@
   <dimension ref="A1:Q230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I79" sqref="I79"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12058,8 +12058,8 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12279,7 +12279,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="49">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D11" s="49">
         <v>4</v>

</xml_diff>

<commit_message>
Functional Red line without stopping at stations Includes map for red line with sections and block logic, switch logic, trivial light logic (needs to be improved) Does not include station icons, and needs work with dispatching trains (in GPS.java there is an enterTrack call hardcoded for GREEN line that needs to be taken care of. Improved logic around switch 0 and going back around the track by increasing spacing. Trackview may not represent this completely correctly and will need further investigation
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan94\Documents\Coding\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylemonto/Documents/Pitt/Senior/COE 1186/ECE1186/TrainSystem/src/com/rogueone/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1296" yWindow="6840" windowWidth="33240" windowHeight="11556" activeTab="5"/>
+    <workbookView xWindow="1300" yWindow="6840" windowWidth="33240" windowHeight="11560" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="SWITCH" sheetId="7" r:id="rId5"/>
     <sheet name="BEACON" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -817,19 +817,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -848,9 +848,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
@@ -858,7 +858,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -874,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -882,7 +882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -890,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -898,7 +898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -906,7 +906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -914,7 +914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -922,7 +922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -930,7 +930,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -938,7 +938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -946,7 +946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -954,7 +954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -962,7 +962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -970,7 +970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -978,7 +978,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -986,7 +986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -994,7 +994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -1264,30 +1264,30 @@
       <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.77734375" style="1"/>
+    <col min="16" max="16" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>69</v>
       </c>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>69</v>
       </c>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>69</v>
       </c>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>69</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>69</v>
       </c>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>69</v>
       </c>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>69</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>69</v>
       </c>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="Q9" s="12"/>
     </row>
-    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>69</v>
       </c>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>69</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="Q12" s="12"/>
     </row>
-    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>69</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>69</v>
       </c>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="Q14" s="16"/>
     </row>
-    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>69</v>
       </c>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>69</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>69</v>
       </c>
@@ -2033,7 +2033,7 @@
       </c>
       <c r="Q17" s="19"/>
     </row>
-    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>69</v>
       </c>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="Q18" s="20"/>
     </row>
-    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>69</v>
       </c>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="Q19" s="20"/>
     </row>
-    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>69</v>
       </c>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="Q20" s="23"/>
     </row>
-    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>69</v>
       </c>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="Q21" s="20"/>
     </row>
-    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
         <v>69</v>
       </c>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="Q22" s="24"/>
     </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
         <v>69</v>
       </c>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="Q23" s="27"/>
     </row>
-    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
         <v>69</v>
       </c>
@@ -2335,7 +2335,7 @@
       </c>
       <c r="Q24" s="24"/>
     </row>
-    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
         <v>69</v>
       </c>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="Q25" s="24"/>
     </row>
-    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="24" t="s">
         <v>69</v>
       </c>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="Q26" s="24"/>
     </row>
-    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
         <v>69</v>
       </c>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="Q27" s="24"/>
     </row>
-    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
         <v>69</v>
       </c>
@@ -2503,7 +2503,7 @@
       </c>
       <c r="Q28" s="24"/>
     </row>
-    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="24" t="s">
         <v>69</v>
       </c>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="Q29" s="24"/>
     </row>
-    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="28" t="s">
         <v>69</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28" t="s">
         <v>69</v>
       </c>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="Q31" s="28"/>
     </row>
-    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
         <v>69</v>
       </c>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="Q32" s="31"/>
     </row>
-    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="28" t="s">
         <v>69</v>
       </c>
@@ -2722,7 +2722,7 @@
       </c>
       <c r="Q33" s="28"/>
     </row>
-    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>69</v>
       </c>
@@ -2767,7 +2767,7 @@
       </c>
       <c r="Q34" s="32"/>
     </row>
-    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>69</v>
       </c>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="Q35" s="32"/>
     </row>
-    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>69</v>
       </c>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="Q36" s="32"/>
     </row>
-    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>69</v>
       </c>
@@ -2900,7 +2900,7 @@
       </c>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>69</v>
       </c>
@@ -2944,7 +2944,7 @@
       </c>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>69</v>
       </c>
@@ -2988,7 +2988,7 @@
       </c>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>69</v>
       </c>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>69</v>
       </c>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>69</v>
       </c>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>69</v>
       </c>
@@ -3164,7 +3164,7 @@
       </c>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>69</v>
       </c>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>69</v>
       </c>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>69</v>
       </c>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>69</v>
       </c>
@@ -3340,7 +3340,7 @@
       </c>
       <c r="Q47" s="5"/>
     </row>
-    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>69</v>
       </c>
@@ -3384,7 +3384,7 @@
       </c>
       <c r="Q48" s="5"/>
     </row>
-    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>69</v>
       </c>
@@ -3428,7 +3428,7 @@
       </c>
       <c r="Q49" s="8"/>
     </row>
-    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>69</v>
       </c>
@@ -3472,7 +3472,7 @@
       </c>
       <c r="Q50" s="5"/>
     </row>
-    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>69</v>
       </c>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="Q51" s="5"/>
     </row>
-    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>69</v>
       </c>
@@ -3560,7 +3560,7 @@
       </c>
       <c r="Q52" s="5"/>
     </row>
-    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>69</v>
       </c>
@@ -3604,7 +3604,7 @@
       </c>
       <c r="Q53" s="5"/>
     </row>
-    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>69</v>
       </c>
@@ -3648,7 +3648,7 @@
       </c>
       <c r="Q54" s="5"/>
     </row>
-    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>69</v>
       </c>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="Q55" s="5"/>
     </row>
-    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>69</v>
       </c>
@@ -3736,7 +3736,7 @@
       </c>
       <c r="Q56" s="5"/>
     </row>
-    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>69</v>
       </c>
@@ -3780,7 +3780,7 @@
       </c>
       <c r="Q57" s="5"/>
     </row>
-    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>69</v>
       </c>
@@ -3826,7 +3826,7 @@
       </c>
       <c r="Q58" s="8"/>
     </row>
-    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
         <v>69</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>69</v>
       </c>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="Q60" s="9"/>
     </row>
-    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>69</v>
       </c>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="Q61" s="9"/>
     </row>
-    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
         <v>69</v>
       </c>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="Q62" s="9"/>
     </row>
-    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>69</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
         <v>69</v>
       </c>
@@ -4090,7 +4090,7 @@
       </c>
       <c r="Q64" s="12"/>
     </row>
-    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
         <v>69</v>
       </c>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="Q65" s="12"/>
     </row>
-    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
         <v>69</v>
       </c>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="Q66" s="14"/>
     </row>
-    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
         <v>69</v>
       </c>
@@ -4216,7 +4216,7 @@
       </c>
       <c r="Q67" s="12"/>
     </row>
-    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="s">
         <v>69</v>
       </c>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="Q68" s="12"/>
     </row>
-    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="12" t="s">
         <v>69</v>
       </c>
@@ -4302,7 +4302,7 @@
       </c>
       <c r="Q69" s="12"/>
     </row>
-    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="16" t="s">
         <v>69</v>
       </c>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="Q70" s="16"/>
     </row>
-    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="s">
         <v>69</v>
       </c>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="Q71" s="16"/>
     </row>
-    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="16" t="s">
         <v>69</v>
       </c>
@@ -4431,7 +4431,7 @@
       </c>
       <c r="Q72" s="16"/>
     </row>
-    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="16" t="s">
         <v>69</v>
       </c>
@@ -4473,7 +4473,7 @@
       </c>
       <c r="Q73" s="16"/>
     </row>
-    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="16" t="s">
         <v>69</v>
       </c>
@@ -4517,7 +4517,7 @@
       </c>
       <c r="Q74" s="19"/>
     </row>
-    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
         <v>69</v>
       </c>
@@ -4562,7 +4562,7 @@
       </c>
       <c r="Q75" s="20"/>
     </row>
-    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
         <v>69</v>
       </c>
@@ -4604,7 +4604,7 @@
       </c>
       <c r="Q76" s="20"/>
     </row>
-    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="20" t="s">
         <v>69</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="24" t="s">
         <v>69</v>
       </c>
@@ -4694,7 +4694,7 @@
       </c>
       <c r="Q78" s="27"/>
     </row>
-    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="24" t="s">
         <v>69</v>
       </c>
@@ -4736,7 +4736,7 @@
       </c>
       <c r="Q79" s="24"/>
     </row>
-    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="24" t="s">
         <v>69</v>
       </c>
@@ -4778,7 +4778,7 @@
       </c>
       <c r="Q80" s="24"/>
     </row>
-    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="24" t="s">
         <v>69</v>
       </c>
@@ -4820,7 +4820,7 @@
       </c>
       <c r="Q81" s="24"/>
     </row>
-    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="24" t="s">
         <v>69</v>
       </c>
@@ -4862,7 +4862,7 @@
       </c>
       <c r="Q82" s="24"/>
     </row>
-    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="24" t="s">
         <v>69</v>
       </c>
@@ -4904,7 +4904,7 @@
       </c>
       <c r="Q83" s="24"/>
     </row>
-    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="24" t="s">
         <v>69</v>
       </c>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="Q84" s="24"/>
     </row>
-    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="24" t="s">
         <v>69</v>
       </c>
@@ -4988,7 +4988,7 @@
       </c>
       <c r="Q85" s="24"/>
     </row>
-    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="24" t="s">
         <v>69</v>
       </c>
@@ -5032,7 +5032,7 @@
       </c>
       <c r="Q86" s="24"/>
     </row>
-    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="28" t="s">
         <v>69</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="28" t="s">
         <v>69</v>
       </c>
@@ -5121,7 +5121,7 @@
       </c>
       <c r="Q88" s="28"/>
     </row>
-    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="28" t="s">
         <v>69</v>
       </c>
@@ -5165,7 +5165,7 @@
       </c>
       <c r="Q89" s="31"/>
     </row>
-    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="32" t="s">
         <v>69</v>
       </c>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="Q90" s="32"/>
     </row>
-    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="32" t="s">
         <v>69</v>
       </c>
@@ -5252,7 +5252,7 @@
       </c>
       <c r="Q91" s="32"/>
     </row>
-    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="32" t="s">
         <v>69</v>
       </c>
@@ -5294,7 +5294,7 @@
       </c>
       <c r="Q92" s="32"/>
     </row>
-    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="32" t="s">
         <v>69</v>
       </c>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="Q93" s="32"/>
     </row>
-    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="32" t="s">
         <v>69</v>
       </c>
@@ -5378,7 +5378,7 @@
       </c>
       <c r="Q94" s="32"/>
     </row>
-    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="32" t="s">
         <v>69</v>
       </c>
@@ -5420,7 +5420,7 @@
       </c>
       <c r="Q95" s="32"/>
     </row>
-    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="32" t="s">
         <v>69</v>
       </c>
@@ -5462,7 +5462,7 @@
       </c>
       <c r="Q96" s="32"/>
     </row>
-    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="32" t="s">
         <v>69</v>
       </c>
@@ -5504,7 +5504,7 @@
       </c>
       <c r="Q97" s="36"/>
     </row>
-    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="32" t="s">
         <v>69</v>
       </c>
@@ -5548,7 +5548,7 @@
       </c>
       <c r="Q98" s="32"/>
     </row>
-    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>69</v>
       </c>
@@ -5593,7 +5593,7 @@
       </c>
       <c r="Q99" s="5"/>
     </row>
-    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>69</v>
       </c>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="Q100" s="5"/>
     </row>
-    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>69</v>
       </c>
@@ -5679,7 +5679,7 @@
       </c>
       <c r="Q101" s="5"/>
     </row>
-    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
         <v>69</v>
       </c>
@@ -5726,7 +5726,7 @@
       </c>
       <c r="Q102" s="9"/>
     </row>
-    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="12" t="s">
         <v>69</v>
       </c>
@@ -5771,7 +5771,7 @@
       </c>
       <c r="Q103" s="12"/>
     </row>
-    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="12" t="s">
         <v>69</v>
       </c>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="Q104" s="12"/>
     </row>
-    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="12" t="s">
         <v>69</v>
       </c>
@@ -5857,7 +5857,7 @@
       </c>
       <c r="Q105" s="12"/>
     </row>
-    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="16" t="s">
         <v>69</v>
       </c>
@@ -5902,7 +5902,7 @@
       </c>
       <c r="Q106" s="19"/>
     </row>
-    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="16" t="s">
         <v>69</v>
       </c>
@@ -5944,7 +5944,7 @@
       </c>
       <c r="Q107" s="16"/>
     </row>
-    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="16" t="s">
         <v>69</v>
       </c>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="Q108" s="16"/>
     </row>
-    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="16" t="s">
         <v>69</v>
       </c>
@@ -6028,7 +6028,7 @@
       </c>
       <c r="Q109" s="16"/>
     </row>
-    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="16" t="s">
         <v>69</v>
       </c>
@@ -6072,7 +6072,7 @@
       </c>
       <c r="Q110" s="16"/>
     </row>
-    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="20" t="s">
         <v>69</v>
       </c>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="Q111" s="20"/>
     </row>
-    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="20" t="s">
         <v>69</v>
       </c>
@@ -6159,7 +6159,7 @@
       </c>
       <c r="Q112" s="20"/>
     </row>
-    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="20" t="s">
         <v>69</v>
       </c>
@@ -6201,7 +6201,7 @@
       </c>
       <c r="Q113" s="20"/>
     </row>
-    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="20" t="s">
         <v>69</v>
       </c>
@@ -6243,7 +6243,7 @@
       </c>
       <c r="Q114" s="20"/>
     </row>
-    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="20" t="s">
         <v>69</v>
       </c>
@@ -6285,7 +6285,7 @@
       </c>
       <c r="Q115" s="23"/>
     </row>
-    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="20" t="s">
         <v>69</v>
       </c>
@@ -6327,7 +6327,7 @@
       </c>
       <c r="Q116" s="20"/>
     </row>
-    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="20" t="s">
         <v>69</v>
       </c>
@@ -6371,7 +6371,7 @@
       </c>
       <c r="Q117" s="20"/>
     </row>
-    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="24" t="s">
         <v>69</v>
       </c>
@@ -6416,7 +6416,7 @@
       </c>
       <c r="Q118" s="24"/>
     </row>
-    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="24" t="s">
         <v>69</v>
       </c>
@@ -6458,7 +6458,7 @@
       </c>
       <c r="Q119" s="24"/>
     </row>
-    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="24" t="s">
         <v>69</v>
       </c>
@@ -6500,7 +6500,7 @@
       </c>
       <c r="Q120" s="24"/>
     </row>
-    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="24" t="s">
         <v>69</v>
       </c>
@@ -6542,7 +6542,7 @@
       </c>
       <c r="Q121" s="24"/>
     </row>
-    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="24" t="s">
         <v>69</v>
       </c>
@@ -6586,7 +6586,7 @@
       </c>
       <c r="Q122" s="24"/>
     </row>
-    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="28" t="s">
         <v>69</v>
       </c>
@@ -6633,7 +6633,7 @@
       </c>
       <c r="Q123" s="28"/>
     </row>
-    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="28" t="s">
         <v>69</v>
       </c>
@@ -6677,7 +6677,7 @@
       </c>
       <c r="Q124" s="28"/>
     </row>
-    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="28" t="s">
         <v>69</v>
       </c>
@@ -6721,7 +6721,7 @@
       </c>
       <c r="Q125" s="28"/>
     </row>
-    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="28" t="s">
         <v>69</v>
       </c>
@@ -6765,7 +6765,7 @@
       </c>
       <c r="Q126" s="28"/>
     </row>
-    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="28" t="s">
         <v>69</v>
       </c>
@@ -6809,7 +6809,7 @@
       </c>
       <c r="Q127" s="28"/>
     </row>
-    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="28" t="s">
         <v>69</v>
       </c>
@@ -6853,7 +6853,7 @@
       </c>
       <c r="Q128" s="28"/>
     </row>
-    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="28" t="s">
         <v>69</v>
       </c>
@@ -6897,7 +6897,7 @@
       </c>
       <c r="Q129" s="28"/>
     </row>
-    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="28" t="s">
         <v>69</v>
       </c>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="Q130" s="28"/>
     </row>
-    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="28" t="s">
         <v>69</v>
       </c>
@@ -6985,7 +6985,7 @@
       </c>
       <c r="Q131" s="28"/>
     </row>
-    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="28" t="s">
         <v>69</v>
       </c>
@@ -7029,7 +7029,7 @@
       </c>
       <c r="Q132" s="28"/>
     </row>
-    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="28" t="s">
         <v>69</v>
       </c>
@@ -7073,7 +7073,7 @@
       </c>
       <c r="Q133" s="28"/>
     </row>
-    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="28" t="s">
         <v>69</v>
       </c>
@@ -7117,7 +7117,7 @@
       </c>
       <c r="Q134" s="28"/>
     </row>
-    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="28" t="s">
         <v>69</v>
       </c>
@@ -7161,7 +7161,7 @@
       </c>
       <c r="Q135" s="28"/>
     </row>
-    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="28" t="s">
         <v>69</v>
       </c>
@@ -7205,7 +7205,7 @@
       </c>
       <c r="Q136" s="28"/>
     </row>
-    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="28" t="s">
         <v>69</v>
       </c>
@@ -7249,7 +7249,7 @@
       </c>
       <c r="Q137" s="28"/>
     </row>
-    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="28" t="s">
         <v>69</v>
       </c>
@@ -7293,7 +7293,7 @@
       </c>
       <c r="Q138" s="28"/>
     </row>
-    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="28" t="s">
         <v>69</v>
       </c>
@@ -7337,7 +7337,7 @@
       </c>
       <c r="Q139" s="28"/>
     </row>
-    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="28" t="s">
         <v>69</v>
       </c>
@@ -7381,7 +7381,7 @@
       </c>
       <c r="Q140" s="28"/>
     </row>
-    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="28" t="s">
         <v>69</v>
       </c>
@@ -7425,7 +7425,7 @@
       </c>
       <c r="Q141" s="28"/>
     </row>
-    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="28" t="s">
         <v>69</v>
       </c>
@@ -7469,7 +7469,7 @@
       </c>
       <c r="Q142" s="28"/>
     </row>
-    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="28" t="s">
         <v>69</v>
       </c>
@@ -7513,7 +7513,7 @@
       </c>
       <c r="Q143" s="28"/>
     </row>
-    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="28" t="s">
         <v>69</v>
       </c>
@@ -7559,7 +7559,7 @@
       </c>
       <c r="Q144" s="28"/>
     </row>
-    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="32" t="s">
         <v>69</v>
       </c>
@@ -7604,7 +7604,7 @@
       </c>
       <c r="Q145" s="32"/>
     </row>
-    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="32" t="s">
         <v>69</v>
       </c>
@@ -7646,7 +7646,7 @@
       </c>
       <c r="Q146" s="32"/>
     </row>
-    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="32" t="s">
         <v>69</v>
       </c>
@@ -7690,7 +7690,7 @@
       </c>
       <c r="Q147" s="32"/>
     </row>
-    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
         <v>69</v>
       </c>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="Q148" s="5"/>
     </row>
-    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
         <v>69</v>
       </c>
@@ -7777,7 +7777,7 @@
       </c>
       <c r="Q149" s="5"/>
     </row>
-    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
         <v>69</v>
       </c>
@@ -7821,7 +7821,7 @@
       </c>
       <c r="Q150" s="5"/>
     </row>
-    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="9" t="s">
         <v>69</v>
       </c>
@@ -7868,7 +7868,7 @@
       </c>
       <c r="Q151" s="9"/>
     </row>
-    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="12" t="s">
         <v>69</v>
       </c>
@@ -7915,7 +7915,7 @@
       </c>
       <c r="Q152" s="12"/>
     </row>
-    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="16" t="s">
         <v>69</v>
       </c>
@@ -7962,7 +7962,7 @@
       </c>
       <c r="Q153" s="16"/>
     </row>
-    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="20" t="s">
         <v>70</v>
       </c>
@@ -8006,7 +8006,7 @@
       </c>
       <c r="Q154" s="20"/>
     </row>
-    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="20" t="s">
         <v>70</v>
       </c>
@@ -8048,7 +8048,7 @@
       </c>
       <c r="Q155" s="20"/>
     </row>
-    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="20" t="s">
         <v>70</v>
       </c>
@@ -8092,7 +8092,7 @@
       </c>
       <c r="Q156" s="20"/>
     </row>
-    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="24" t="s">
         <v>70</v>
       </c>
@@ -8136,7 +8136,7 @@
       </c>
       <c r="Q157" s="24"/>
     </row>
-    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="24" t="s">
         <v>70</v>
       </c>
@@ -8178,7 +8178,7 @@
       </c>
       <c r="Q158" s="24"/>
     </row>
-    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="24" t="s">
         <v>70</v>
       </c>
@@ -8222,7 +8222,7 @@
       </c>
       <c r="Q159" s="24"/>
     </row>
-    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="28" t="s">
         <v>70</v>
       </c>
@@ -8266,7 +8266,7 @@
       </c>
       <c r="Q160" s="31"/>
     </row>
-    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="28" t="s">
         <v>70</v>
       </c>
@@ -8308,7 +8308,7 @@
       </c>
       <c r="Q161" s="28"/>
     </row>
-    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="28" t="s">
         <v>70</v>
       </c>
@@ -8354,7 +8354,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163" s="32" t="s">
         <v>70</v>
       </c>
@@ -8398,7 +8398,7 @@
       </c>
       <c r="Q163" s="32"/>
     </row>
-    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="32" t="s">
         <v>70</v>
       </c>
@@ -8440,7 +8440,7 @@
       </c>
       <c r="Q164" s="32"/>
     </row>
-    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="32" t="s">
         <v>70</v>
       </c>
@@ -8484,7 +8484,7 @@
       </c>
       <c r="Q165" s="32"/>
     </row>
-    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
         <v>70</v>
       </c>
@@ -8528,7 +8528,7 @@
       </c>
       <c r="Q166" s="5"/>
     </row>
-    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
         <v>70</v>
       </c>
@@ -8570,7 +8570,7 @@
       </c>
       <c r="Q167" s="5"/>
     </row>
-    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
         <v>70</v>
       </c>
@@ -8616,7 +8616,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="9" t="s">
         <v>70</v>
       </c>
@@ -8660,7 +8660,7 @@
       </c>
       <c r="Q169" s="35"/>
     </row>
-    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="9" t="s">
         <v>70</v>
       </c>
@@ -8702,7 +8702,7 @@
       </c>
       <c r="Q170" s="9"/>
     </row>
-    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A171" s="9" t="s">
         <v>70</v>
       </c>
@@ -8744,7 +8744,7 @@
       </c>
       <c r="Q171" s="9"/>
     </row>
-    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172" s="9" t="s">
         <v>70</v>
       </c>
@@ -8786,7 +8786,7 @@
       </c>
       <c r="Q172" s="9"/>
     </row>
-    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A173" s="9" t="s">
         <v>70</v>
       </c>
@@ -8830,7 +8830,7 @@
       </c>
       <c r="Q173" s="9"/>
     </row>
-    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="12" t="s">
         <v>70</v>
       </c>
@@ -8874,7 +8874,7 @@
       </c>
       <c r="Q174" s="14"/>
     </row>
-    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175" s="12" t="s">
         <v>70</v>
       </c>
@@ -8916,7 +8916,7 @@
       </c>
       <c r="Q175" s="12"/>
     </row>
-    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A176" s="12" t="s">
         <v>70</v>
       </c>
@@ -8960,7 +8960,7 @@
       </c>
       <c r="Q176" s="12"/>
     </row>
-    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A177" s="16" t="s">
         <v>70</v>
       </c>
@@ -9006,7 +9006,7 @@
       </c>
       <c r="Q177" s="16"/>
     </row>
-    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A178" s="16" t="s">
         <v>70</v>
       </c>
@@ -9050,7 +9050,7 @@
       </c>
       <c r="Q178" s="19"/>
     </row>
-    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A179" s="16" t="s">
         <v>70</v>
       </c>
@@ -9094,7 +9094,7 @@
       </c>
       <c r="Q179" s="16"/>
     </row>
-    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A180" s="16" t="s">
         <v>70</v>
       </c>
@@ -9140,7 +9140,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A181" s="16" t="s">
         <v>70</v>
       </c>
@@ -9184,7 +9184,7 @@
       </c>
       <c r="Q181" s="16"/>
     </row>
-    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A182" s="16" t="s">
         <v>70</v>
       </c>
@@ -9228,7 +9228,7 @@
       </c>
       <c r="Q182" s="16"/>
     </row>
-    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A183" s="16" t="s">
         <v>70</v>
       </c>
@@ -9272,7 +9272,7 @@
       </c>
       <c r="Q183" s="16"/>
     </row>
-    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A184" s="16" t="s">
         <v>70</v>
       </c>
@@ -9316,7 +9316,7 @@
       </c>
       <c r="Q184" s="16"/>
     </row>
-    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A185" s="16" t="s">
         <v>70</v>
       </c>
@@ -9362,7 +9362,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A186" s="16" t="s">
         <v>70</v>
       </c>
@@ -9406,7 +9406,7 @@
       </c>
       <c r="Q186" s="16"/>
     </row>
-    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A187" s="16" t="s">
         <v>70</v>
       </c>
@@ -9450,7 +9450,7 @@
       </c>
       <c r="Q187" s="16"/>
     </row>
-    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A188" s="16" t="s">
         <v>70</v>
       </c>
@@ -9494,7 +9494,7 @@
       </c>
       <c r="Q188" s="19"/>
     </row>
-    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A189" s="16" t="s">
         <v>70</v>
       </c>
@@ -9538,7 +9538,7 @@
       </c>
       <c r="Q189" s="16"/>
     </row>
-    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A190" s="16" t="s">
         <v>70</v>
       </c>
@@ -9582,7 +9582,7 @@
       </c>
       <c r="Q190" s="16"/>
     </row>
-    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A191" s="16" t="s">
         <v>70</v>
       </c>
@@ -9628,7 +9628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192" s="16" t="s">
         <v>70</v>
       </c>
@@ -9672,7 +9672,7 @@
       </c>
       <c r="Q192" s="16"/>
     </row>
-    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193" s="16" t="s">
         <v>70</v>
       </c>
@@ -9716,7 +9716,7 @@
       </c>
       <c r="Q193" s="16"/>
     </row>
-    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="16" t="s">
         <v>70</v>
       </c>
@@ -9760,7 +9760,7 @@
       </c>
       <c r="Q194" s="16"/>
     </row>
-    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="16" t="s">
         <v>70</v>
       </c>
@@ -9804,7 +9804,7 @@
       </c>
       <c r="Q195" s="16"/>
     </row>
-    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196" s="16" t="s">
         <v>70</v>
       </c>
@@ -9850,7 +9850,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A197" s="16" t="s">
         <v>70</v>
       </c>
@@ -9894,7 +9894,7 @@
       </c>
       <c r="Q197" s="16"/>
     </row>
-    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198" s="16" t="s">
         <v>70</v>
       </c>
@@ -9940,7 +9940,7 @@
       </c>
       <c r="Q198" s="19"/>
     </row>
-    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199" s="20" t="s">
         <v>70</v>
       </c>
@@ -9986,7 +9986,7 @@
       </c>
       <c r="Q199" s="20"/>
     </row>
-    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200" s="20" t="s">
         <v>70</v>
       </c>
@@ -10030,7 +10030,7 @@
       </c>
       <c r="Q200" s="23"/>
     </row>
-    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201" s="20" t="s">
         <v>70</v>
       </c>
@@ -10074,7 +10074,7 @@
       </c>
       <c r="Q201" s="23"/>
     </row>
-    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202" s="24" t="s">
         <v>70</v>
       </c>
@@ -10118,7 +10118,7 @@
       </c>
       <c r="Q202" s="24"/>
     </row>
-    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A203" s="24" t="s">
         <v>70</v>
       </c>
@@ -10160,7 +10160,7 @@
       </c>
       <c r="Q203" s="24"/>
     </row>
-    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204" s="24" t="s">
         <v>70</v>
       </c>
@@ -10202,7 +10202,7 @@
       </c>
       <c r="Q204" s="24"/>
     </row>
-    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A205" s="24" t="s">
         <v>70</v>
       </c>
@@ -10246,7 +10246,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206" s="24" t="s">
         <v>70</v>
       </c>
@@ -10288,7 +10288,7 @@
       </c>
       <c r="Q206" s="24"/>
     </row>
-    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A207" s="24" t="s">
         <v>70</v>
       </c>
@@ -10332,7 +10332,7 @@
       </c>
       <c r="Q207" s="24"/>
     </row>
-    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A208" s="28" t="s">
         <v>70</v>
       </c>
@@ -10376,7 +10376,7 @@
       </c>
       <c r="Q208" s="28"/>
     </row>
-    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A209" s="28" t="s">
         <v>70</v>
       </c>
@@ -10418,7 +10418,7 @@
       </c>
       <c r="Q209" s="28"/>
     </row>
-    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" s="28" t="s">
         <v>70</v>
       </c>
@@ -10462,7 +10462,7 @@
       </c>
       <c r="Q210" s="28"/>
     </row>
-    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A211" s="32" t="s">
         <v>70</v>
       </c>
@@ -10506,7 +10506,7 @@
       </c>
       <c r="Q211" s="32"/>
     </row>
-    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A212" s="32" t="s">
         <v>70</v>
       </c>
@@ -10548,7 +10548,7 @@
       </c>
       <c r="Q212" s="32"/>
     </row>
-    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A213" s="32" t="s">
         <v>70</v>
       </c>
@@ -10592,7 +10592,7 @@
       </c>
       <c r="Q213" s="36"/>
     </row>
-    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A214" s="5" t="s">
         <v>70</v>
       </c>
@@ -10636,7 +10636,7 @@
       </c>
       <c r="Q214" s="5"/>
     </row>
-    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A215" s="5" t="s">
         <v>70</v>
       </c>
@@ -10678,7 +10678,7 @@
       </c>
       <c r="Q215" s="5"/>
     </row>
-    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A216" s="5" t="s">
         <v>70</v>
       </c>
@@ -10722,7 +10722,7 @@
       </c>
       <c r="Q216" s="5"/>
     </row>
-    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A217" s="9" t="s">
         <v>70</v>
       </c>
@@ -10766,7 +10766,7 @@
       </c>
       <c r="Q217" s="9"/>
     </row>
-    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218" s="9" t="s">
         <v>70</v>
       </c>
@@ -10808,7 +10808,7 @@
       </c>
       <c r="Q218" s="9"/>
     </row>
-    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A219" s="9" t="s">
         <v>70</v>
       </c>
@@ -10852,7 +10852,7 @@
       </c>
       <c r="Q219" s="9"/>
     </row>
-    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A220" s="12" t="s">
         <v>70</v>
       </c>
@@ -10898,7 +10898,7 @@
       </c>
       <c r="Q220" s="12"/>
     </row>
-    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A221" s="16" t="s">
         <v>70</v>
       </c>
@@ -10944,7 +10944,7 @@
       </c>
       <c r="Q221" s="16"/>
     </row>
-    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A222" s="16" t="s">
         <v>70</v>
       </c>
@@ -10988,7 +10988,7 @@
       </c>
       <c r="Q222" s="16"/>
     </row>
-    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A223" s="16" t="s">
         <v>70</v>
       </c>
@@ -11034,7 +11034,7 @@
       </c>
       <c r="Q223" s="16"/>
     </row>
-    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A224" s="20" t="s">
         <v>70</v>
       </c>
@@ -11080,7 +11080,7 @@
       </c>
       <c r="Q224" s="20"/>
     </row>
-    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225" s="24" t="s">
         <v>70</v>
       </c>
@@ -11126,7 +11126,7 @@
       </c>
       <c r="Q225" s="24"/>
     </row>
-    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A226" s="28" t="s">
         <v>70</v>
       </c>
@@ -11172,7 +11172,7 @@
       </c>
       <c r="Q226" s="28"/>
     </row>
-    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A227" s="28" t="s">
         <v>70</v>
       </c>
@@ -11216,7 +11216,7 @@
       </c>
       <c r="Q227" s="28"/>
     </row>
-    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A228" s="28" t="s">
         <v>70</v>
       </c>
@@ -11262,7 +11262,7 @@
       </c>
       <c r="Q228" s="28"/>
     </row>
-    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A229" s="32" t="s">
         <v>70</v>
       </c>
@@ -11308,7 +11308,7 @@
       </c>
       <c r="Q229" s="32"/>
     </row>
-    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A230" s="5" t="s">
         <v>70</v>
       </c>
@@ -11367,19 +11367,19 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
         <v>68</v>
       </c>
@@ -11402,7 +11402,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11419,7 +11419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11442,7 +11442,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11465,7 +11465,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11482,7 +11482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11499,7 +11499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11522,7 +11522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11562,7 +11562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11579,7 +11579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11602,7 +11602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11619,7 +11619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11636,7 +11636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11653,7 +11653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11670,7 +11670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11687,7 +11687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11704,7 +11704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11721,7 +11721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -11738,7 +11738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -11755,7 +11755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -11772,7 +11772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -11802,14 +11802,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>55</v>
       </c>
@@ -11826,7 +11826,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -11843,7 +11843,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -11860,7 +11860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -11877,7 +11877,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -11894,7 +11894,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -11911,7 +11911,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -11928,7 +11928,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -11945,7 +11945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -11962,7 +11962,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -11973,13 +11973,13 @@
         <v>33</v>
       </c>
       <c r="D10">
+        <v>32</v>
+      </c>
+      <c r="E10">
         <v>72</v>
       </c>
-      <c r="E10">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -11990,13 +11990,13 @@
         <v>38</v>
       </c>
       <c r="D11">
+        <v>39</v>
+      </c>
+      <c r="E11">
         <v>71</v>
       </c>
-      <c r="E11">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -12007,13 +12007,13 @@
         <v>44</v>
       </c>
       <c r="D12">
+        <v>43</v>
+      </c>
+      <c r="E12">
         <v>67</v>
       </c>
-      <c r="E12">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -12024,13 +12024,13 @@
         <v>52</v>
       </c>
       <c r="D13">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E13">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -12057,21 +12057,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="47" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.88671875" style="47"/>
-    <col min="6" max="6" width="10.109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="47"/>
+    <col min="3" max="5" width="8.83203125" style="47"/>
+    <col min="6" max="6" width="10.1640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>74</v>
       </c>
@@ -12091,7 +12091,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="48">
         <v>1</v>
       </c>
@@ -12111,7 +12111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="48">
         <v>2</v>
       </c>
@@ -12131,7 +12131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="48">
         <v>3</v>
       </c>
@@ -12151,7 +12151,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="48">
         <v>4</v>
       </c>
@@ -12171,7 +12171,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="49">
         <v>6</v>
       </c>
@@ -12191,7 +12191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="49">
         <v>7</v>
       </c>
@@ -12211,7 +12211,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="49">
         <v>8</v>
       </c>
@@ -12231,7 +12231,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="49">
         <v>9</v>
       </c>
@@ -12251,7 +12251,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="49">
         <v>10</v>
       </c>
@@ -12271,7 +12271,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="49">
         <v>11</v>
       </c>
@@ -12291,7 +12291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="49">
         <v>12</v>
       </c>
@@ -12311,7 +12311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="49">
         <v>13</v>
       </c>
@@ -12331,7 +12331,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="49">
         <v>14</v>
       </c>
@@ -12351,7 +12351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="49">
         <v>15</v>
       </c>
@@ -12371,7 +12371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="49">
         <v>16</v>
       </c>
@@ -12391,7 +12391,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="49">
         <v>17</v>
       </c>
@@ -12411,7 +12411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="49">
         <v>18</v>
       </c>
@@ -12431,7 +12431,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49">
         <v>19</v>
       </c>
@@ -12451,7 +12451,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="49">
         <v>20</v>
       </c>
@@ -12471,7 +12471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="49">
         <v>21</v>
       </c>
@@ -12491,7 +12491,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="49">
         <v>22</v>
       </c>
@@ -12511,7 +12511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="49">
         <v>23</v>
       </c>
@@ -12531,7 +12531,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="49">
         <v>24</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="49">
         <v>25</v>
       </c>
@@ -12571,7 +12571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="49">
         <v>26</v>
       </c>
@@ -12591,7 +12591,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="49">
         <v>27</v>
       </c>
@@ -12611,7 +12611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="49">
         <v>28</v>
       </c>
@@ -12631,7 +12631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="49">
         <v>29</v>
       </c>
@@ -12651,7 +12651,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="49">
         <v>30</v>
       </c>
@@ -12671,7 +12671,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="49">
         <v>31</v>
       </c>
@@ -12691,7 +12691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="49">
         <v>32</v>
       </c>
@@ -12711,7 +12711,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="49">
         <v>33</v>
       </c>
@@ -12731,7 +12731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="49">
         <v>34</v>
       </c>
@@ -12751,7 +12751,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="49">
         <v>35</v>
       </c>
@@ -12771,7 +12771,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="49">
         <v>36</v>
       </c>
@@ -12791,7 +12791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="49">
         <v>37</v>
       </c>
@@ -12811,7 +12811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="49">
         <v>38</v>
       </c>
@@ -12831,7 +12831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="49">
         <v>39</v>
       </c>
@@ -12851,7 +12851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="49">
         <v>40</v>
       </c>
@@ -12871,7 +12871,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="49">
         <v>41</v>
       </c>
@@ -12891,7 +12891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="49">
         <v>42</v>
       </c>
@@ -12911,7 +12911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="49">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Added beacon to TrackData file.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylemonto/Documents/Pitt/Senior/COE 1186/ECE1186/TrainSystem/src/com/rogueone/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan94\Documents\Coding\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="6840" windowWidth="33240" windowHeight="11560" activeTab="4"/>
+    <workbookView xWindow="1296" yWindow="6840" windowWidth="33240" windowHeight="11556" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="78">
   <si>
     <t>A</t>
   </si>
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -817,19 +817,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -848,9 +848,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
@@ -858,7 +858,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -874,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -882,7 +882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -890,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -898,7 +898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -906,7 +906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -914,7 +914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -922,7 +922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -930,7 +930,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -938,7 +938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -946,7 +946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -954,7 +954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -962,7 +962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -970,7 +970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -978,7 +978,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -986,7 +986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -994,7 +994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -1260,34 +1260,34 @@
   <dimension ref="A1:Q230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I161" sqref="I161:I162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.83203125" style="1"/>
+    <col min="16" max="16" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>69</v>
       </c>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>69</v>
       </c>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>69</v>
       </c>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>69</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>69</v>
       </c>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>69</v>
       </c>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>69</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>69</v>
       </c>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="Q9" s="12"/>
     </row>
-    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>69</v>
       </c>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>69</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="Q12" s="12"/>
     </row>
-    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>69</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>69</v>
       </c>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="Q14" s="16"/>
     </row>
-    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>69</v>
       </c>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>69</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>69</v>
       </c>
@@ -2033,7 +2033,7 @@
       </c>
       <c r="Q17" s="19"/>
     </row>
-    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>69</v>
       </c>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="Q18" s="20"/>
     </row>
-    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>69</v>
       </c>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="Q19" s="20"/>
     </row>
-    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>69</v>
       </c>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="Q20" s="23"/>
     </row>
-    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>69</v>
       </c>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="Q21" s="20"/>
     </row>
-    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>69</v>
       </c>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="Q22" s="24"/>
     </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>69</v>
       </c>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="Q23" s="27"/>
     </row>
-    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>69</v>
       </c>
@@ -2335,7 +2335,7 @@
       </c>
       <c r="Q24" s="24"/>
     </row>
-    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>69</v>
       </c>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="Q25" s="24"/>
     </row>
-    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>69</v>
       </c>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="Q26" s="24"/>
     </row>
-    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>69</v>
       </c>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="Q27" s="24"/>
     </row>
-    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>69</v>
       </c>
@@ -2503,7 +2503,7 @@
       </c>
       <c r="Q28" s="24"/>
     </row>
-    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>69</v>
       </c>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="Q29" s="24"/>
     </row>
-    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
         <v>69</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
         <v>69</v>
       </c>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="Q31" s="28"/>
     </row>
-    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
         <v>69</v>
       </c>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="Q32" s="31"/>
     </row>
-    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
         <v>69</v>
       </c>
@@ -2722,7 +2722,7 @@
       </c>
       <c r="Q33" s="28"/>
     </row>
-    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="32" t="s">
         <v>69</v>
       </c>
@@ -2767,7 +2767,7 @@
       </c>
       <c r="Q34" s="32"/>
     </row>
-    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="32" t="s">
         <v>69</v>
       </c>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="Q35" s="32"/>
     </row>
-    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="32" t="s">
         <v>69</v>
       </c>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="Q36" s="32"/>
     </row>
-    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>69</v>
       </c>
@@ -2900,7 +2900,7 @@
       </c>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>69</v>
       </c>
@@ -2944,7 +2944,7 @@
       </c>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>69</v>
       </c>
@@ -2988,7 +2988,7 @@
       </c>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>69</v>
       </c>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>69</v>
       </c>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>69</v>
       </c>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>69</v>
       </c>
@@ -3164,7 +3164,7 @@
       </c>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>69</v>
       </c>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>69</v>
       </c>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>69</v>
       </c>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>69</v>
       </c>
@@ -3340,7 +3340,7 @@
       </c>
       <c r="Q47" s="5"/>
     </row>
-    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>69</v>
       </c>
@@ -3384,7 +3384,7 @@
       </c>
       <c r="Q48" s="5"/>
     </row>
-    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>69</v>
       </c>
@@ -3428,7 +3428,7 @@
       </c>
       <c r="Q49" s="8"/>
     </row>
-    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>69</v>
       </c>
@@ -3472,7 +3472,7 @@
       </c>
       <c r="Q50" s="5"/>
     </row>
-    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>69</v>
       </c>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="Q51" s="5"/>
     </row>
-    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>69</v>
       </c>
@@ -3560,7 +3560,7 @@
       </c>
       <c r="Q52" s="5"/>
     </row>
-    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>69</v>
       </c>
@@ -3604,7 +3604,7 @@
       </c>
       <c r="Q53" s="5"/>
     </row>
-    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>69</v>
       </c>
@@ -3648,7 +3648,7 @@
       </c>
       <c r="Q54" s="5"/>
     </row>
-    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>69</v>
       </c>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="Q55" s="5"/>
     </row>
-    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>69</v>
       </c>
@@ -3736,7 +3736,7 @@
       </c>
       <c r="Q56" s="5"/>
     </row>
-    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>69</v>
       </c>
@@ -3780,7 +3780,7 @@
       </c>
       <c r="Q57" s="5"/>
     </row>
-    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>69</v>
       </c>
@@ -3826,7 +3826,7 @@
       </c>
       <c r="Q58" s="8"/>
     </row>
-    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
         <v>69</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>69</v>
       </c>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="Q60" s="9"/>
     </row>
-    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>69</v>
       </c>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="Q61" s="9"/>
     </row>
-    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>69</v>
       </c>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="Q62" s="9"/>
     </row>
-    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>69</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
         <v>69</v>
       </c>
@@ -4090,7 +4090,7 @@
       </c>
       <c r="Q64" s="12"/>
     </row>
-    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
         <v>69</v>
       </c>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="Q65" s="12"/>
     </row>
-    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
         <v>69</v>
       </c>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="Q66" s="14"/>
     </row>
-    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
         <v>69</v>
       </c>
@@ -4216,7 +4216,7 @@
       </c>
       <c r="Q67" s="12"/>
     </row>
-    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
         <v>69</v>
       </c>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="Q68" s="12"/>
     </row>
-    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
         <v>69</v>
       </c>
@@ -4302,7 +4302,7 @@
       </c>
       <c r="Q69" s="12"/>
     </row>
-    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
         <v>69</v>
       </c>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="Q70" s="16"/>
     </row>
-    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
         <v>69</v>
       </c>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="Q71" s="16"/>
     </row>
-    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
         <v>69</v>
       </c>
@@ -4431,7 +4431,7 @@
       </c>
       <c r="Q72" s="16"/>
     </row>
-    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
         <v>69</v>
       </c>
@@ -4473,7 +4473,7 @@
       </c>
       <c r="Q73" s="16"/>
     </row>
-    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
         <v>69</v>
       </c>
@@ -4517,7 +4517,7 @@
       </c>
       <c r="Q74" s="19"/>
     </row>
-    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="20" t="s">
         <v>69</v>
       </c>
@@ -4562,7 +4562,7 @@
       </c>
       <c r="Q75" s="20"/>
     </row>
-    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="20" t="s">
         <v>69</v>
       </c>
@@ -4604,7 +4604,7 @@
       </c>
       <c r="Q76" s="20"/>
     </row>
-    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="20" t="s">
         <v>69</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="24" t="s">
         <v>69</v>
       </c>
@@ -4694,7 +4694,7 @@
       </c>
       <c r="Q78" s="27"/>
     </row>
-    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="24" t="s">
         <v>69</v>
       </c>
@@ -4736,7 +4736,7 @@
       </c>
       <c r="Q79" s="24"/>
     </row>
-    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="24" t="s">
         <v>69</v>
       </c>
@@ -4778,7 +4778,7 @@
       </c>
       <c r="Q80" s="24"/>
     </row>
-    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
         <v>69</v>
       </c>
@@ -4820,7 +4820,7 @@
       </c>
       <c r="Q81" s="24"/>
     </row>
-    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="24" t="s">
         <v>69</v>
       </c>
@@ -4862,7 +4862,7 @@
       </c>
       <c r="Q82" s="24"/>
     </row>
-    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="24" t="s">
         <v>69</v>
       </c>
@@ -4904,7 +4904,7 @@
       </c>
       <c r="Q83" s="24"/>
     </row>
-    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="24" t="s">
         <v>69</v>
       </c>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="Q84" s="24"/>
     </row>
-    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="24" t="s">
         <v>69</v>
       </c>
@@ -4988,7 +4988,7 @@
       </c>
       <c r="Q85" s="24"/>
     </row>
-    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="24" t="s">
         <v>69</v>
       </c>
@@ -5032,7 +5032,7 @@
       </c>
       <c r="Q86" s="24"/>
     </row>
-    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="28" t="s">
         <v>69</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="28" t="s">
         <v>69</v>
       </c>
@@ -5121,7 +5121,7 @@
       </c>
       <c r="Q88" s="28"/>
     </row>
-    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="28" t="s">
         <v>69</v>
       </c>
@@ -5165,7 +5165,7 @@
       </c>
       <c r="Q89" s="31"/>
     </row>
-    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="32" t="s">
         <v>69</v>
       </c>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="Q90" s="32"/>
     </row>
-    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="32" t="s">
         <v>69</v>
       </c>
@@ -5252,7 +5252,7 @@
       </c>
       <c r="Q91" s="32"/>
     </row>
-    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="32" t="s">
         <v>69</v>
       </c>
@@ -5294,7 +5294,7 @@
       </c>
       <c r="Q92" s="32"/>
     </row>
-    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="32" t="s">
         <v>69</v>
       </c>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="Q93" s="32"/>
     </row>
-    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="32" t="s">
         <v>69</v>
       </c>
@@ -5378,7 +5378,7 @@
       </c>
       <c r="Q94" s="32"/>
     </row>
-    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="32" t="s">
         <v>69</v>
       </c>
@@ -5420,7 +5420,7 @@
       </c>
       <c r="Q95" s="32"/>
     </row>
-    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="32" t="s">
         <v>69</v>
       </c>
@@ -5462,7 +5462,7 @@
       </c>
       <c r="Q96" s="32"/>
     </row>
-    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="32" t="s">
         <v>69</v>
       </c>
@@ -5504,7 +5504,7 @@
       </c>
       <c r="Q97" s="36"/>
     </row>
-    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="32" t="s">
         <v>69</v>
       </c>
@@ -5548,7 +5548,7 @@
       </c>
       <c r="Q98" s="32"/>
     </row>
-    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>69</v>
       </c>
@@ -5593,7 +5593,7 @@
       </c>
       <c r="Q99" s="5"/>
     </row>
-    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>69</v>
       </c>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="Q100" s="5"/>
     </row>
-    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>69</v>
       </c>
@@ -5679,7 +5679,7 @@
       </c>
       <c r="Q101" s="5"/>
     </row>
-    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
         <v>69</v>
       </c>
@@ -5726,7 +5726,7 @@
       </c>
       <c r="Q102" s="9"/>
     </row>
-    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
         <v>69</v>
       </c>
@@ -5771,7 +5771,7 @@
       </c>
       <c r="Q103" s="12"/>
     </row>
-    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
         <v>69</v>
       </c>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="Q104" s="12"/>
     </row>
-    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
         <v>69</v>
       </c>
@@ -5857,7 +5857,7 @@
       </c>
       <c r="Q105" s="12"/>
     </row>
-    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="16" t="s">
         <v>69</v>
       </c>
@@ -5902,7 +5902,7 @@
       </c>
       <c r="Q106" s="19"/>
     </row>
-    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="16" t="s">
         <v>69</v>
       </c>
@@ -5944,7 +5944,7 @@
       </c>
       <c r="Q107" s="16"/>
     </row>
-    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="16" t="s">
         <v>69</v>
       </c>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="Q108" s="16"/>
     </row>
-    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="16" t="s">
         <v>69</v>
       </c>
@@ -6028,7 +6028,7 @@
       </c>
       <c r="Q109" s="16"/>
     </row>
-    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="16" t="s">
         <v>69</v>
       </c>
@@ -6072,7 +6072,7 @@
       </c>
       <c r="Q110" s="16"/>
     </row>
-    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="20" t="s">
         <v>69</v>
       </c>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="Q111" s="20"/>
     </row>
-    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="20" t="s">
         <v>69</v>
       </c>
@@ -6159,7 +6159,7 @@
       </c>
       <c r="Q112" s="20"/>
     </row>
-    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="20" t="s">
         <v>69</v>
       </c>
@@ -6201,7 +6201,7 @@
       </c>
       <c r="Q113" s="20"/>
     </row>
-    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="20" t="s">
         <v>69</v>
       </c>
@@ -6243,7 +6243,7 @@
       </c>
       <c r="Q114" s="20"/>
     </row>
-    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="20" t="s">
         <v>69</v>
       </c>
@@ -6285,7 +6285,7 @@
       </c>
       <c r="Q115" s="23"/>
     </row>
-    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="20" t="s">
         <v>69</v>
       </c>
@@ -6327,7 +6327,7 @@
       </c>
       <c r="Q116" s="20"/>
     </row>
-    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="20" t="s">
         <v>69</v>
       </c>
@@ -6371,7 +6371,7 @@
       </c>
       <c r="Q117" s="20"/>
     </row>
-    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="24" t="s">
         <v>69</v>
       </c>
@@ -6416,7 +6416,7 @@
       </c>
       <c r="Q118" s="24"/>
     </row>
-    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="24" t="s">
         <v>69</v>
       </c>
@@ -6458,7 +6458,7 @@
       </c>
       <c r="Q119" s="24"/>
     </row>
-    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="24" t="s">
         <v>69</v>
       </c>
@@ -6500,7 +6500,7 @@
       </c>
       <c r="Q120" s="24"/>
     </row>
-    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="24" t="s">
         <v>69</v>
       </c>
@@ -6542,7 +6542,7 @@
       </c>
       <c r="Q121" s="24"/>
     </row>
-    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="24" t="s">
         <v>69</v>
       </c>
@@ -6586,7 +6586,7 @@
       </c>
       <c r="Q122" s="24"/>
     </row>
-    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="28" t="s">
         <v>69</v>
       </c>
@@ -6633,7 +6633,7 @@
       </c>
       <c r="Q123" s="28"/>
     </row>
-    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="28" t="s">
         <v>69</v>
       </c>
@@ -6677,7 +6677,7 @@
       </c>
       <c r="Q124" s="28"/>
     </row>
-    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="28" t="s">
         <v>69</v>
       </c>
@@ -6721,7 +6721,7 @@
       </c>
       <c r="Q125" s="28"/>
     </row>
-    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="28" t="s">
         <v>69</v>
       </c>
@@ -6765,7 +6765,7 @@
       </c>
       <c r="Q126" s="28"/>
     </row>
-    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="28" t="s">
         <v>69</v>
       </c>
@@ -6809,7 +6809,7 @@
       </c>
       <c r="Q127" s="28"/>
     </row>
-    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="28" t="s">
         <v>69</v>
       </c>
@@ -6853,7 +6853,7 @@
       </c>
       <c r="Q128" s="28"/>
     </row>
-    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="28" t="s">
         <v>69</v>
       </c>
@@ -6897,7 +6897,7 @@
       </c>
       <c r="Q129" s="28"/>
     </row>
-    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="28" t="s">
         <v>69</v>
       </c>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="Q130" s="28"/>
     </row>
-    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="28" t="s">
         <v>69</v>
       </c>
@@ -6985,7 +6985,7 @@
       </c>
       <c r="Q131" s="28"/>
     </row>
-    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="28" t="s">
         <v>69</v>
       </c>
@@ -7029,7 +7029,7 @@
       </c>
       <c r="Q132" s="28"/>
     </row>
-    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="28" t="s">
         <v>69</v>
       </c>
@@ -7073,7 +7073,7 @@
       </c>
       <c r="Q133" s="28"/>
     </row>
-    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="28" t="s">
         <v>69</v>
       </c>
@@ -7117,7 +7117,7 @@
       </c>
       <c r="Q134" s="28"/>
     </row>
-    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="28" t="s">
         <v>69</v>
       </c>
@@ -7161,7 +7161,7 @@
       </c>
       <c r="Q135" s="28"/>
     </row>
-    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="28" t="s">
         <v>69</v>
       </c>
@@ -7205,7 +7205,7 @@
       </c>
       <c r="Q136" s="28"/>
     </row>
-    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="28" t="s">
         <v>69</v>
       </c>
@@ -7249,7 +7249,7 @@
       </c>
       <c r="Q137" s="28"/>
     </row>
-    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="28" t="s">
         <v>69</v>
       </c>
@@ -7293,7 +7293,7 @@
       </c>
       <c r="Q138" s="28"/>
     </row>
-    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="28" t="s">
         <v>69</v>
       </c>
@@ -7337,7 +7337,7 @@
       </c>
       <c r="Q139" s="28"/>
     </row>
-    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="28" t="s">
         <v>69</v>
       </c>
@@ -7381,7 +7381,7 @@
       </c>
       <c r="Q140" s="28"/>
     </row>
-    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="28" t="s">
         <v>69</v>
       </c>
@@ -7425,7 +7425,7 @@
       </c>
       <c r="Q141" s="28"/>
     </row>
-    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="28" t="s">
         <v>69</v>
       </c>
@@ -7469,7 +7469,7 @@
       </c>
       <c r="Q142" s="28"/>
     </row>
-    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="28" t="s">
         <v>69</v>
       </c>
@@ -7513,7 +7513,7 @@
       </c>
       <c r="Q143" s="28"/>
     </row>
-    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="28" t="s">
         <v>69</v>
       </c>
@@ -7559,7 +7559,7 @@
       </c>
       <c r="Q144" s="28"/>
     </row>
-    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="32" t="s">
         <v>69</v>
       </c>
@@ -7604,7 +7604,7 @@
       </c>
       <c r="Q145" s="32"/>
     </row>
-    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="32" t="s">
         <v>69</v>
       </c>
@@ -7646,7 +7646,7 @@
       </c>
       <c r="Q146" s="32"/>
     </row>
-    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="32" t="s">
         <v>69</v>
       </c>
@@ -7690,7 +7690,7 @@
       </c>
       <c r="Q147" s="32"/>
     </row>
-    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>69</v>
       </c>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="Q148" s="5"/>
     </row>
-    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>69</v>
       </c>
@@ -7777,7 +7777,7 @@
       </c>
       <c r="Q149" s="5"/>
     </row>
-    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>69</v>
       </c>
@@ -7821,7 +7821,7 @@
       </c>
       <c r="Q150" s="5"/>
     </row>
-    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="9" t="s">
         <v>69</v>
       </c>
@@ -7868,7 +7868,7 @@
       </c>
       <c r="Q151" s="9"/>
     </row>
-    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="12" t="s">
         <v>69</v>
       </c>
@@ -7915,7 +7915,7 @@
       </c>
       <c r="Q152" s="12"/>
     </row>
-    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="16" t="s">
         <v>69</v>
       </c>
@@ -7962,7 +7962,7 @@
       </c>
       <c r="Q153" s="16"/>
     </row>
-    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="20" t="s">
         <v>70</v>
       </c>
@@ -8006,7 +8006,7 @@
       </c>
       <c r="Q154" s="20"/>
     </row>
-    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="20" t="s">
         <v>70</v>
       </c>
@@ -8048,7 +8048,7 @@
       </c>
       <c r="Q155" s="20"/>
     </row>
-    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="20" t="s">
         <v>70</v>
       </c>
@@ -8092,7 +8092,7 @@
       </c>
       <c r="Q156" s="20"/>
     </row>
-    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="24" t="s">
         <v>70</v>
       </c>
@@ -8136,7 +8136,7 @@
       </c>
       <c r="Q157" s="24"/>
     </row>
-    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
         <v>70</v>
       </c>
@@ -8178,7 +8178,7 @@
       </c>
       <c r="Q158" s="24"/>
     </row>
-    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="24" t="s">
         <v>70</v>
       </c>
@@ -8222,7 +8222,7 @@
       </c>
       <c r="Q159" s="24"/>
     </row>
-    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="28" t="s">
         <v>70</v>
       </c>
@@ -8266,7 +8266,7 @@
       </c>
       <c r="Q160" s="31"/>
     </row>
-    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="28" t="s">
         <v>70</v>
       </c>
@@ -8308,7 +8308,7 @@
       </c>
       <c r="Q161" s="28"/>
     </row>
-    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="28" t="s">
         <v>70</v>
       </c>
@@ -8354,7 +8354,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="32" t="s">
         <v>70</v>
       </c>
@@ -8398,7 +8398,7 @@
       </c>
       <c r="Q163" s="32"/>
     </row>
-    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="32" t="s">
         <v>70</v>
       </c>
@@ -8440,7 +8440,7 @@
       </c>
       <c r="Q164" s="32"/>
     </row>
-    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="32" t="s">
         <v>70</v>
       </c>
@@ -8484,7 +8484,7 @@
       </c>
       <c r="Q165" s="32"/>
     </row>
-    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>70</v>
       </c>
@@ -8528,7 +8528,7 @@
       </c>
       <c r="Q166" s="5"/>
     </row>
-    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>70</v>
       </c>
@@ -8570,7 +8570,7 @@
       </c>
       <c r="Q167" s="5"/>
     </row>
-    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>70</v>
       </c>
@@ -8616,7 +8616,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="9" t="s">
         <v>70</v>
       </c>
@@ -8660,7 +8660,7 @@
       </c>
       <c r="Q169" s="35"/>
     </row>
-    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="9" t="s">
         <v>70</v>
       </c>
@@ -8702,7 +8702,7 @@
       </c>
       <c r="Q170" s="9"/>
     </row>
-    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A171" s="9" t="s">
         <v>70</v>
       </c>
@@ -8744,7 +8744,7 @@
       </c>
       <c r="Q171" s="9"/>
     </row>
-    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="9" t="s">
         <v>70</v>
       </c>
@@ -8786,7 +8786,7 @@
       </c>
       <c r="Q172" s="9"/>
     </row>
-    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="9" t="s">
         <v>70</v>
       </c>
@@ -8830,7 +8830,7 @@
       </c>
       <c r="Q173" s="9"/>
     </row>
-    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
         <v>70</v>
       </c>
@@ -8874,7 +8874,7 @@
       </c>
       <c r="Q174" s="14"/>
     </row>
-    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
         <v>70</v>
       </c>
@@ -8916,7 +8916,7 @@
       </c>
       <c r="Q175" s="12"/>
     </row>
-    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
         <v>70</v>
       </c>
@@ -8960,7 +8960,7 @@
       </c>
       <c r="Q176" s="12"/>
     </row>
-    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A177" s="16" t="s">
         <v>70</v>
       </c>
@@ -9006,7 +9006,7 @@
       </c>
       <c r="Q177" s="16"/>
     </row>
-    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="16" t="s">
         <v>70</v>
       </c>
@@ -9050,7 +9050,7 @@
       </c>
       <c r="Q178" s="19"/>
     </row>
-    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="16" t="s">
         <v>70</v>
       </c>
@@ -9094,7 +9094,7 @@
       </c>
       <c r="Q179" s="16"/>
     </row>
-    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="16" t="s">
         <v>70</v>
       </c>
@@ -9140,7 +9140,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A181" s="16" t="s">
         <v>70</v>
       </c>
@@ -9184,7 +9184,7 @@
       </c>
       <c r="Q181" s="16"/>
     </row>
-    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182" s="16" t="s">
         <v>70</v>
       </c>
@@ -9228,7 +9228,7 @@
       </c>
       <c r="Q182" s="16"/>
     </row>
-    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="16" t="s">
         <v>70</v>
       </c>
@@ -9272,7 +9272,7 @@
       </c>
       <c r="Q183" s="16"/>
     </row>
-    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="16" t="s">
         <v>70</v>
       </c>
@@ -9316,7 +9316,7 @@
       </c>
       <c r="Q184" s="16"/>
     </row>
-    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="16" t="s">
         <v>70</v>
       </c>
@@ -9362,7 +9362,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A186" s="16" t="s">
         <v>70</v>
       </c>
@@ -9406,7 +9406,7 @@
       </c>
       <c r="Q186" s="16"/>
     </row>
-    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="16" t="s">
         <v>70</v>
       </c>
@@ -9450,7 +9450,7 @@
       </c>
       <c r="Q187" s="16"/>
     </row>
-    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="16" t="s">
         <v>70</v>
       </c>
@@ -9494,7 +9494,7 @@
       </c>
       <c r="Q188" s="19"/>
     </row>
-    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="16" t="s">
         <v>70</v>
       </c>
@@ -9538,7 +9538,7 @@
       </c>
       <c r="Q189" s="16"/>
     </row>
-    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="16" t="s">
         <v>70</v>
       </c>
@@ -9582,7 +9582,7 @@
       </c>
       <c r="Q190" s="16"/>
     </row>
-    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="16" t="s">
         <v>70</v>
       </c>
@@ -9628,7 +9628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="16" t="s">
         <v>70</v>
       </c>
@@ -9672,7 +9672,7 @@
       </c>
       <c r="Q192" s="16"/>
     </row>
-    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="16" t="s">
         <v>70</v>
       </c>
@@ -9716,7 +9716,7 @@
       </c>
       <c r="Q193" s="16"/>
     </row>
-    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="16" t="s">
         <v>70</v>
       </c>
@@ -9760,7 +9760,7 @@
       </c>
       <c r="Q194" s="16"/>
     </row>
-    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A195" s="16" t="s">
         <v>70</v>
       </c>
@@ -9804,7 +9804,7 @@
       </c>
       <c r="Q195" s="16"/>
     </row>
-    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="16" t="s">
         <v>70</v>
       </c>
@@ -9850,7 +9850,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="16" t="s">
         <v>70</v>
       </c>
@@ -9894,7 +9894,7 @@
       </c>
       <c r="Q197" s="16"/>
     </row>
-    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="16" t="s">
         <v>70</v>
       </c>
@@ -9940,7 +9940,7 @@
       </c>
       <c r="Q198" s="19"/>
     </row>
-    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A199" s="20" t="s">
         <v>70</v>
       </c>
@@ -9986,7 +9986,7 @@
       </c>
       <c r="Q199" s="20"/>
     </row>
-    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A200" s="20" t="s">
         <v>70</v>
       </c>
@@ -10030,7 +10030,7 @@
       </c>
       <c r="Q200" s="23"/>
     </row>
-    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A201" s="20" t="s">
         <v>70</v>
       </c>
@@ -10074,7 +10074,7 @@
       </c>
       <c r="Q201" s="23"/>
     </row>
-    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="24" t="s">
         <v>70</v>
       </c>
@@ -10118,7 +10118,7 @@
       </c>
       <c r="Q202" s="24"/>
     </row>
-    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A203" s="24" t="s">
         <v>70</v>
       </c>
@@ -10160,7 +10160,7 @@
       </c>
       <c r="Q203" s="24"/>
     </row>
-    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A204" s="24" t="s">
         <v>70</v>
       </c>
@@ -10202,7 +10202,7 @@
       </c>
       <c r="Q204" s="24"/>
     </row>
-    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="24" t="s">
         <v>70</v>
       </c>
@@ -10246,7 +10246,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A206" s="24" t="s">
         <v>70</v>
       </c>
@@ -10288,7 +10288,7 @@
       </c>
       <c r="Q206" s="24"/>
     </row>
-    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207" s="24" t="s">
         <v>70</v>
       </c>
@@ -10332,7 +10332,7 @@
       </c>
       <c r="Q207" s="24"/>
     </row>
-    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="28" t="s">
         <v>70</v>
       </c>
@@ -10376,7 +10376,7 @@
       </c>
       <c r="Q208" s="28"/>
     </row>
-    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="28" t="s">
         <v>70</v>
       </c>
@@ -10418,7 +10418,7 @@
       </c>
       <c r="Q209" s="28"/>
     </row>
-    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="28" t="s">
         <v>70</v>
       </c>
@@ -10462,7 +10462,7 @@
       </c>
       <c r="Q210" s="28"/>
     </row>
-    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="32" t="s">
         <v>70</v>
       </c>
@@ -10506,7 +10506,7 @@
       </c>
       <c r="Q211" s="32"/>
     </row>
-    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="32" t="s">
         <v>70</v>
       </c>
@@ -10548,7 +10548,7 @@
       </c>
       <c r="Q212" s="32"/>
     </row>
-    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="32" t="s">
         <v>70</v>
       </c>
@@ -10592,7 +10592,7 @@
       </c>
       <c r="Q213" s="36"/>
     </row>
-    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
         <v>70</v>
       </c>
@@ -10636,7 +10636,7 @@
       </c>
       <c r="Q214" s="5"/>
     </row>
-    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
         <v>70</v>
       </c>
@@ -10678,7 +10678,7 @@
       </c>
       <c r="Q215" s="5"/>
     </row>
-    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
         <v>70</v>
       </c>
@@ -10722,7 +10722,7 @@
       </c>
       <c r="Q216" s="5"/>
     </row>
-    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="9" t="s">
         <v>70</v>
       </c>
@@ -10766,7 +10766,7 @@
       </c>
       <c r="Q217" s="9"/>
     </row>
-    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="9" t="s">
         <v>70</v>
       </c>
@@ -10808,7 +10808,7 @@
       </c>
       <c r="Q218" s="9"/>
     </row>
-    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" s="9" t="s">
         <v>70</v>
       </c>
@@ -10852,7 +10852,7 @@
       </c>
       <c r="Q219" s="9"/>
     </row>
-    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A220" s="12" t="s">
         <v>70</v>
       </c>
@@ -10898,7 +10898,7 @@
       </c>
       <c r="Q220" s="12"/>
     </row>
-    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A221" s="16" t="s">
         <v>70</v>
       </c>
@@ -10944,7 +10944,7 @@
       </c>
       <c r="Q221" s="16"/>
     </row>
-    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A222" s="16" t="s">
         <v>70</v>
       </c>
@@ -10988,7 +10988,7 @@
       </c>
       <c r="Q222" s="16"/>
     </row>
-    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="16" t="s">
         <v>70</v>
       </c>
@@ -11034,7 +11034,7 @@
       </c>
       <c r="Q223" s="16"/>
     </row>
-    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A224" s="20" t="s">
         <v>70</v>
       </c>
@@ -11080,7 +11080,7 @@
       </c>
       <c r="Q224" s="20"/>
     </row>
-    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="24" t="s">
         <v>70</v>
       </c>
@@ -11126,7 +11126,7 @@
       </c>
       <c r="Q225" s="24"/>
     </row>
-    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A226" s="28" t="s">
         <v>70</v>
       </c>
@@ -11172,7 +11172,7 @@
       </c>
       <c r="Q226" s="28"/>
     </row>
-    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A227" s="28" t="s">
         <v>70</v>
       </c>
@@ -11216,7 +11216,7 @@
       </c>
       <c r="Q227" s="28"/>
     </row>
-    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" s="28" t="s">
         <v>70</v>
       </c>
@@ -11262,7 +11262,7 @@
       </c>
       <c r="Q228" s="28"/>
     </row>
-    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A229" s="32" t="s">
         <v>70</v>
       </c>
@@ -11308,7 +11308,7 @@
       </c>
       <c r="Q229" s="32"/>
     </row>
-    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
         <v>70</v>
       </c>
@@ -11367,19 +11367,19 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>68</v>
       </c>
@@ -11402,7 +11402,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11419,7 +11419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11442,7 +11442,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11465,7 +11465,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11482,7 +11482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11499,7 +11499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11522,7 +11522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11562,7 +11562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11579,7 +11579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11602,7 +11602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11619,7 +11619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11636,7 +11636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11653,7 +11653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11670,7 +11670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11687,7 +11687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11704,7 +11704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11721,7 +11721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -11738,7 +11738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -11755,7 +11755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -11772,7 +11772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -11802,14 +11802,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>55</v>
       </c>
@@ -11826,7 +11826,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -11843,7 +11843,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -11860,7 +11860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -11877,7 +11877,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -11894,7 +11894,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -11911,7 +11911,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -11928,7 +11928,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -11945,7 +11945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -11962,7 +11962,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -11979,7 +11979,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -11996,7 +11996,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -12013,7 +12013,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -12030,7 +12030,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -12055,23 +12055,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="47" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.83203125" style="47"/>
-    <col min="6" max="6" width="10.1640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="47"/>
+    <col min="3" max="5" width="8.77734375" style="47"/>
+    <col min="6" max="6" width="10.109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.77734375" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>74</v>
       </c>
@@ -12091,7 +12091,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48">
         <v>1</v>
       </c>
@@ -12111,7 +12111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48">
         <v>2</v>
       </c>
@@ -12131,7 +12131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48">
         <v>3</v>
       </c>
@@ -12151,7 +12151,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="48">
         <v>4</v>
       </c>
@@ -12171,7 +12171,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="49">
         <v>6</v>
       </c>
@@ -12191,7 +12191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="49">
         <v>7</v>
       </c>
@@ -12211,7 +12211,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="49">
         <v>8</v>
       </c>
@@ -12231,7 +12231,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="49">
         <v>9</v>
       </c>
@@ -12251,7 +12251,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="49">
         <v>10</v>
       </c>
@@ -12271,7 +12271,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="49">
         <v>11</v>
       </c>
@@ -12291,7 +12291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="49">
         <v>12</v>
       </c>
@@ -12311,7 +12311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="49">
         <v>13</v>
       </c>
@@ -12331,7 +12331,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="49">
         <v>14</v>
       </c>
@@ -12351,7 +12351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="49">
         <v>15</v>
       </c>
@@ -12371,7 +12371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="49">
         <v>16</v>
       </c>
@@ -12391,7 +12391,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="49">
         <v>17</v>
       </c>
@@ -12411,7 +12411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="49">
         <v>18</v>
       </c>
@@ -12431,7 +12431,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="49">
         <v>19</v>
       </c>
@@ -12451,7 +12451,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="49">
         <v>20</v>
       </c>
@@ -12471,7 +12471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="49">
         <v>21</v>
       </c>
@@ -12491,7 +12491,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="49">
         <v>22</v>
       </c>
@@ -12511,7 +12511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="49">
         <v>23</v>
       </c>
@@ -12531,7 +12531,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="49">
         <v>24</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="49">
         <v>25</v>
       </c>
@@ -12571,7 +12571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="49">
         <v>26</v>
       </c>
@@ -12591,7 +12591,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="49">
         <v>27</v>
       </c>
@@ -12611,7 +12611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="49">
         <v>28</v>
       </c>
@@ -12631,7 +12631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="49">
         <v>29</v>
       </c>
@@ -12651,7 +12651,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="49">
         <v>30</v>
       </c>
@@ -12671,7 +12671,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="49">
         <v>31</v>
       </c>
@@ -12691,7 +12691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="49">
         <v>32</v>
       </c>
@@ -12711,47 +12711,47 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="49">
         <v>33</v>
       </c>
       <c r="B33" s="49" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C33" s="49">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="D33" s="49">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E33" s="49">
         <v>200</v>
       </c>
       <c r="F33" s="49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="49">
         <v>34</v>
       </c>
       <c r="B34" s="49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C34" s="49">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="D34" s="49">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E34" s="49">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="F34" s="49" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="49">
         <v>35</v>
       </c>
@@ -12759,7 +12759,7 @@
         <v>70</v>
       </c>
       <c r="C35" s="49">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D35" s="49">
         <v>17</v>
@@ -12768,10 +12768,10 @@
         <v>225</v>
       </c>
       <c r="F35" s="49" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="49">
         <v>36</v>
       </c>
@@ -12779,19 +12779,19 @@
         <v>70</v>
       </c>
       <c r="C36" s="49">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="D36" s="49">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E36" s="49">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="F36" s="49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="49">
         <v>37</v>
       </c>
@@ -12799,19 +12799,19 @@
         <v>70</v>
       </c>
       <c r="C37" s="49">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D37" s="49">
         <v>18</v>
       </c>
       <c r="E37" s="49">
-        <v>192.2</v>
+        <v>200</v>
       </c>
       <c r="F37" s="49" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="49">
         <v>38</v>
       </c>
@@ -12819,19 +12819,19 @@
         <v>70</v>
       </c>
       <c r="C38" s="49">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D38" s="49">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E38" s="49">
-        <v>200</v>
+        <v>192.2</v>
       </c>
       <c r="F38" s="49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="49">
         <v>39</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>70</v>
       </c>
       <c r="C39" s="49">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D39" s="49">
         <v>19</v>
@@ -12848,10 +12848,10 @@
         <v>200</v>
       </c>
       <c r="F39" s="49" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="49">
         <v>40</v>
       </c>
@@ -12859,10 +12859,10 @@
         <v>70</v>
       </c>
       <c r="C40" s="49">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D40" s="49">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E40" s="49">
         <v>200</v>
@@ -12871,7 +12871,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="49">
         <v>41</v>
       </c>
@@ -12879,7 +12879,7 @@
         <v>70</v>
       </c>
       <c r="C41" s="49">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D41" s="49">
         <v>20</v>
@@ -12888,30 +12888,30 @@
         <v>200</v>
       </c>
       <c r="F41" s="49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="49">
         <v>42</v>
       </c>
       <c r="B42" s="49" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C42" s="49">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D42" s="49">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E42" s="49">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="F42" s="49" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="49">
         <v>43</v>
       </c>
@@ -12919,7 +12919,7 @@
         <v>69</v>
       </c>
       <c r="C43" s="49">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D43" s="49">
         <v>21</v>
@@ -12928,6 +12928,26 @@
         <v>300</v>
       </c>
       <c r="F43" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="49">
+        <v>44</v>
+      </c>
+      <c r="B44" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="49">
+        <v>23</v>
+      </c>
+      <c r="D44" s="49">
+        <v>21</v>
+      </c>
+      <c r="E44" s="49">
+        <v>300</v>
+      </c>
+      <c r="F44" s="49" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 4 beacons to TrackData file
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="78">
   <si>
     <t>A</t>
   </si>
@@ -1260,8 +1260,8 @@
   <dimension ref="A1:Q230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I198" sqref="I198:I200"/>
+      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I229" sqref="I220:I229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12055,11 +12055,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12859,7 +12859,7 @@
         <v>70</v>
       </c>
       <c r="C40" s="49">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D40" s="49">
         <v>19</v>
@@ -12949,6 +12949,86 @@
       </c>
       <c r="F44" s="49" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="49">
+        <v>45</v>
+      </c>
+      <c r="B45" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="49">
+        <v>75</v>
+      </c>
+      <c r="D45" s="49">
+        <v>11</v>
+      </c>
+      <c r="E45" s="49">
+        <v>200</v>
+      </c>
+      <c r="F45" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="49">
+        <v>46</v>
+      </c>
+      <c r="B46" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="49">
+        <v>73</v>
+      </c>
+      <c r="D46" s="49">
+        <v>19</v>
+      </c>
+      <c r="E46" s="49">
+        <v>200</v>
+      </c>
+      <c r="F46" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="49">
+        <v>47</v>
+      </c>
+      <c r="B47" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="49">
+        <v>71</v>
+      </c>
+      <c r="D47" s="49">
+        <v>19</v>
+      </c>
+      <c r="E47" s="49">
+        <v>200</v>
+      </c>
+      <c r="F47" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="49">
+        <v>48</v>
+      </c>
+      <c r="B48" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="49">
+        <v>69</v>
+      </c>
+      <c r="D48" s="49">
+        <v>5</v>
+      </c>
+      <c r="E48" s="49">
+        <v>200</v>
+      </c>
+      <c r="F48" s="49" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Train around the red line to all stations! Don't take waysides
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan94\Documents\Coding\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1296" yWindow="6840" windowWidth="33240" windowHeight="11556" activeTab="5"/>
+    <workbookView xWindow="1300" yWindow="6840" windowWidth="33240" windowHeight="11560" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -21,9 +21,6 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -32,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="78">
   <si>
     <t>A</t>
   </si>
@@ -271,7 +268,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -817,19 +814,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -848,9 +845,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
@@ -858,7 +855,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -866,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -874,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -882,7 +879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -890,7 +887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -898,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -906,7 +903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -914,7 +911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -922,7 +919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -930,7 +927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -938,7 +935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -946,7 +943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -954,7 +951,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -962,7 +959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -970,7 +967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -978,7 +975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -986,7 +983,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -994,7 +991,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1002,7 +999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1010,7 +1007,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1018,7 +1015,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1026,7 +1023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -1034,7 +1031,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1042,7 +1039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -1050,7 +1047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -1058,7 +1055,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -1066,7 +1063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -1074,7 +1071,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1082,7 +1079,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -1090,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -1098,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1106,7 +1103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -1114,7 +1111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -1122,7 +1119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -1130,7 +1127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1138,7 +1135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1146,7 +1143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1154,7 +1151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -1162,7 +1159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -1170,7 +1167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1178,7 +1175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -1186,7 +1183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -1194,7 +1191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -1202,7 +1199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -1210,7 +1207,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -1218,7 +1215,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -1226,7 +1223,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -1234,7 +1231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -1242,7 +1239,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -1260,34 +1257,34 @@
   <dimension ref="A1:Q230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I229" sqref="I220:I229"/>
+      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I198" sqref="I198:I200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.77734375" style="1"/>
+    <col min="14" max="14" width="9.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -1340,7 +1337,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>69</v>
       </c>
@@ -1384,7 +1381,7 @@
       </c>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>69</v>
       </c>
@@ -1426,7 +1423,7 @@
       </c>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>69</v>
       </c>
@@ -1471,7 +1468,7 @@
       </c>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>69</v>
       </c>
@@ -1515,7 +1512,7 @@
       </c>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>69</v>
       </c>
@@ -1557,7 +1554,7 @@
       </c>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>69</v>
       </c>
@@ -1602,7 +1599,7 @@
       </c>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>69</v>
       </c>
@@ -1646,7 +1643,7 @@
       </c>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>69</v>
       </c>
@@ -1688,7 +1685,7 @@
       </c>
       <c r="Q9" s="12"/>
     </row>
-    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -1730,7 +1727,7 @@
       </c>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>69</v>
       </c>
@@ -1772,7 +1769,7 @@
       </c>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>69</v>
       </c>
@@ -1814,7 +1811,7 @@
       </c>
       <c r="Q12" s="12"/>
     </row>
-    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>69</v>
       </c>
@@ -1861,7 +1858,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>69</v>
       </c>
@@ -1905,7 +1902,7 @@
       </c>
       <c r="Q14" s="16"/>
     </row>
-    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>69</v>
       </c>
@@ -1947,7 +1944,7 @@
       </c>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>69</v>
       </c>
@@ -1989,7 +1986,7 @@
       </c>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>69</v>
       </c>
@@ -2033,7 +2030,7 @@
       </c>
       <c r="Q17" s="19"/>
     </row>
-    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
         <v>69</v>
       </c>
@@ -2077,7 +2074,7 @@
       </c>
       <c r="Q18" s="20"/>
     </row>
-    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
         <v>69</v>
       </c>
@@ -2119,7 +2116,7 @@
       </c>
       <c r="Q19" s="20"/>
     </row>
-    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>69</v>
       </c>
@@ -2163,7 +2160,7 @@
       </c>
       <c r="Q20" s="23"/>
     </row>
-    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
         <v>69</v>
       </c>
@@ -2207,7 +2204,7 @@
       </c>
       <c r="Q21" s="20"/>
     </row>
-    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="24" t="s">
         <v>69</v>
       </c>
@@ -2251,7 +2248,7 @@
       </c>
       <c r="Q22" s="24"/>
     </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="24" t="s">
         <v>69</v>
       </c>
@@ -2293,7 +2290,7 @@
       </c>
       <c r="Q23" s="27"/>
     </row>
-    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="24" t="s">
         <v>69</v>
       </c>
@@ -2335,7 +2332,7 @@
       </c>
       <c r="Q24" s="24"/>
     </row>
-    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="24" t="s">
         <v>69</v>
       </c>
@@ -2377,7 +2374,7 @@
       </c>
       <c r="Q25" s="24"/>
     </row>
-    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="24" t="s">
         <v>69</v>
       </c>
@@ -2419,7 +2416,7 @@
       </c>
       <c r="Q26" s="24"/>
     </row>
-    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="24" t="s">
         <v>69</v>
       </c>
@@ -2461,7 +2458,7 @@
       </c>
       <c r="Q27" s="24"/>
     </row>
-    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="24" t="s">
         <v>69</v>
       </c>
@@ -2503,7 +2500,7 @@
       </c>
       <c r="Q28" s="24"/>
     </row>
-    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="24" t="s">
         <v>69</v>
       </c>
@@ -2547,7 +2544,7 @@
       </c>
       <c r="Q29" s="24"/>
     </row>
-    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
         <v>69</v>
       </c>
@@ -2594,7 +2591,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
         <v>69</v>
       </c>
@@ -2636,7 +2633,7 @@
       </c>
       <c r="Q31" s="28"/>
     </row>
-    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>69</v>
       </c>
@@ -2678,7 +2675,7 @@
       </c>
       <c r="Q32" s="31"/>
     </row>
-    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
         <v>69</v>
       </c>
@@ -2722,7 +2719,7 @@
       </c>
       <c r="Q33" s="28"/>
     </row>
-    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="32" t="s">
         <v>69</v>
       </c>
@@ -2767,7 +2764,7 @@
       </c>
       <c r="Q34" s="32"/>
     </row>
-    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="32" t="s">
         <v>69</v>
       </c>
@@ -2809,7 +2806,7 @@
       </c>
       <c r="Q35" s="32"/>
     </row>
-    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="32" t="s">
         <v>69</v>
       </c>
@@ -2853,7 +2850,7 @@
       </c>
       <c r="Q36" s="32"/>
     </row>
-    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>69</v>
       </c>
@@ -2900,7 +2897,7 @@
       </c>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>69</v>
       </c>
@@ -2944,7 +2941,7 @@
       </c>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>69</v>
       </c>
@@ -2988,7 +2985,7 @@
       </c>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>69</v>
       </c>
@@ -3032,7 +3029,7 @@
       </c>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>69</v>
       </c>
@@ -3076,7 +3073,7 @@
       </c>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>69</v>
       </c>
@@ -3120,7 +3117,7 @@
       </c>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>69</v>
       </c>
@@ -3164,7 +3161,7 @@
       </c>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>69</v>
       </c>
@@ -3208,7 +3205,7 @@
       </c>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>69</v>
       </c>
@@ -3252,7 +3249,7 @@
       </c>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>69</v>
       </c>
@@ -3296,7 +3293,7 @@
       </c>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>69</v>
       </c>
@@ -3340,7 +3337,7 @@
       </c>
       <c r="Q47" s="5"/>
     </row>
-    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>69</v>
       </c>
@@ -3384,7 +3381,7 @@
       </c>
       <c r="Q48" s="5"/>
     </row>
-    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>69</v>
       </c>
@@ -3428,7 +3425,7 @@
       </c>
       <c r="Q49" s="8"/>
     </row>
-    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>69</v>
       </c>
@@ -3472,7 +3469,7 @@
       </c>
       <c r="Q50" s="5"/>
     </row>
-    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>69</v>
       </c>
@@ -3516,7 +3513,7 @@
       </c>
       <c r="Q51" s="5"/>
     </row>
-    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>69</v>
       </c>
@@ -3560,7 +3557,7 @@
       </c>
       <c r="Q52" s="5"/>
     </row>
-    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>69</v>
       </c>
@@ -3604,7 +3601,7 @@
       </c>
       <c r="Q53" s="5"/>
     </row>
-    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>69</v>
       </c>
@@ -3648,7 +3645,7 @@
       </c>
       <c r="Q54" s="5"/>
     </row>
-    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>69</v>
       </c>
@@ -3692,7 +3689,7 @@
       </c>
       <c r="Q55" s="5"/>
     </row>
-    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>69</v>
       </c>
@@ -3736,7 +3733,7 @@
       </c>
       <c r="Q56" s="5"/>
     </row>
-    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>69</v>
       </c>
@@ -3780,7 +3777,7 @@
       </c>
       <c r="Q57" s="5"/>
     </row>
-    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>69</v>
       </c>
@@ -3826,7 +3823,7 @@
       </c>
       <c r="Q58" s="8"/>
     </row>
-    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>69</v>
       </c>
@@ -3873,7 +3870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>69</v>
       </c>
@@ -3915,7 +3912,7 @@
       </c>
       <c r="Q60" s="9"/>
     </row>
-    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>69</v>
       </c>
@@ -3957,7 +3954,7 @@
       </c>
       <c r="Q61" s="9"/>
     </row>
-    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>69</v>
       </c>
@@ -3999,7 +3996,7 @@
       </c>
       <c r="Q62" s="9"/>
     </row>
-    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>69</v>
       </c>
@@ -4045,7 +4042,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
         <v>69</v>
       </c>
@@ -4090,7 +4087,7 @@
       </c>
       <c r="Q64" s="12"/>
     </row>
-    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="12" t="s">
         <v>69</v>
       </c>
@@ -4132,7 +4129,7 @@
       </c>
       <c r="Q65" s="12"/>
     </row>
-    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="12" t="s">
         <v>69</v>
       </c>
@@ -4174,7 +4171,7 @@
       </c>
       <c r="Q66" s="14"/>
     </row>
-    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="12" t="s">
         <v>69</v>
       </c>
@@ -4216,7 +4213,7 @@
       </c>
       <c r="Q67" s="12"/>
     </row>
-    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="12" t="s">
         <v>69</v>
       </c>
@@ -4258,7 +4255,7 @@
       </c>
       <c r="Q68" s="12"/>
     </row>
-    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="12" t="s">
         <v>69</v>
       </c>
@@ -4302,7 +4299,7 @@
       </c>
       <c r="Q69" s="12"/>
     </row>
-    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="16" t="s">
         <v>69</v>
       </c>
@@ -4347,7 +4344,7 @@
       </c>
       <c r="Q70" s="16"/>
     </row>
-    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="16" t="s">
         <v>69</v>
       </c>
@@ -4389,7 +4386,7 @@
       </c>
       <c r="Q71" s="16"/>
     </row>
-    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="16" t="s">
         <v>69</v>
       </c>
@@ -4431,7 +4428,7 @@
       </c>
       <c r="Q72" s="16"/>
     </row>
-    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="16" t="s">
         <v>69</v>
       </c>
@@ -4473,7 +4470,7 @@
       </c>
       <c r="Q73" s="16"/>
     </row>
-    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="16" t="s">
         <v>69</v>
       </c>
@@ -4517,7 +4514,7 @@
       </c>
       <c r="Q74" s="19"/>
     </row>
-    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="20" t="s">
         <v>69</v>
       </c>
@@ -4562,7 +4559,7 @@
       </c>
       <c r="Q75" s="20"/>
     </row>
-    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="20" t="s">
         <v>69</v>
       </c>
@@ -4604,7 +4601,7 @@
       </c>
       <c r="Q76" s="20"/>
     </row>
-    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="20" t="s">
         <v>69</v>
       </c>
@@ -4650,7 +4647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="24" t="s">
         <v>69</v>
       </c>
@@ -4694,7 +4691,7 @@
       </c>
       <c r="Q78" s="27"/>
     </row>
-    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="24" t="s">
         <v>69</v>
       </c>
@@ -4736,7 +4733,7 @@
       </c>
       <c r="Q79" s="24"/>
     </row>
-    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="24" t="s">
         <v>69</v>
       </c>
@@ -4778,7 +4775,7 @@
       </c>
       <c r="Q80" s="24"/>
     </row>
-    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="24" t="s">
         <v>69</v>
       </c>
@@ -4820,7 +4817,7 @@
       </c>
       <c r="Q81" s="24"/>
     </row>
-    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="24" t="s">
         <v>69</v>
       </c>
@@ -4862,7 +4859,7 @@
       </c>
       <c r="Q82" s="24"/>
     </row>
-    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="24" t="s">
         <v>69</v>
       </c>
@@ -4904,7 +4901,7 @@
       </c>
       <c r="Q83" s="24"/>
     </row>
-    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="24" t="s">
         <v>69</v>
       </c>
@@ -4946,7 +4943,7 @@
       </c>
       <c r="Q84" s="24"/>
     </row>
-    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="24" t="s">
         <v>69</v>
       </c>
@@ -4988,7 +4985,7 @@
       </c>
       <c r="Q85" s="24"/>
     </row>
-    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="24" t="s">
         <v>69</v>
       </c>
@@ -5032,7 +5029,7 @@
       </c>
       <c r="Q86" s="24"/>
     </row>
-    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="28" t="s">
         <v>69</v>
       </c>
@@ -5079,7 +5076,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="28" t="s">
         <v>69</v>
       </c>
@@ -5121,7 +5118,7 @@
       </c>
       <c r="Q88" s="28"/>
     </row>
-    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="28" t="s">
         <v>69</v>
       </c>
@@ -5165,7 +5162,7 @@
       </c>
       <c r="Q89" s="31"/>
     </row>
-    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="32" t="s">
         <v>69</v>
       </c>
@@ -5210,7 +5207,7 @@
       </c>
       <c r="Q90" s="32"/>
     </row>
-    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="32" t="s">
         <v>69</v>
       </c>
@@ -5252,7 +5249,7 @@
       </c>
       <c r="Q91" s="32"/>
     </row>
-    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="32" t="s">
         <v>69</v>
       </c>
@@ -5294,7 +5291,7 @@
       </c>
       <c r="Q92" s="32"/>
     </row>
-    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="32" t="s">
         <v>69</v>
       </c>
@@ -5336,7 +5333,7 @@
       </c>
       <c r="Q93" s="32"/>
     </row>
-    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="32" t="s">
         <v>69</v>
       </c>
@@ -5378,7 +5375,7 @@
       </c>
       <c r="Q94" s="32"/>
     </row>
-    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="32" t="s">
         <v>69</v>
       </c>
@@ -5420,7 +5417,7 @@
       </c>
       <c r="Q95" s="32"/>
     </row>
-    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="32" t="s">
         <v>69</v>
       </c>
@@ -5462,7 +5459,7 @@
       </c>
       <c r="Q96" s="32"/>
     </row>
-    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="32" t="s">
         <v>69</v>
       </c>
@@ -5504,7 +5501,7 @@
       </c>
       <c r="Q97" s="36"/>
     </row>
-    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="32" t="s">
         <v>69</v>
       </c>
@@ -5548,7 +5545,7 @@
       </c>
       <c r="Q98" s="32"/>
     </row>
-    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>69</v>
       </c>
@@ -5593,7 +5590,7 @@
       </c>
       <c r="Q99" s="5"/>
     </row>
-    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>69</v>
       </c>
@@ -5635,7 +5632,7 @@
       </c>
       <c r="Q100" s="5"/>
     </row>
-    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
         <v>69</v>
       </c>
@@ -5679,7 +5676,7 @@
       </c>
       <c r="Q101" s="5"/>
     </row>
-    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="s">
         <v>69</v>
       </c>
@@ -5726,7 +5723,7 @@
       </c>
       <c r="Q102" s="9"/>
     </row>
-    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="12" t="s">
         <v>69</v>
       </c>
@@ -5771,7 +5768,7 @@
       </c>
       <c r="Q103" s="12"/>
     </row>
-    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="12" t="s">
         <v>69</v>
       </c>
@@ -5813,7 +5810,7 @@
       </c>
       <c r="Q104" s="12"/>
     </row>
-    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="12" t="s">
         <v>69</v>
       </c>
@@ -5857,7 +5854,7 @@
       </c>
       <c r="Q105" s="12"/>
     </row>
-    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="16" t="s">
         <v>69</v>
       </c>
@@ -5902,7 +5899,7 @@
       </c>
       <c r="Q106" s="19"/>
     </row>
-    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="16" t="s">
         <v>69</v>
       </c>
@@ -5944,7 +5941,7 @@
       </c>
       <c r="Q107" s="16"/>
     </row>
-    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="16" t="s">
         <v>69</v>
       </c>
@@ -5986,7 +5983,7 @@
       </c>
       <c r="Q108" s="16"/>
     </row>
-    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A109" s="16" t="s">
         <v>69</v>
       </c>
@@ -6028,7 +6025,7 @@
       </c>
       <c r="Q109" s="16"/>
     </row>
-    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="16" t="s">
         <v>69</v>
       </c>
@@ -6072,7 +6069,7 @@
       </c>
       <c r="Q110" s="16"/>
     </row>
-    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="20" t="s">
         <v>69</v>
       </c>
@@ -6117,7 +6114,7 @@
       </c>
       <c r="Q111" s="20"/>
     </row>
-    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="20" t="s">
         <v>69</v>
       </c>
@@ -6159,7 +6156,7 @@
       </c>
       <c r="Q112" s="20"/>
     </row>
-    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="20" t="s">
         <v>69</v>
       </c>
@@ -6201,7 +6198,7 @@
       </c>
       <c r="Q113" s="20"/>
     </row>
-    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="20" t="s">
         <v>69</v>
       </c>
@@ -6243,7 +6240,7 @@
       </c>
       <c r="Q114" s="20"/>
     </row>
-    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" s="20" t="s">
         <v>69</v>
       </c>
@@ -6285,7 +6282,7 @@
       </c>
       <c r="Q115" s="23"/>
     </row>
-    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A116" s="20" t="s">
         <v>69</v>
       </c>
@@ -6327,7 +6324,7 @@
       </c>
       <c r="Q116" s="20"/>
     </row>
-    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A117" s="20" t="s">
         <v>69</v>
       </c>
@@ -6371,7 +6368,7 @@
       </c>
       <c r="Q117" s="20"/>
     </row>
-    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A118" s="24" t="s">
         <v>69</v>
       </c>
@@ -6416,7 +6413,7 @@
       </c>
       <c r="Q118" s="24"/>
     </row>
-    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A119" s="24" t="s">
         <v>69</v>
       </c>
@@ -6458,7 +6455,7 @@
       </c>
       <c r="Q119" s="24"/>
     </row>
-    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A120" s="24" t="s">
         <v>69</v>
       </c>
@@ -6500,7 +6497,7 @@
       </c>
       <c r="Q120" s="24"/>
     </row>
-    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A121" s="24" t="s">
         <v>69</v>
       </c>
@@ -6542,7 +6539,7 @@
       </c>
       <c r="Q121" s="24"/>
     </row>
-    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A122" s="24" t="s">
         <v>69</v>
       </c>
@@ -6586,7 +6583,7 @@
       </c>
       <c r="Q122" s="24"/>
     </row>
-    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A123" s="28" t="s">
         <v>69</v>
       </c>
@@ -6633,7 +6630,7 @@
       </c>
       <c r="Q123" s="28"/>
     </row>
-    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A124" s="28" t="s">
         <v>69</v>
       </c>
@@ -6677,7 +6674,7 @@
       </c>
       <c r="Q124" s="28"/>
     </row>
-    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A125" s="28" t="s">
         <v>69</v>
       </c>
@@ -6721,7 +6718,7 @@
       </c>
       <c r="Q125" s="28"/>
     </row>
-    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A126" s="28" t="s">
         <v>69</v>
       </c>
@@ -6765,7 +6762,7 @@
       </c>
       <c r="Q126" s="28"/>
     </row>
-    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A127" s="28" t="s">
         <v>69</v>
       </c>
@@ -6809,7 +6806,7 @@
       </c>
       <c r="Q127" s="28"/>
     </row>
-    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A128" s="28" t="s">
         <v>69</v>
       </c>
@@ -6853,7 +6850,7 @@
       </c>
       <c r="Q128" s="28"/>
     </row>
-    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A129" s="28" t="s">
         <v>69</v>
       </c>
@@ -6897,7 +6894,7 @@
       </c>
       <c r="Q129" s="28"/>
     </row>
-    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A130" s="28" t="s">
         <v>69</v>
       </c>
@@ -6941,7 +6938,7 @@
       </c>
       <c r="Q130" s="28"/>
     </row>
-    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A131" s="28" t="s">
         <v>69</v>
       </c>
@@ -6985,7 +6982,7 @@
       </c>
       <c r="Q131" s="28"/>
     </row>
-    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A132" s="28" t="s">
         <v>69</v>
       </c>
@@ -7029,7 +7026,7 @@
       </c>
       <c r="Q132" s="28"/>
     </row>
-    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A133" s="28" t="s">
         <v>69</v>
       </c>
@@ -7073,7 +7070,7 @@
       </c>
       <c r="Q133" s="28"/>
     </row>
-    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A134" s="28" t="s">
         <v>69</v>
       </c>
@@ -7117,7 +7114,7 @@
       </c>
       <c r="Q134" s="28"/>
     </row>
-    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A135" s="28" t="s">
         <v>69</v>
       </c>
@@ -7161,7 +7158,7 @@
       </c>
       <c r="Q135" s="28"/>
     </row>
-    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A136" s="28" t="s">
         <v>69</v>
       </c>
@@ -7205,7 +7202,7 @@
       </c>
       <c r="Q136" s="28"/>
     </row>
-    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A137" s="28" t="s">
         <v>69</v>
       </c>
@@ -7249,7 +7246,7 @@
       </c>
       <c r="Q137" s="28"/>
     </row>
-    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A138" s="28" t="s">
         <v>69</v>
       </c>
@@ -7293,7 +7290,7 @@
       </c>
       <c r="Q138" s="28"/>
     </row>
-    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A139" s="28" t="s">
         <v>69</v>
       </c>
@@ -7337,7 +7334,7 @@
       </c>
       <c r="Q139" s="28"/>
     </row>
-    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A140" s="28" t="s">
         <v>69</v>
       </c>
@@ -7381,7 +7378,7 @@
       </c>
       <c r="Q140" s="28"/>
     </row>
-    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A141" s="28" t="s">
         <v>69</v>
       </c>
@@ -7425,7 +7422,7 @@
       </c>
       <c r="Q141" s="28"/>
     </row>
-    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A142" s="28" t="s">
         <v>69</v>
       </c>
@@ -7469,7 +7466,7 @@
       </c>
       <c r="Q142" s="28"/>
     </row>
-    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A143" s="28" t="s">
         <v>69</v>
       </c>
@@ -7513,7 +7510,7 @@
       </c>
       <c r="Q143" s="28"/>
     </row>
-    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A144" s="28" t="s">
         <v>69</v>
       </c>
@@ -7559,7 +7556,7 @@
       </c>
       <c r="Q144" s="28"/>
     </row>
-    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A145" s="32" t="s">
         <v>69</v>
       </c>
@@ -7604,7 +7601,7 @@
       </c>
       <c r="Q145" s="32"/>
     </row>
-    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A146" s="32" t="s">
         <v>69</v>
       </c>
@@ -7646,7 +7643,7 @@
       </c>
       <c r="Q146" s="32"/>
     </row>
-    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A147" s="32" t="s">
         <v>69</v>
       </c>
@@ -7690,7 +7687,7 @@
       </c>
       <c r="Q147" s="32"/>
     </row>
-    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
         <v>69</v>
       </c>
@@ -7735,7 +7732,7 @@
       </c>
       <c r="Q148" s="5"/>
     </row>
-    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A149" s="5" t="s">
         <v>69</v>
       </c>
@@ -7777,7 +7774,7 @@
       </c>
       <c r="Q149" s="5"/>
     </row>
-    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
         <v>69</v>
       </c>
@@ -7821,7 +7818,7 @@
       </c>
       <c r="Q150" s="5"/>
     </row>
-    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A151" s="9" t="s">
         <v>69</v>
       </c>
@@ -7868,7 +7865,7 @@
       </c>
       <c r="Q151" s="9"/>
     </row>
-    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A152" s="12" t="s">
         <v>69</v>
       </c>
@@ -7915,7 +7912,7 @@
       </c>
       <c r="Q152" s="12"/>
     </row>
-    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A153" s="16" t="s">
         <v>69</v>
       </c>
@@ -7962,7 +7959,7 @@
       </c>
       <c r="Q153" s="16"/>
     </row>
-    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A154" s="20" t="s">
         <v>70</v>
       </c>
@@ -8006,7 +8003,7 @@
       </c>
       <c r="Q154" s="20"/>
     </row>
-    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A155" s="20" t="s">
         <v>70</v>
       </c>
@@ -8048,7 +8045,7 @@
       </c>
       <c r="Q155" s="20"/>
     </row>
-    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A156" s="20" t="s">
         <v>70</v>
       </c>
@@ -8092,7 +8089,7 @@
       </c>
       <c r="Q156" s="20"/>
     </row>
-    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A157" s="24" t="s">
         <v>70</v>
       </c>
@@ -8136,7 +8133,7 @@
       </c>
       <c r="Q157" s="24"/>
     </row>
-    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A158" s="24" t="s">
         <v>70</v>
       </c>
@@ -8178,7 +8175,7 @@
       </c>
       <c r="Q158" s="24"/>
     </row>
-    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A159" s="24" t="s">
         <v>70</v>
       </c>
@@ -8222,7 +8219,7 @@
       </c>
       <c r="Q159" s="24"/>
     </row>
-    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A160" s="28" t="s">
         <v>70</v>
       </c>
@@ -8266,7 +8263,7 @@
       </c>
       <c r="Q160" s="31"/>
     </row>
-    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A161" s="28" t="s">
         <v>70</v>
       </c>
@@ -8308,7 +8305,7 @@
       </c>
       <c r="Q161" s="28"/>
     </row>
-    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A162" s="28" t="s">
         <v>70</v>
       </c>
@@ -8354,7 +8351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A163" s="32" t="s">
         <v>70</v>
       </c>
@@ -8398,7 +8395,7 @@
       </c>
       <c r="Q163" s="32"/>
     </row>
-    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A164" s="32" t="s">
         <v>70</v>
       </c>
@@ -8440,7 +8437,7 @@
       </c>
       <c r="Q164" s="32"/>
     </row>
-    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A165" s="32" t="s">
         <v>70</v>
       </c>
@@ -8484,7 +8481,7 @@
       </c>
       <c r="Q165" s="32"/>
     </row>
-    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
         <v>70</v>
       </c>
@@ -8528,7 +8525,7 @@
       </c>
       <c r="Q166" s="5"/>
     </row>
-    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A167" s="5" t="s">
         <v>70</v>
       </c>
@@ -8570,7 +8567,7 @@
       </c>
       <c r="Q167" s="5"/>
     </row>
-    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A168" s="5" t="s">
         <v>70</v>
       </c>
@@ -8616,7 +8613,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A169" s="9" t="s">
         <v>70</v>
       </c>
@@ -8660,7 +8657,7 @@
       </c>
       <c r="Q169" s="35"/>
     </row>
-    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A170" s="9" t="s">
         <v>70</v>
       </c>
@@ -8702,7 +8699,7 @@
       </c>
       <c r="Q170" s="9"/>
     </row>
-    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A171" s="9" t="s">
         <v>70</v>
       </c>
@@ -8744,7 +8741,7 @@
       </c>
       <c r="Q171" s="9"/>
     </row>
-    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A172" s="9" t="s">
         <v>70</v>
       </c>
@@ -8786,7 +8783,7 @@
       </c>
       <c r="Q172" s="9"/>
     </row>
-    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A173" s="9" t="s">
         <v>70</v>
       </c>
@@ -8830,7 +8827,7 @@
       </c>
       <c r="Q173" s="9"/>
     </row>
-    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A174" s="12" t="s">
         <v>70</v>
       </c>
@@ -8874,7 +8871,7 @@
       </c>
       <c r="Q174" s="14"/>
     </row>
-    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A175" s="12" t="s">
         <v>70</v>
       </c>
@@ -8916,7 +8913,7 @@
       </c>
       <c r="Q175" s="12"/>
     </row>
-    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A176" s="12" t="s">
         <v>70</v>
       </c>
@@ -8960,7 +8957,7 @@
       </c>
       <c r="Q176" s="12"/>
     </row>
-    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A177" s="16" t="s">
         <v>70</v>
       </c>
@@ -9006,7 +9003,7 @@
       </c>
       <c r="Q177" s="16"/>
     </row>
-    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A178" s="16" t="s">
         <v>70</v>
       </c>
@@ -9050,7 +9047,7 @@
       </c>
       <c r="Q178" s="19"/>
     </row>
-    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A179" s="16" t="s">
         <v>70</v>
       </c>
@@ -9094,7 +9091,7 @@
       </c>
       <c r="Q179" s="16"/>
     </row>
-    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A180" s="16" t="s">
         <v>70</v>
       </c>
@@ -9140,7 +9137,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A181" s="16" t="s">
         <v>70</v>
       </c>
@@ -9184,7 +9181,7 @@
       </c>
       <c r="Q181" s="16"/>
     </row>
-    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A182" s="16" t="s">
         <v>70</v>
       </c>
@@ -9228,7 +9225,7 @@
       </c>
       <c r="Q182" s="16"/>
     </row>
-    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A183" s="16" t="s">
         <v>70</v>
       </c>
@@ -9272,7 +9269,7 @@
       </c>
       <c r="Q183" s="16"/>
     </row>
-    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A184" s="16" t="s">
         <v>70</v>
       </c>
@@ -9316,7 +9313,7 @@
       </c>
       <c r="Q184" s="16"/>
     </row>
-    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A185" s="16" t="s">
         <v>70</v>
       </c>
@@ -9362,7 +9359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A186" s="16" t="s">
         <v>70</v>
       </c>
@@ -9406,7 +9403,7 @@
       </c>
       <c r="Q186" s="16"/>
     </row>
-    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A187" s="16" t="s">
         <v>70</v>
       </c>
@@ -9450,7 +9447,7 @@
       </c>
       <c r="Q187" s="16"/>
     </row>
-    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A188" s="16" t="s">
         <v>70</v>
       </c>
@@ -9494,7 +9491,7 @@
       </c>
       <c r="Q188" s="19"/>
     </row>
-    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A189" s="16" t="s">
         <v>70</v>
       </c>
@@ -9538,7 +9535,7 @@
       </c>
       <c r="Q189" s="16"/>
     </row>
-    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A190" s="16" t="s">
         <v>70</v>
       </c>
@@ -9582,7 +9579,7 @@
       </c>
       <c r="Q190" s="16"/>
     </row>
-    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A191" s="16" t="s">
         <v>70</v>
       </c>
@@ -9628,7 +9625,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A192" s="16" t="s">
         <v>70</v>
       </c>
@@ -9672,7 +9669,7 @@
       </c>
       <c r="Q192" s="16"/>
     </row>
-    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A193" s="16" t="s">
         <v>70</v>
       </c>
@@ -9716,7 +9713,7 @@
       </c>
       <c r="Q193" s="16"/>
     </row>
-    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A194" s="16" t="s">
         <v>70</v>
       </c>
@@ -9760,7 +9757,7 @@
       </c>
       <c r="Q194" s="16"/>
     </row>
-    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A195" s="16" t="s">
         <v>70</v>
       </c>
@@ -9804,7 +9801,7 @@
       </c>
       <c r="Q195" s="16"/>
     </row>
-    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A196" s="16" t="s">
         <v>70</v>
       </c>
@@ -9850,7 +9847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A197" s="16" t="s">
         <v>70</v>
       </c>
@@ -9894,7 +9891,7 @@
       </c>
       <c r="Q197" s="16"/>
     </row>
-    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A198" s="16" t="s">
         <v>70</v>
       </c>
@@ -9940,7 +9937,7 @@
       </c>
       <c r="Q198" s="19"/>
     </row>
-    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A199" s="20" t="s">
         <v>70</v>
       </c>
@@ -9986,7 +9983,7 @@
       </c>
       <c r="Q199" s="20"/>
     </row>
-    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A200" s="20" t="s">
         <v>70</v>
       </c>
@@ -10030,7 +10027,7 @@
       </c>
       <c r="Q200" s="23"/>
     </row>
-    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A201" s="20" t="s">
         <v>70</v>
       </c>
@@ -10074,7 +10071,7 @@
       </c>
       <c r="Q201" s="23"/>
     </row>
-    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A202" s="24" t="s">
         <v>70</v>
       </c>
@@ -10118,7 +10115,7 @@
       </c>
       <c r="Q202" s="24"/>
     </row>
-    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A203" s="24" t="s">
         <v>70</v>
       </c>
@@ -10160,7 +10157,7 @@
       </c>
       <c r="Q203" s="24"/>
     </row>
-    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A204" s="24" t="s">
         <v>70</v>
       </c>
@@ -10202,7 +10199,7 @@
       </c>
       <c r="Q204" s="24"/>
     </row>
-    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A205" s="24" t="s">
         <v>70</v>
       </c>
@@ -10246,7 +10243,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A206" s="24" t="s">
         <v>70</v>
       </c>
@@ -10288,7 +10285,7 @@
       </c>
       <c r="Q206" s="24"/>
     </row>
-    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A207" s="24" t="s">
         <v>70</v>
       </c>
@@ -10332,7 +10329,7 @@
       </c>
       <c r="Q207" s="24"/>
     </row>
-    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A208" s="28" t="s">
         <v>70</v>
       </c>
@@ -10376,7 +10373,7 @@
       </c>
       <c r="Q208" s="28"/>
     </row>
-    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A209" s="28" t="s">
         <v>70</v>
       </c>
@@ -10418,7 +10415,7 @@
       </c>
       <c r="Q209" s="28"/>
     </row>
-    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A210" s="28" t="s">
         <v>70</v>
       </c>
@@ -10462,7 +10459,7 @@
       </c>
       <c r="Q210" s="28"/>
     </row>
-    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A211" s="32" t="s">
         <v>70</v>
       </c>
@@ -10506,7 +10503,7 @@
       </c>
       <c r="Q211" s="32"/>
     </row>
-    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A212" s="32" t="s">
         <v>70</v>
       </c>
@@ -10548,7 +10545,7 @@
       </c>
       <c r="Q212" s="32"/>
     </row>
-    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A213" s="32" t="s">
         <v>70</v>
       </c>
@@ -10592,7 +10589,7 @@
       </c>
       <c r="Q213" s="36"/>
     </row>
-    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A214" s="5" t="s">
         <v>70</v>
       </c>
@@ -10636,7 +10633,7 @@
       </c>
       <c r="Q214" s="5"/>
     </row>
-    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A215" s="5" t="s">
         <v>70</v>
       </c>
@@ -10678,7 +10675,7 @@
       </c>
       <c r="Q215" s="5"/>
     </row>
-    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A216" s="5" t="s">
         <v>70</v>
       </c>
@@ -10722,7 +10719,7 @@
       </c>
       <c r="Q216" s="5"/>
     </row>
-    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A217" s="9" t="s">
         <v>70</v>
       </c>
@@ -10766,7 +10763,7 @@
       </c>
       <c r="Q217" s="9"/>
     </row>
-    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A218" s="9" t="s">
         <v>70</v>
       </c>
@@ -10808,7 +10805,7 @@
       </c>
       <c r="Q218" s="9"/>
     </row>
-    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A219" s="9" t="s">
         <v>70</v>
       </c>
@@ -10852,7 +10849,7 @@
       </c>
       <c r="Q219" s="9"/>
     </row>
-    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A220" s="12" t="s">
         <v>70</v>
       </c>
@@ -10898,7 +10895,7 @@
       </c>
       <c r="Q220" s="12"/>
     </row>
-    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A221" s="16" t="s">
         <v>70</v>
       </c>
@@ -10944,7 +10941,7 @@
       </c>
       <c r="Q221" s="16"/>
     </row>
-    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A222" s="16" t="s">
         <v>70</v>
       </c>
@@ -10988,7 +10985,7 @@
       </c>
       <c r="Q222" s="16"/>
     </row>
-    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A223" s="16" t="s">
         <v>70</v>
       </c>
@@ -11034,7 +11031,7 @@
       </c>
       <c r="Q223" s="16"/>
     </row>
-    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A224" s="20" t="s">
         <v>70</v>
       </c>
@@ -11080,7 +11077,7 @@
       </c>
       <c r="Q224" s="20"/>
     </row>
-    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A225" s="24" t="s">
         <v>70</v>
       </c>
@@ -11126,7 +11123,7 @@
       </c>
       <c r="Q225" s="24"/>
     </row>
-    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A226" s="28" t="s">
         <v>70</v>
       </c>
@@ -11172,7 +11169,7 @@
       </c>
       <c r="Q226" s="28"/>
     </row>
-    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A227" s="28" t="s">
         <v>70</v>
       </c>
@@ -11216,7 +11213,7 @@
       </c>
       <c r="Q227" s="28"/>
     </row>
-    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A228" s="28" t="s">
         <v>70</v>
       </c>
@@ -11262,7 +11259,7 @@
       </c>
       <c r="Q228" s="28"/>
     </row>
-    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A229" s="32" t="s">
         <v>70</v>
       </c>
@@ -11308,7 +11305,7 @@
       </c>
       <c r="Q229" s="32"/>
     </row>
-    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A230" s="5" t="s">
         <v>70</v>
       </c>
@@ -11367,19 +11364,19 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="46" t="s">
         <v>68</v>
       </c>
@@ -11402,7 +11399,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11419,7 +11416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11442,7 +11439,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11465,7 +11462,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11482,7 +11479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11499,7 +11496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11522,7 +11519,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11539,7 +11536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11562,7 +11559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11579,7 +11576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11602,7 +11599,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11619,7 +11616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11636,7 +11633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11653,7 +11650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11670,7 +11667,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11687,7 +11684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11704,7 +11701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11721,7 +11718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -11738,7 +11735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -11755,7 +11752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -11772,7 +11769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -11807,9 +11804,9 @@
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
         <v>55</v>
       </c>
@@ -11826,7 +11823,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -11843,7 +11840,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -11860,7 +11857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -11877,7 +11874,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -11894,7 +11891,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -11911,7 +11908,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -11928,7 +11925,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -11945,7 +11942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -11962,7 +11959,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -11979,7 +11976,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -11996,7 +11993,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -12013,7 +12010,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -12030,7 +12027,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -12055,23 +12052,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" style="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.77734375" style="47"/>
-    <col min="6" max="6" width="10.109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="47"/>
+    <col min="2" max="2" width="6.6328125" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.81640625" style="47"/>
+    <col min="6" max="6" width="10.08984375" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
         <v>74</v>
       </c>
@@ -12091,7 +12088,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="48">
         <v>1</v>
       </c>
@@ -12111,7 +12108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="48">
         <v>2</v>
       </c>
@@ -12131,7 +12128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="48">
         <v>3</v>
       </c>
@@ -12151,7 +12148,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="48">
         <v>4</v>
       </c>
@@ -12171,7 +12168,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="49">
         <v>6</v>
       </c>
@@ -12191,7 +12188,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="49">
         <v>7</v>
       </c>
@@ -12211,7 +12208,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="49">
         <v>8</v>
       </c>
@@ -12231,7 +12228,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="49">
         <v>9</v>
       </c>
@@ -12251,7 +12248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="49">
         <v>10</v>
       </c>
@@ -12271,7 +12268,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="49">
         <v>11</v>
       </c>
@@ -12291,7 +12288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="49">
         <v>12</v>
       </c>
@@ -12311,7 +12308,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="49">
         <v>13</v>
       </c>
@@ -12319,19 +12316,19 @@
         <v>70</v>
       </c>
       <c r="C13" s="49">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="49">
         <v>5</v>
       </c>
       <c r="E13" s="49">
-        <v>225</v>
+        <v>150</v>
       </c>
       <c r="F13" s="49" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="49">
         <v>14</v>
       </c>
@@ -12351,7 +12348,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="49">
         <v>15</v>
       </c>
@@ -12371,7 +12368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="49">
         <v>16</v>
       </c>
@@ -12391,7 +12388,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="49">
         <v>17</v>
       </c>
@@ -12411,7 +12408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="49">
         <v>18</v>
       </c>
@@ -12431,7 +12428,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="49">
         <v>19</v>
       </c>
@@ -12451,7 +12448,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="49">
         <v>20</v>
       </c>
@@ -12471,7 +12468,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="49">
         <v>21</v>
       </c>
@@ -12491,7 +12488,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="49">
         <v>22</v>
       </c>
@@ -12511,7 +12508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="49">
         <v>23</v>
       </c>
@@ -12531,7 +12528,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="49">
         <v>24</v>
       </c>
@@ -12551,7 +12548,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="49">
         <v>25</v>
       </c>
@@ -12571,7 +12568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="49">
         <v>26</v>
       </c>
@@ -12591,7 +12588,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="49">
         <v>27</v>
       </c>
@@ -12611,7 +12608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="49">
         <v>28</v>
       </c>
@@ -12631,7 +12628,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="49">
         <v>29</v>
       </c>
@@ -12651,7 +12648,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="49">
         <v>30</v>
       </c>
@@ -12671,7 +12668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="49">
         <v>31</v>
       </c>
@@ -12691,7 +12688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="49">
         <v>32</v>
       </c>
@@ -12711,7 +12708,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="49">
         <v>33</v>
       </c>
@@ -12731,7 +12728,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="49">
         <v>34</v>
       </c>
@@ -12751,7 +12748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="49">
         <v>35</v>
       </c>
@@ -12771,7 +12768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="49">
         <v>36</v>
       </c>
@@ -12791,7 +12788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="49">
         <v>37</v>
       </c>
@@ -12799,7 +12796,7 @@
         <v>70</v>
       </c>
       <c r="C37" s="49">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D37" s="49">
         <v>18</v>
@@ -12811,7 +12808,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="49">
         <v>38</v>
       </c>
@@ -12831,7 +12828,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="49">
         <v>39</v>
       </c>
@@ -12851,7 +12848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="49">
         <v>40</v>
       </c>
@@ -12871,7 +12868,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="49">
         <v>41</v>
       </c>
@@ -12891,7 +12888,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="49">
         <v>42</v>
       </c>
@@ -12911,7 +12908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="49">
         <v>43</v>
       </c>
@@ -12931,7 +12928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="49">
         <v>44</v>
       </c>
@@ -12949,86 +12946,6 @@
       </c>
       <c r="F44" s="49" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="49">
-        <v>45</v>
-      </c>
-      <c r="B45" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" s="49">
-        <v>75</v>
-      </c>
-      <c r="D45" s="49">
-        <v>11</v>
-      </c>
-      <c r="E45" s="49">
-        <v>200</v>
-      </c>
-      <c r="F45" s="49" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="49">
-        <v>46</v>
-      </c>
-      <c r="B46" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="49">
-        <v>73</v>
-      </c>
-      <c r="D46" s="49">
-        <v>19</v>
-      </c>
-      <c r="E46" s="49">
-        <v>200</v>
-      </c>
-      <c r="F46" s="49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="49">
-        <v>47</v>
-      </c>
-      <c r="B47" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" s="49">
-        <v>71</v>
-      </c>
-      <c r="D47" s="49">
-        <v>19</v>
-      </c>
-      <c r="E47" s="49">
-        <v>200</v>
-      </c>
-      <c r="F47" s="49" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="49">
-        <v>48</v>
-      </c>
-      <c r="B48" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C48" s="49">
-        <v>69</v>
-      </c>
-      <c r="D48" s="49">
-        <v>5</v>
-      </c>
-      <c r="E48" s="49">
-        <v>200</v>
-      </c>
-      <c r="F48" s="49" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved Beacon farther from Yard.
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan94\Documents\Coding\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="6840" windowWidth="33240" windowHeight="11560" activeTab="5"/>
+    <workbookView xWindow="1296" yWindow="6840" windowWidth="33240" windowHeight="11556" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LINE" sheetId="9" r:id="rId1"/>
@@ -268,7 +268,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -814,19 +814,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -845,9 +845,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>48</v>
       </c>
@@ -855,7 +855,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -871,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -879,7 +879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -887,7 +887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -895,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -903,7 +903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -911,7 +911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -919,7 +919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -927,7 +927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -935,7 +935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -943,7 +943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -951,7 +951,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -959,7 +959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -967,7 +967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -975,7 +975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -983,7 +983,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -991,7 +991,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -999,7 +999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -1257,34 +1257,34 @@
   <dimension ref="A1:Q230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I198" sqref="I198:I200"/>
+      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I230" sqref="I230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.81640625" style="1"/>
+    <col min="14" max="14" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>69</v>
       </c>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>69</v>
       </c>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>69</v>
       </c>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>69</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>69</v>
       </c>
@@ -1554,7 +1554,7 @@
       </c>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>69</v>
       </c>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>69</v>
       </c>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>69</v>
       </c>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="Q9" s="12"/>
     </row>
-    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>69</v>
       </c>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>69</v>
       </c>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="Q12" s="12"/>
     </row>
-    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>69</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>69</v>
       </c>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="Q14" s="16"/>
     </row>
-    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>69</v>
       </c>
@@ -1944,7 +1944,7 @@
       </c>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>69</v>
       </c>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>69</v>
       </c>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="Q17" s="19"/>
     </row>
-    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>69</v>
       </c>
@@ -2074,7 +2074,7 @@
       </c>
       <c r="Q18" s="20"/>
     </row>
-    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>69</v>
       </c>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="Q19" s="20"/>
     </row>
-    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>69</v>
       </c>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="Q20" s="23"/>
     </row>
-    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>69</v>
       </c>
@@ -2204,7 +2204,7 @@
       </c>
       <c r="Q21" s="20"/>
     </row>
-    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>69</v>
       </c>
@@ -2248,7 +2248,7 @@
       </c>
       <c r="Q22" s="24"/>
     </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>69</v>
       </c>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="Q23" s="27"/>
     </row>
-    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>69</v>
       </c>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="Q24" s="24"/>
     </row>
-    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>69</v>
       </c>
@@ -2374,7 +2374,7 @@
       </c>
       <c r="Q25" s="24"/>
     </row>
-    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>69</v>
       </c>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="Q26" s="24"/>
     </row>
-    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>69</v>
       </c>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="Q27" s="24"/>
     </row>
-    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>69</v>
       </c>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="Q28" s="24"/>
     </row>
-    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>69</v>
       </c>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="Q29" s="24"/>
     </row>
-    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
         <v>69</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
         <v>69</v>
       </c>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="Q31" s="28"/>
     </row>
-    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
         <v>69</v>
       </c>
@@ -2675,7 +2675,7 @@
       </c>
       <c r="Q32" s="31"/>
     </row>
-    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
         <v>69</v>
       </c>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="Q33" s="28"/>
     </row>
-    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="32" t="s">
         <v>69</v>
       </c>
@@ -2764,7 +2764,7 @@
       </c>
       <c r="Q34" s="32"/>
     </row>
-    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="32" t="s">
         <v>69</v>
       </c>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="Q35" s="32"/>
     </row>
-    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="32" t="s">
         <v>69</v>
       </c>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="Q36" s="32"/>
     </row>
-    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>69</v>
       </c>
@@ -2897,7 +2897,7 @@
       </c>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>69</v>
       </c>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>69</v>
       </c>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>69</v>
       </c>
@@ -3029,7 +3029,7 @@
       </c>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>69</v>
       </c>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>69</v>
       </c>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>69</v>
       </c>
@@ -3161,7 +3161,7 @@
       </c>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>69</v>
       </c>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>69</v>
       </c>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>69</v>
       </c>
@@ -3293,7 +3293,7 @@
       </c>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>69</v>
       </c>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="Q47" s="5"/>
     </row>
-    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>69</v>
       </c>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="Q48" s="5"/>
     </row>
-    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>69</v>
       </c>
@@ -3425,7 +3425,7 @@
       </c>
       <c r="Q49" s="8"/>
     </row>
-    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>69</v>
       </c>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="Q50" s="5"/>
     </row>
-    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>69</v>
       </c>
@@ -3513,7 +3513,7 @@
       </c>
       <c r="Q51" s="5"/>
     </row>
-    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>69</v>
       </c>
@@ -3557,7 +3557,7 @@
       </c>
       <c r="Q52" s="5"/>
     </row>
-    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>69</v>
       </c>
@@ -3601,7 +3601,7 @@
       </c>
       <c r="Q53" s="5"/>
     </row>
-    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>69</v>
       </c>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="Q54" s="5"/>
     </row>
-    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>69</v>
       </c>
@@ -3689,7 +3689,7 @@
       </c>
       <c r="Q55" s="5"/>
     </row>
-    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>69</v>
       </c>
@@ -3733,7 +3733,7 @@
       </c>
       <c r="Q56" s="5"/>
     </row>
-    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>69</v>
       </c>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="Q57" s="5"/>
     </row>
-    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>69</v>
       </c>
@@ -3823,7 +3823,7 @@
       </c>
       <c r="Q58" s="8"/>
     </row>
-    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
         <v>69</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>69</v>
       </c>
@@ -3912,7 +3912,7 @@
       </c>
       <c r="Q60" s="9"/>
     </row>
-    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>69</v>
       </c>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="Q61" s="9"/>
     </row>
-    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>69</v>
       </c>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="Q62" s="9"/>
     </row>
-    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>69</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
         <v>69</v>
       </c>
@@ -4087,7 +4087,7 @@
       </c>
       <c r="Q64" s="12"/>
     </row>
-    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
         <v>69</v>
       </c>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="Q65" s="12"/>
     </row>
-    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
         <v>69</v>
       </c>
@@ -4171,7 +4171,7 @@
       </c>
       <c r="Q66" s="14"/>
     </row>
-    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
         <v>69</v>
       </c>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="Q67" s="12"/>
     </row>
-    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
         <v>69</v>
       </c>
@@ -4255,7 +4255,7 @@
       </c>
       <c r="Q68" s="12"/>
     </row>
-    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
         <v>69</v>
       </c>
@@ -4299,7 +4299,7 @@
       </c>
       <c r="Q69" s="12"/>
     </row>
-    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
         <v>69</v>
       </c>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="Q70" s="16"/>
     </row>
-    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
         <v>69</v>
       </c>
@@ -4386,7 +4386,7 @@
       </c>
       <c r="Q71" s="16"/>
     </row>
-    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
         <v>69</v>
       </c>
@@ -4428,7 +4428,7 @@
       </c>
       <c r="Q72" s="16"/>
     </row>
-    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
         <v>69</v>
       </c>
@@ -4470,7 +4470,7 @@
       </c>
       <c r="Q73" s="16"/>
     </row>
-    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
         <v>69</v>
       </c>
@@ -4514,7 +4514,7 @@
       </c>
       <c r="Q74" s="19"/>
     </row>
-    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="20" t="s">
         <v>69</v>
       </c>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="Q75" s="20"/>
     </row>
-    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="20" t="s">
         <v>69</v>
       </c>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="Q76" s="20"/>
     </row>
-    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="20" t="s">
         <v>69</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="24" t="s">
         <v>69</v>
       </c>
@@ -4691,7 +4691,7 @@
       </c>
       <c r="Q78" s="27"/>
     </row>
-    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="24" t="s">
         <v>69</v>
       </c>
@@ -4733,7 +4733,7 @@
       </c>
       <c r="Q79" s="24"/>
     </row>
-    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="24" t="s">
         <v>69</v>
       </c>
@@ -4775,7 +4775,7 @@
       </c>
       <c r="Q80" s="24"/>
     </row>
-    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
         <v>69</v>
       </c>
@@ -4817,7 +4817,7 @@
       </c>
       <c r="Q81" s="24"/>
     </row>
-    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="24" t="s">
         <v>69</v>
       </c>
@@ -4859,7 +4859,7 @@
       </c>
       <c r="Q82" s="24"/>
     </row>
-    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="24" t="s">
         <v>69</v>
       </c>
@@ -4901,7 +4901,7 @@
       </c>
       <c r="Q83" s="24"/>
     </row>
-    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="24" t="s">
         <v>69</v>
       </c>
@@ -4943,7 +4943,7 @@
       </c>
       <c r="Q84" s="24"/>
     </row>
-    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="24" t="s">
         <v>69</v>
       </c>
@@ -4985,7 +4985,7 @@
       </c>
       <c r="Q85" s="24"/>
     </row>
-    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="24" t="s">
         <v>69</v>
       </c>
@@ -5029,7 +5029,7 @@
       </c>
       <c r="Q86" s="24"/>
     </row>
-    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="28" t="s">
         <v>69</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="28" t="s">
         <v>69</v>
       </c>
@@ -5118,7 +5118,7 @@
       </c>
       <c r="Q88" s="28"/>
     </row>
-    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="28" t="s">
         <v>69</v>
       </c>
@@ -5162,7 +5162,7 @@
       </c>
       <c r="Q89" s="31"/>
     </row>
-    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="32" t="s">
         <v>69</v>
       </c>
@@ -5207,7 +5207,7 @@
       </c>
       <c r="Q90" s="32"/>
     </row>
-    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="32" t="s">
         <v>69</v>
       </c>
@@ -5249,7 +5249,7 @@
       </c>
       <c r="Q91" s="32"/>
     </row>
-    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="32" t="s">
         <v>69</v>
       </c>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="Q92" s="32"/>
     </row>
-    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="32" t="s">
         <v>69</v>
       </c>
@@ -5333,7 +5333,7 @@
       </c>
       <c r="Q93" s="32"/>
     </row>
-    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="32" t="s">
         <v>69</v>
       </c>
@@ -5375,7 +5375,7 @@
       </c>
       <c r="Q94" s="32"/>
     </row>
-    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="32" t="s">
         <v>69</v>
       </c>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="Q95" s="32"/>
     </row>
-    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="32" t="s">
         <v>69</v>
       </c>
@@ -5459,7 +5459,7 @@
       </c>
       <c r="Q96" s="32"/>
     </row>
-    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="32" t="s">
         <v>69</v>
       </c>
@@ -5501,7 +5501,7 @@
       </c>
       <c r="Q97" s="36"/>
     </row>
-    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="32" t="s">
         <v>69</v>
       </c>
@@ -5545,7 +5545,7 @@
       </c>
       <c r="Q98" s="32"/>
     </row>
-    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>69</v>
       </c>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="Q99" s="5"/>
     </row>
-    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>69</v>
       </c>
@@ -5632,7 +5632,7 @@
       </c>
       <c r="Q100" s="5"/>
     </row>
-    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>69</v>
       </c>
@@ -5676,7 +5676,7 @@
       </c>
       <c r="Q101" s="5"/>
     </row>
-    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
         <v>69</v>
       </c>
@@ -5723,7 +5723,7 @@
       </c>
       <c r="Q102" s="9"/>
     </row>
-    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
         <v>69</v>
       </c>
@@ -5768,7 +5768,7 @@
       </c>
       <c r="Q103" s="12"/>
     </row>
-    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
         <v>69</v>
       </c>
@@ -5810,7 +5810,7 @@
       </c>
       <c r="Q104" s="12"/>
     </row>
-    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
         <v>69</v>
       </c>
@@ -5854,7 +5854,7 @@
       </c>
       <c r="Q105" s="12"/>
     </row>
-    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="16" t="s">
         <v>69</v>
       </c>
@@ -5899,7 +5899,7 @@
       </c>
       <c r="Q106" s="19"/>
     </row>
-    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="16" t="s">
         <v>69</v>
       </c>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="Q107" s="16"/>
     </row>
-    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="16" t="s">
         <v>69</v>
       </c>
@@ -5983,7 +5983,7 @@
       </c>
       <c r="Q108" s="16"/>
     </row>
-    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="16" t="s">
         <v>69</v>
       </c>
@@ -6025,7 +6025,7 @@
       </c>
       <c r="Q109" s="16"/>
     </row>
-    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="16" t="s">
         <v>69</v>
       </c>
@@ -6069,7 +6069,7 @@
       </c>
       <c r="Q110" s="16"/>
     </row>
-    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="20" t="s">
         <v>69</v>
       </c>
@@ -6114,7 +6114,7 @@
       </c>
       <c r="Q111" s="20"/>
     </row>
-    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="20" t="s">
         <v>69</v>
       </c>
@@ -6156,7 +6156,7 @@
       </c>
       <c r="Q112" s="20"/>
     </row>
-    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="20" t="s">
         <v>69</v>
       </c>
@@ -6198,7 +6198,7 @@
       </c>
       <c r="Q113" s="20"/>
     </row>
-    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="20" t="s">
         <v>69</v>
       </c>
@@ -6240,7 +6240,7 @@
       </c>
       <c r="Q114" s="20"/>
     </row>
-    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="20" t="s">
         <v>69</v>
       </c>
@@ -6282,7 +6282,7 @@
       </c>
       <c r="Q115" s="23"/>
     </row>
-    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="20" t="s">
         <v>69</v>
       </c>
@@ -6324,7 +6324,7 @@
       </c>
       <c r="Q116" s="20"/>
     </row>
-    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="20" t="s">
         <v>69</v>
       </c>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="Q117" s="20"/>
     </row>
-    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="24" t="s">
         <v>69</v>
       </c>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="Q118" s="24"/>
     </row>
-    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="24" t="s">
         <v>69</v>
       </c>
@@ -6455,7 +6455,7 @@
       </c>
       <c r="Q119" s="24"/>
     </row>
-    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="24" t="s">
         <v>69</v>
       </c>
@@ -6497,7 +6497,7 @@
       </c>
       <c r="Q120" s="24"/>
     </row>
-    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="24" t="s">
         <v>69</v>
       </c>
@@ -6539,7 +6539,7 @@
       </c>
       <c r="Q121" s="24"/>
     </row>
-    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="24" t="s">
         <v>69</v>
       </c>
@@ -6583,7 +6583,7 @@
       </c>
       <c r="Q122" s="24"/>
     </row>
-    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="28" t="s">
         <v>69</v>
       </c>
@@ -6630,7 +6630,7 @@
       </c>
       <c r="Q123" s="28"/>
     </row>
-    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="28" t="s">
         <v>69</v>
       </c>
@@ -6674,7 +6674,7 @@
       </c>
       <c r="Q124" s="28"/>
     </row>
-    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="28" t="s">
         <v>69</v>
       </c>
@@ -6718,7 +6718,7 @@
       </c>
       <c r="Q125" s="28"/>
     </row>
-    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="28" t="s">
         <v>69</v>
       </c>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="Q126" s="28"/>
     </row>
-    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="28" t="s">
         <v>69</v>
       </c>
@@ -6806,7 +6806,7 @@
       </c>
       <c r="Q127" s="28"/>
     </row>
-    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="28" t="s">
         <v>69</v>
       </c>
@@ -6850,7 +6850,7 @@
       </c>
       <c r="Q128" s="28"/>
     </row>
-    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="28" t="s">
         <v>69</v>
       </c>
@@ -6894,7 +6894,7 @@
       </c>
       <c r="Q129" s="28"/>
     </row>
-    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="28" t="s">
         <v>69</v>
       </c>
@@ -6938,7 +6938,7 @@
       </c>
       <c r="Q130" s="28"/>
     </row>
-    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="28" t="s">
         <v>69</v>
       </c>
@@ -6982,7 +6982,7 @@
       </c>
       <c r="Q131" s="28"/>
     </row>
-    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="28" t="s">
         <v>69</v>
       </c>
@@ -7026,7 +7026,7 @@
       </c>
       <c r="Q132" s="28"/>
     </row>
-    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="28" t="s">
         <v>69</v>
       </c>
@@ -7070,7 +7070,7 @@
       </c>
       <c r="Q133" s="28"/>
     </row>
-    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="28" t="s">
         <v>69</v>
       </c>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="Q134" s="28"/>
     </row>
-    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="28" t="s">
         <v>69</v>
       </c>
@@ -7158,7 +7158,7 @@
       </c>
       <c r="Q135" s="28"/>
     </row>
-    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="28" t="s">
         <v>69</v>
       </c>
@@ -7202,7 +7202,7 @@
       </c>
       <c r="Q136" s="28"/>
     </row>
-    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="28" t="s">
         <v>69</v>
       </c>
@@ -7246,7 +7246,7 @@
       </c>
       <c r="Q137" s="28"/>
     </row>
-    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="28" t="s">
         <v>69</v>
       </c>
@@ -7290,7 +7290,7 @@
       </c>
       <c r="Q138" s="28"/>
     </row>
-    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="28" t="s">
         <v>69</v>
       </c>
@@ -7334,7 +7334,7 @@
       </c>
       <c r="Q139" s="28"/>
     </row>
-    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="28" t="s">
         <v>69</v>
       </c>
@@ -7378,7 +7378,7 @@
       </c>
       <c r="Q140" s="28"/>
     </row>
-    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="28" t="s">
         <v>69</v>
       </c>
@@ -7422,7 +7422,7 @@
       </c>
       <c r="Q141" s="28"/>
     </row>
-    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="28" t="s">
         <v>69</v>
       </c>
@@ -7466,7 +7466,7 @@
       </c>
       <c r="Q142" s="28"/>
     </row>
-    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="28" t="s">
         <v>69</v>
       </c>
@@ -7510,7 +7510,7 @@
       </c>
       <c r="Q143" s="28"/>
     </row>
-    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="28" t="s">
         <v>69</v>
       </c>
@@ -7556,7 +7556,7 @@
       </c>
       <c r="Q144" s="28"/>
     </row>
-    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="32" t="s">
         <v>69</v>
       </c>
@@ -7601,7 +7601,7 @@
       </c>
       <c r="Q145" s="32"/>
     </row>
-    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="32" t="s">
         <v>69</v>
       </c>
@@ -7643,7 +7643,7 @@
       </c>
       <c r="Q146" s="32"/>
     </row>
-    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="32" t="s">
         <v>69</v>
       </c>
@@ -7687,7 +7687,7 @@
       </c>
       <c r="Q147" s="32"/>
     </row>
-    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>69</v>
       </c>
@@ -7732,7 +7732,7 @@
       </c>
       <c r="Q148" s="5"/>
     </row>
-    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>69</v>
       </c>
@@ -7774,7 +7774,7 @@
       </c>
       <c r="Q149" s="5"/>
     </row>
-    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>69</v>
       </c>
@@ -7818,7 +7818,7 @@
       </c>
       <c r="Q150" s="5"/>
     </row>
-    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="9" t="s">
         <v>69</v>
       </c>
@@ -7865,7 +7865,7 @@
       </c>
       <c r="Q151" s="9"/>
     </row>
-    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="12" t="s">
         <v>69</v>
       </c>
@@ -7912,7 +7912,7 @@
       </c>
       <c r="Q152" s="12"/>
     </row>
-    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="16" t="s">
         <v>69</v>
       </c>
@@ -7959,7 +7959,7 @@
       </c>
       <c r="Q153" s="16"/>
     </row>
-    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="20" t="s">
         <v>70</v>
       </c>
@@ -8003,7 +8003,7 @@
       </c>
       <c r="Q154" s="20"/>
     </row>
-    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="20" t="s">
         <v>70</v>
       </c>
@@ -8045,7 +8045,7 @@
       </c>
       <c r="Q155" s="20"/>
     </row>
-    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="20" t="s">
         <v>70</v>
       </c>
@@ -8089,7 +8089,7 @@
       </c>
       <c r="Q156" s="20"/>
     </row>
-    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="24" t="s">
         <v>70</v>
       </c>
@@ -8133,7 +8133,7 @@
       </c>
       <c r="Q157" s="24"/>
     </row>
-    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
         <v>70</v>
       </c>
@@ -8175,7 +8175,7 @@
       </c>
       <c r="Q158" s="24"/>
     </row>
-    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="24" t="s">
         <v>70</v>
       </c>
@@ -8219,7 +8219,7 @@
       </c>
       <c r="Q159" s="24"/>
     </row>
-    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="28" t="s">
         <v>70</v>
       </c>
@@ -8263,7 +8263,7 @@
       </c>
       <c r="Q160" s="31"/>
     </row>
-    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="28" t="s">
         <v>70</v>
       </c>
@@ -8305,7 +8305,7 @@
       </c>
       <c r="Q161" s="28"/>
     </row>
-    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="28" t="s">
         <v>70</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="32" t="s">
         <v>70</v>
       </c>
@@ -8395,7 +8395,7 @@
       </c>
       <c r="Q163" s="32"/>
     </row>
-    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="32" t="s">
         <v>70</v>
       </c>
@@ -8437,7 +8437,7 @@
       </c>
       <c r="Q164" s="32"/>
     </row>
-    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="32" t="s">
         <v>70</v>
       </c>
@@ -8481,7 +8481,7 @@
       </c>
       <c r="Q165" s="32"/>
     </row>
-    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>70</v>
       </c>
@@ -8525,7 +8525,7 @@
       </c>
       <c r="Q166" s="5"/>
     </row>
-    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>70</v>
       </c>
@@ -8567,7 +8567,7 @@
       </c>
       <c r="Q167" s="5"/>
     </row>
-    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>70</v>
       </c>
@@ -8613,7 +8613,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="9" t="s">
         <v>70</v>
       </c>
@@ -8657,7 +8657,7 @@
       </c>
       <c r="Q169" s="35"/>
     </row>
-    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="9" t="s">
         <v>70</v>
       </c>
@@ -8699,7 +8699,7 @@
       </c>
       <c r="Q170" s="9"/>
     </row>
-    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A171" s="9" t="s">
         <v>70</v>
       </c>
@@ -8741,7 +8741,7 @@
       </c>
       <c r="Q171" s="9"/>
     </row>
-    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="9" t="s">
         <v>70</v>
       </c>
@@ -8783,7 +8783,7 @@
       </c>
       <c r="Q172" s="9"/>
     </row>
-    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="9" t="s">
         <v>70</v>
       </c>
@@ -8827,7 +8827,7 @@
       </c>
       <c r="Q173" s="9"/>
     </row>
-    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
         <v>70</v>
       </c>
@@ -8871,7 +8871,7 @@
       </c>
       <c r="Q174" s="14"/>
     </row>
-    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
         <v>70</v>
       </c>
@@ -8913,7 +8913,7 @@
       </c>
       <c r="Q175" s="12"/>
     </row>
-    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
         <v>70</v>
       </c>
@@ -8957,7 +8957,7 @@
       </c>
       <c r="Q176" s="12"/>
     </row>
-    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A177" s="16" t="s">
         <v>70</v>
       </c>
@@ -9003,7 +9003,7 @@
       </c>
       <c r="Q177" s="16"/>
     </row>
-    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="16" t="s">
         <v>70</v>
       </c>
@@ -9047,7 +9047,7 @@
       </c>
       <c r="Q178" s="19"/>
     </row>
-    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="16" t="s">
         <v>70</v>
       </c>
@@ -9091,7 +9091,7 @@
       </c>
       <c r="Q179" s="16"/>
     </row>
-    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="16" t="s">
         <v>70</v>
       </c>
@@ -9137,7 +9137,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A181" s="16" t="s">
         <v>70</v>
       </c>
@@ -9181,7 +9181,7 @@
       </c>
       <c r="Q181" s="16"/>
     </row>
-    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182" s="16" t="s">
         <v>70</v>
       </c>
@@ -9225,7 +9225,7 @@
       </c>
       <c r="Q182" s="16"/>
     </row>
-    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="16" t="s">
         <v>70</v>
       </c>
@@ -9269,7 +9269,7 @@
       </c>
       <c r="Q183" s="16"/>
     </row>
-    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="16" t="s">
         <v>70</v>
       </c>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="Q184" s="16"/>
     </row>
-    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="16" t="s">
         <v>70</v>
       </c>
@@ -9359,7 +9359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A186" s="16" t="s">
         <v>70</v>
       </c>
@@ -9403,7 +9403,7 @@
       </c>
       <c r="Q186" s="16"/>
     </row>
-    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="16" t="s">
         <v>70</v>
       </c>
@@ -9447,7 +9447,7 @@
       </c>
       <c r="Q187" s="16"/>
     </row>
-    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="16" t="s">
         <v>70</v>
       </c>
@@ -9491,7 +9491,7 @@
       </c>
       <c r="Q188" s="19"/>
     </row>
-    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="16" t="s">
         <v>70</v>
       </c>
@@ -9535,7 +9535,7 @@
       </c>
       <c r="Q189" s="16"/>
     </row>
-    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="16" t="s">
         <v>70</v>
       </c>
@@ -9579,7 +9579,7 @@
       </c>
       <c r="Q190" s="16"/>
     </row>
-    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="16" t="s">
         <v>70</v>
       </c>
@@ -9625,7 +9625,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="16" t="s">
         <v>70</v>
       </c>
@@ -9669,7 +9669,7 @@
       </c>
       <c r="Q192" s="16"/>
     </row>
-    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="16" t="s">
         <v>70</v>
       </c>
@@ -9713,7 +9713,7 @@
       </c>
       <c r="Q193" s="16"/>
     </row>
-    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="16" t="s">
         <v>70</v>
       </c>
@@ -9757,7 +9757,7 @@
       </c>
       <c r="Q194" s="16"/>
     </row>
-    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A195" s="16" t="s">
         <v>70</v>
       </c>
@@ -9801,7 +9801,7 @@
       </c>
       <c r="Q195" s="16"/>
     </row>
-    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="16" t="s">
         <v>70</v>
       </c>
@@ -9847,7 +9847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="16" t="s">
         <v>70</v>
       </c>
@@ -9891,7 +9891,7 @@
       </c>
       <c r="Q197" s="16"/>
     </row>
-    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="16" t="s">
         <v>70</v>
       </c>
@@ -9937,7 +9937,7 @@
       </c>
       <c r="Q198" s="19"/>
     </row>
-    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A199" s="20" t="s">
         <v>70</v>
       </c>
@@ -9983,7 +9983,7 @@
       </c>
       <c r="Q199" s="20"/>
     </row>
-    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A200" s="20" t="s">
         <v>70</v>
       </c>
@@ -10027,7 +10027,7 @@
       </c>
       <c r="Q200" s="23"/>
     </row>
-    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A201" s="20" t="s">
         <v>70</v>
       </c>
@@ -10071,7 +10071,7 @@
       </c>
       <c r="Q201" s="23"/>
     </row>
-    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="24" t="s">
         <v>70</v>
       </c>
@@ -10115,7 +10115,7 @@
       </c>
       <c r="Q202" s="24"/>
     </row>
-    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A203" s="24" t="s">
         <v>70</v>
       </c>
@@ -10157,7 +10157,7 @@
       </c>
       <c r="Q203" s="24"/>
     </row>
-    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A204" s="24" t="s">
         <v>70</v>
       </c>
@@ -10199,7 +10199,7 @@
       </c>
       <c r="Q204" s="24"/>
     </row>
-    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="24" t="s">
         <v>70</v>
       </c>
@@ -10243,7 +10243,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A206" s="24" t="s">
         <v>70</v>
       </c>
@@ -10285,7 +10285,7 @@
       </c>
       <c r="Q206" s="24"/>
     </row>
-    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207" s="24" t="s">
         <v>70</v>
       </c>
@@ -10329,7 +10329,7 @@
       </c>
       <c r="Q207" s="24"/>
     </row>
-    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="28" t="s">
         <v>70</v>
       </c>
@@ -10373,7 +10373,7 @@
       </c>
       <c r="Q208" s="28"/>
     </row>
-    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="28" t="s">
         <v>70</v>
       </c>
@@ -10415,7 +10415,7 @@
       </c>
       <c r="Q209" s="28"/>
     </row>
-    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="28" t="s">
         <v>70</v>
       </c>
@@ -10459,7 +10459,7 @@
       </c>
       <c r="Q210" s="28"/>
     </row>
-    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="32" t="s">
         <v>70</v>
       </c>
@@ -10503,7 +10503,7 @@
       </c>
       <c r="Q211" s="32"/>
     </row>
-    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="32" t="s">
         <v>70</v>
       </c>
@@ -10545,7 +10545,7 @@
       </c>
       <c r="Q212" s="32"/>
     </row>
-    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="32" t="s">
         <v>70</v>
       </c>
@@ -10589,7 +10589,7 @@
       </c>
       <c r="Q213" s="36"/>
     </row>
-    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
         <v>70</v>
       </c>
@@ -10633,7 +10633,7 @@
       </c>
       <c r="Q214" s="5"/>
     </row>
-    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
         <v>70</v>
       </c>
@@ -10675,7 +10675,7 @@
       </c>
       <c r="Q215" s="5"/>
     </row>
-    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
         <v>70</v>
       </c>
@@ -10719,7 +10719,7 @@
       </c>
       <c r="Q216" s="5"/>
     </row>
-    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="9" t="s">
         <v>70</v>
       </c>
@@ -10763,7 +10763,7 @@
       </c>
       <c r="Q217" s="9"/>
     </row>
-    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="9" t="s">
         <v>70</v>
       </c>
@@ -10805,7 +10805,7 @@
       </c>
       <c r="Q218" s="9"/>
     </row>
-    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" s="9" t="s">
         <v>70</v>
       </c>
@@ -10849,7 +10849,7 @@
       </c>
       <c r="Q219" s="9"/>
     </row>
-    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A220" s="12" t="s">
         <v>70</v>
       </c>
@@ -10895,7 +10895,7 @@
       </c>
       <c r="Q220" s="12"/>
     </row>
-    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A221" s="16" t="s">
         <v>70</v>
       </c>
@@ -10941,7 +10941,7 @@
       </c>
       <c r="Q221" s="16"/>
     </row>
-    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A222" s="16" t="s">
         <v>70</v>
       </c>
@@ -10985,7 +10985,7 @@
       </c>
       <c r="Q222" s="16"/>
     </row>
-    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="16" t="s">
         <v>70</v>
       </c>
@@ -11031,7 +11031,7 @@
       </c>
       <c r="Q223" s="16"/>
     </row>
-    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A224" s="20" t="s">
         <v>70</v>
       </c>
@@ -11077,7 +11077,7 @@
       </c>
       <c r="Q224" s="20"/>
     </row>
-    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="24" t="s">
         <v>70</v>
       </c>
@@ -11123,7 +11123,7 @@
       </c>
       <c r="Q225" s="24"/>
     </row>
-    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A226" s="28" t="s">
         <v>70</v>
       </c>
@@ -11169,7 +11169,7 @@
       </c>
       <c r="Q226" s="28"/>
     </row>
-    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A227" s="28" t="s">
         <v>70</v>
       </c>
@@ -11213,7 +11213,7 @@
       </c>
       <c r="Q227" s="28"/>
     </row>
-    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" s="28" t="s">
         <v>70</v>
       </c>
@@ -11259,7 +11259,7 @@
       </c>
       <c r="Q228" s="28"/>
     </row>
-    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A229" s="32" t="s">
         <v>70</v>
       </c>
@@ -11305,7 +11305,7 @@
       </c>
       <c r="Q229" s="32"/>
     </row>
-    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
         <v>70</v>
       </c>
@@ -11364,19 +11364,19 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>68</v>
       </c>
@@ -11399,7 +11399,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11416,7 +11416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11439,7 +11439,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11462,7 +11462,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11479,7 +11479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11496,7 +11496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11519,7 +11519,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11536,7 +11536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11559,7 +11559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11576,7 +11576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11599,7 +11599,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11616,7 +11616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11633,7 +11633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11650,7 +11650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11667,7 +11667,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11684,7 +11684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11701,7 +11701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11718,7 +11718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -11735,7 +11735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -11752,7 +11752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -11769,7 +11769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -11804,9 +11804,9 @@
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>55</v>
       </c>
@@ -11823,7 +11823,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -11840,7 +11840,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -11857,7 +11857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -11874,7 +11874,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -11891,7 +11891,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -11908,7 +11908,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -11925,7 +11925,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -11942,7 +11942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -11959,7 +11959,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -11976,7 +11976,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -11993,7 +11993,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -12010,7 +12010,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -12027,7 +12027,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -12055,20 +12055,20 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6328125" style="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.81640625" style="47"/>
-    <col min="6" max="6" width="10.08984375" style="47" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="47"/>
+    <col min="2" max="2" width="6.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.77734375" style="47"/>
+    <col min="6" max="6" width="10.109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.77734375" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>74</v>
       </c>
@@ -12088,7 +12088,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48">
         <v>1</v>
       </c>
@@ -12108,7 +12108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48">
         <v>2</v>
       </c>
@@ -12128,7 +12128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48">
         <v>3</v>
       </c>
@@ -12148,7 +12148,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="48">
         <v>4</v>
       </c>
@@ -12168,7 +12168,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="49">
         <v>6</v>
       </c>
@@ -12188,7 +12188,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="49">
         <v>7</v>
       </c>
@@ -12208,7 +12208,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="49">
         <v>8</v>
       </c>
@@ -12228,7 +12228,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="49">
         <v>9</v>
       </c>
@@ -12248,7 +12248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="49">
         <v>10</v>
       </c>
@@ -12268,7 +12268,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="49">
         <v>11</v>
       </c>
@@ -12288,7 +12288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="49">
         <v>12</v>
       </c>
@@ -12308,7 +12308,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="49">
         <v>13</v>
       </c>
@@ -12328,7 +12328,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="49">
         <v>14</v>
       </c>
@@ -12348,7 +12348,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="49">
         <v>15</v>
       </c>
@@ -12368,7 +12368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="49">
         <v>16</v>
       </c>
@@ -12388,7 +12388,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="49">
         <v>17</v>
       </c>
@@ -12408,7 +12408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="49">
         <v>18</v>
       </c>
@@ -12428,7 +12428,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="49">
         <v>19</v>
       </c>
@@ -12448,7 +12448,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="49">
         <v>20</v>
       </c>
@@ -12468,7 +12468,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="49">
         <v>21</v>
       </c>
@@ -12488,7 +12488,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="49">
         <v>22</v>
       </c>
@@ -12508,7 +12508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="49">
         <v>23</v>
       </c>
@@ -12528,7 +12528,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="49">
         <v>24</v>
       </c>
@@ -12548,7 +12548,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="49">
         <v>25</v>
       </c>
@@ -12568,7 +12568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="49">
         <v>26</v>
       </c>
@@ -12588,7 +12588,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="49">
         <v>27</v>
       </c>
@@ -12608,7 +12608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="49">
         <v>28</v>
       </c>
@@ -12628,7 +12628,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="49">
         <v>29</v>
       </c>
@@ -12648,7 +12648,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="49">
         <v>30</v>
       </c>
@@ -12668,7 +12668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="49">
         <v>31</v>
       </c>
@@ -12688,7 +12688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="49">
         <v>32</v>
       </c>
@@ -12708,7 +12708,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="49">
         <v>33</v>
       </c>
@@ -12716,19 +12716,19 @@
         <v>70</v>
       </c>
       <c r="C33" s="49">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="D33" s="49">
         <v>15</v>
       </c>
       <c r="E33" s="49">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="F33" s="49" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="49">
         <v>34</v>
       </c>
@@ -12748,7 +12748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="49">
         <v>35</v>
       </c>
@@ -12768,7 +12768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="49">
         <v>36</v>
       </c>
@@ -12788,7 +12788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="49">
         <v>37</v>
       </c>
@@ -12808,7 +12808,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="49">
         <v>38</v>
       </c>
@@ -12828,7 +12828,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="49">
         <v>39</v>
       </c>
@@ -12848,7 +12848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="49">
         <v>40</v>
       </c>
@@ -12868,7 +12868,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="49">
         <v>41</v>
       </c>
@@ -12888,7 +12888,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="49">
         <v>42</v>
       </c>
@@ -12908,7 +12908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="49">
         <v>43</v>
       </c>
@@ -12928,7 +12928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="49">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Wayside beacons change so Train now stops at all stations regardless of waysides taken
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/TrackData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan94\Documents\Coding\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Kenneson\SCHOOL\University of Pitt\Senior Year\Spring 2017\Software Engineering\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
     <sheet name="SWITCH" sheetId="7" r:id="rId5"/>
     <sheet name="BEACON" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="78">
   <si>
     <t>A</t>
   </si>
@@ -12052,11 +12052,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12099,10 +12099,10 @@
         <v>76</v>
       </c>
       <c r="D2" s="48">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E2" s="48">
-        <v>-1</v>
+        <v>150</v>
       </c>
       <c r="F2" s="48" t="s">
         <v>13</v>
@@ -12119,10 +12119,10 @@
         <v>72</v>
       </c>
       <c r="D3" s="48">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E3" s="48">
-        <v>-1</v>
+        <v>150</v>
       </c>
       <c r="F3" s="48" t="s">
         <v>13</v>
@@ -12139,10 +12139,10 @@
         <v>71</v>
       </c>
       <c r="D4" s="48">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E4" s="48">
-        <v>-1</v>
+        <v>200</v>
       </c>
       <c r="F4" s="48" t="s">
         <v>13</v>
@@ -12159,10 +12159,10 @@
         <v>67</v>
       </c>
       <c r="D5" s="48">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5" s="48">
-        <v>-1</v>
+        <v>100</v>
       </c>
       <c r="F5" s="48" t="s">
         <v>13</v>
@@ -12946,6 +12946,26 @@
       </c>
       <c r="F44" s="49" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="49">
+        <v>45</v>
+      </c>
+      <c r="B45" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="49">
+        <v>77</v>
+      </c>
+      <c r="D45" s="49">
+        <v>15</v>
+      </c>
+      <c r="E45" s="49">
+        <v>200</v>
+      </c>
+      <c r="F45" s="49" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>